<commit_message>
Camera tweaks and toolbar opaque to mouse clicks
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="147">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Create new Github repo and commit project</t>
   </si>
   <si>
-    <t>Camera limiting function should have a min dist to screen center instead of preventing zoom</t>
-  </si>
-  <si>
     <t>Function for moving camera should prevent camera intersecting colliders</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   </si>
   <si>
     <t>Track Data object must store one or two variables defining curvature</t>
+  </si>
+  <si>
+    <t>Camera limiting function should have a min height from terrain instead of preventing zoom</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,134 +1765,152 @@
       <c r="B79" s="9" t="s">
         <v>118</v>
       </c>
+      <c r="C79" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="31"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C80" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="31"/>
       <c r="B82" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="31" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="31"/>
       <c r="B84" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
+      <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
-      <c r="B85" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="31" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="31"/>
       <c r="B87" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="31"/>
       <c r="B88" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="31"/>
       <c r="B89" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="31"/>
       <c r="B90" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="31"/>
       <c r="B91" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="31"/>
       <c r="B93" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="31"/>
       <c r="B94" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="31"/>
       <c r="B95" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="31" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="31"/>
       <c r="B97" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="31"/>
       <c r="B98" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1901,25 +1919,25 @@
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="31"/>
       <c r="B100" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="31"/>
       <c r="B101" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="31"/>
       <c r="B102" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1928,19 +1946,19 @@
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="31"/>
       <c r="B104" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="31"/>
       <c r="B105" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,13 +1967,13 @@
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="31"/>
       <c r="B107" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1964,11 +1982,11 @@
         <v>I want curved sections of track to save and load properly.</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D108">
         <f>COUNTA(C79:C108)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baubles at the ends of track sections
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="147">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -636,22 +636,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -666,7 +657,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -973,7 +973,7 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,14 +995,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="str">
+      <c r="A3" s="23" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1023,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1032,7 +1032,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="str">
+      <c r="A6" s="23" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1044,7 +1044,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1062,7 +1062,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1071,7 +1071,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="23" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1110,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1119,7 +1119,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="str">
+      <c r="A15" s="23" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1131,7 +1131,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="str">
+      <c r="A19" s="23" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="str">
+      <c r="A21" s="23" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1204,11 +1204,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1223,7 +1223,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="str">
+      <c r="A25" s="23" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="str">
+      <c r="A27" s="23" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1274,7 +1274,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1283,7 +1283,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1292,7 +1292,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="str">
+      <c r="A34" s="23" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1322,7 +1322,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1331,7 +1331,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="str">
+      <c r="A38" s="23" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1361,7 +1361,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1382,7 +1382,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="str">
+      <c r="A41" s="23" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1403,7 +1403,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1412,7 +1412,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="str">
+      <c r="A45" s="23" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="str">
+      <c r="A47" s="23" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1476,14 +1476,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="27"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="str">
+      <c r="A51" s="23" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="str">
+      <c r="A54" s="23" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="str">
+      <c r="A56" s="23" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="str">
+      <c r="A58" s="23" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1567,7 +1567,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="23"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
+      <c r="A64" s="23"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="str">
+      <c r="A65" s="23" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="str">
+      <c r="A67" s="23" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1661,7 +1661,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="str">
+      <c r="A69" s="23" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1673,21 +1673,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="str">
+      <c r="A73" s="23" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="str">
+      <c r="A75" s="23" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1729,7 +1729,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1751,14 +1751,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="str">
+      <c r="A79" s="21" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="str">
+      <c r="A81" s="21" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="str">
+      <c r="A83" s="21" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1821,52 +1821,70 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="31" t="str">
+      <c r="A86" s="21" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>124</v>
       </c>
+      <c r="C86" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="31"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="C87" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
+      <c r="C88" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="C89" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
+      <c r="C90" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
+      <c r="C91" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="31" t="str">
+      <c r="A92" s="21" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -1875,25 +1893,25 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="31"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="31"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="31" t="str">
+      <c r="A96" s="21" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -1902,19 +1920,19 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31" t="str">
+      <c r="A99" s="21" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -1923,25 +1941,25 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="31"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="31" t="str">
+      <c r="A103" s="21" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -1950,19 +1968,19 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="31"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="31" t="str">
+      <c r="A106" s="21" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -1971,7 +1989,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+      <c r="A107" s="21"/>
       <c r="B107" s="9" t="s">
         <v>144</v>
       </c>
@@ -1986,35 +2004,11 @@
       </c>
       <c r="D108">
         <f>COUNTA(C79:C108)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2026,6 +2020,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="A103:A105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
VertexBender (mostly) finished and passing unit tests
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,18 +1891,27 @@
       <c r="B92" s="9" t="s">
         <v>130</v>
       </c>
+      <c r="C92" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
+      <c r="C93" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
+      <c r="C94" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
@@ -2004,7 +2013,7 @@
       </c>
       <c r="D108">
         <f>COUNTA(C79:C108)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Track sections are bending to the mouse cursor
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -460,6 +460,12 @@
   </si>
   <si>
     <t>Camera limiting function should have a min height from terrain instead of preventing zoom</t>
+  </si>
+  <si>
+    <t>Register a track section to be curved if any section is clicked on</t>
+  </si>
+  <si>
+    <t>Get straight sections approximation of curve</t>
   </si>
 </sst>
 </file>
@@ -636,13 +642,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -657,16 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,14 +1001,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="str">
+      <c r="A3" s="21" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1014,7 +1020,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1029,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1032,7 +1038,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="str">
+      <c r="A6" s="21" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1044,7 +1050,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1059,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1062,7 +1068,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1071,7 +1077,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1080,7 +1086,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1095,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="str">
+      <c r="A12" s="21" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1101,7 +1107,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1116,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1119,7 +1125,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="str">
+      <c r="A15" s="21" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1131,7 +1137,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1146,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1149,7 +1155,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1158,7 +1164,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="str">
+      <c r="A19" s="21" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1170,7 +1176,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1179,7 +1185,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="str">
+      <c r="A21" s="21" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1191,7 +1197,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1204,11 +1210,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1223,7 +1229,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="str">
+      <c r="A25" s="21" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1235,7 +1241,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1244,7 +1250,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="str">
+      <c r="A27" s="21" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1256,7 +1262,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1265,7 +1271,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1274,7 +1280,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1283,7 +1289,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1292,7 +1298,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1301,7 +1307,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1310,7 +1316,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="str">
+      <c r="A34" s="21" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1322,7 +1328,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1331,7 +1337,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1340,7 +1346,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1349,7 +1355,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="str">
+      <c r="A38" s="21" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1361,7 +1367,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1382,7 +1388,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="str">
+      <c r="A41" s="21" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1394,7 +1400,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1403,7 +1409,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1412,7 +1418,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1421,7 +1427,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="str">
+      <c r="A45" s="21" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1433,7 +1439,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1442,7 +1448,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="str">
+      <c r="A47" s="21" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1454,7 +1460,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1463,7 +1469,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1476,14 +1482,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="27"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="str">
+      <c r="A51" s="21" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1495,7 +1501,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1504,7 +1510,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1513,7 +1519,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="str">
+      <c r="A54" s="21" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1525,7 +1531,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1534,7 +1540,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="str">
+      <c r="A56" s="21" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1546,7 +1552,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1555,7 +1561,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="str">
+      <c r="A58" s="21" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1567,7 +1573,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1576,7 +1582,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1585,7 +1591,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1594,7 +1600,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1603,7 +1609,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1612,7 +1618,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1621,7 +1627,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="str">
+      <c r="A65" s="21" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1631,7 +1637,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1640,7 +1646,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="str">
+      <c r="A67" s="21" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1652,7 +1658,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1661,7 +1667,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="str">
+      <c r="A69" s="21" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1673,21 +1679,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1696,7 +1702,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="str">
+      <c r="A73" s="21" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1708,7 +1714,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1717,7 +1723,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="str">
+      <c r="A75" s="21" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1729,7 +1735,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1738,7 +1744,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1751,14 +1757,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="22"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="str">
+      <c r="A79" s="31" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1770,7 +1776,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1779,7 +1785,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="21" t="str">
+      <c r="A81" s="31" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1791,7 +1797,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="21"/>
+      <c r="A82" s="31"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1800,7 +1806,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="str">
+      <c r="A83" s="31" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1812,7 +1818,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
+      <c r="A84" s="31"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1821,13 +1827,13 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
+      <c r="A85" s="31"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="str">
+      <c r="A86" s="31" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1839,7 +1845,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
+      <c r="A87" s="31"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1848,7 +1854,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
+      <c r="A88" s="31"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1857,7 +1863,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1866,7 +1872,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1875,7 +1881,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -1884,7 +1890,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="str">
+      <c r="A92" s="31" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -1896,7 +1902,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -1905,7 +1911,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -1914,110 +1920,155 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="str">
+      <c r="A96" s="31" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="21"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="21"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="21" t="str">
+      <c r="A99" s="31" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>136</v>
       </c>
+      <c r="C99" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="21"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
+      <c r="C100" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="21"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="21"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="21" t="str">
+      <c r="C102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
+      <c r="B103" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="31" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B104" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="21"/>
-      <c r="B104" s="9" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="31"/>
+      <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="21"/>
-      <c r="B105" s="9" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
+      <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="21" t="str">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="31" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B107" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="21"/>
-      <c r="B107" s="9" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
+      <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="str">
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="str">
         <f>'Stories 4'!A10</f>
         <v>I want curved sections of track to save and load properly.</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B109" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D108">
-        <f>COUNTA(C79:C108)</f>
-        <v>15</v>
+      <c r="D109">
+        <f>COUNTA(C79:C109)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2029,30 +2080,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A103:A105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Vertex Bender properly smooths the curvature.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="149">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -642,22 +642,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -672,7 +663,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -979,7 +979,7 @@
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,14 +1001,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="str">
+      <c r="A3" s="23" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1029,7 +1029,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="str">
+      <c r="A6" s="23" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1077,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="23" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="str">
+      <c r="A15" s="23" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1164,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="str">
+      <c r="A19" s="23" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="str">
+      <c r="A21" s="23" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1210,11 +1210,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1229,7 +1229,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="str">
+      <c r="A25" s="23" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1250,7 +1250,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="str">
+      <c r="A27" s="23" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="str">
+      <c r="A34" s="23" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="str">
+      <c r="A38" s="23" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1388,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="str">
+      <c r="A41" s="23" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1400,7 +1400,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="str">
+      <c r="A45" s="23" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="str">
+      <c r="A47" s="23" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1482,14 +1482,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="27"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="str">
+      <c r="A51" s="23" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="str">
+      <c r="A54" s="23" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1540,7 +1540,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="str">
+      <c r="A56" s="23" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="str">
+      <c r="A58" s="23" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="23"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1591,7 +1591,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1600,7 +1600,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
+      <c r="A64" s="23"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="str">
+      <c r="A65" s="23" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="str">
+      <c r="A67" s="23" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="str">
+      <c r="A69" s="23" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1679,21 +1679,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="str">
+      <c r="A73" s="23" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="str">
+      <c r="A75" s="23" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1744,7 +1744,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1757,14 +1757,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="str">
+      <c r="A79" s="21" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1785,7 +1785,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="str">
+      <c r="A81" s="21" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1797,7 +1797,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="str">
+      <c r="A83" s="21" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1827,13 +1827,13 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="31" t="str">
+      <c r="A86" s="21" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="31"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="31" t="str">
+      <c r="A92" s="21" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -1911,7 +1911,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="31"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -1920,13 +1920,16 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="31"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
+      <c r="C95" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="31" t="str">
+      <c r="A96" s="21" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -1935,19 +1938,19 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31" t="str">
+      <c r="A99" s="21" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -1959,7 +1962,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="31"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -1968,7 +1971,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -1977,7 +1980,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -1986,7 +1989,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -1995,7 +1998,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="31" t="str">
+      <c r="A104" s="21" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2004,19 +2007,19 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+      <c r="A106" s="21"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="31" t="str">
+      <c r="A107" s="21" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2025,7 +2028,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+      <c r="A108" s="21"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2040,35 +2043,11 @@
       </c>
       <c r="D109">
         <f>COUNTA(C79:C109)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2080,6 +2059,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Curved rail now had terrain adjust to it properly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="149">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -642,13 +642,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -663,16 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -979,7 +979,7 @@
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,14 +1001,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="str">
+      <c r="A3" s="21" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1029,7 +1029,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="str">
+      <c r="A6" s="21" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1077,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="str">
+      <c r="A12" s="21" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="str">
+      <c r="A15" s="21" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1164,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="str">
+      <c r="A19" s="21" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="str">
+      <c r="A21" s="21" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1210,11 +1210,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1229,7 +1229,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="str">
+      <c r="A25" s="21" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1250,7 +1250,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="str">
+      <c r="A27" s="21" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="str">
+      <c r="A34" s="21" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="str">
+      <c r="A38" s="21" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1388,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="str">
+      <c r="A41" s="21" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1400,7 +1400,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="str">
+      <c r="A45" s="21" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="str">
+      <c r="A47" s="21" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1482,14 +1482,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="27"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="str">
+      <c r="A51" s="21" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="str">
+      <c r="A54" s="21" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1540,7 +1540,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="str">
+      <c r="A56" s="21" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="str">
+      <c r="A58" s="21" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1591,7 +1591,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1600,7 +1600,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="str">
+      <c r="A65" s="21" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="str">
+      <c r="A67" s="21" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="str">
+      <c r="A69" s="21" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1679,21 +1679,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="str">
+      <c r="A73" s="21" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="str">
+      <c r="A75" s="21" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1744,7 +1744,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1757,14 +1757,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="22"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="str">
+      <c r="A79" s="31" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1785,7 +1785,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="21" t="str">
+      <c r="A81" s="31" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1797,7 +1797,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="21"/>
+      <c r="A82" s="31"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="str">
+      <c r="A83" s="31" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
+      <c r="A84" s="31"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1827,13 +1827,13 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
+      <c r="A85" s="31"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="str">
+      <c r="A86" s="31" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
+      <c r="A87" s="31"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
+      <c r="A88" s="31"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="str">
+      <c r="A92" s="31" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -1911,7 +1911,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -1920,7 +1920,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -1929,28 +1929,37 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="str">
+      <c r="A96" s="31" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>148</v>
       </c>
+      <c r="C96" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="21"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
+      <c r="C97" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="21"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
+      <c r="C98" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="21" t="str">
+      <c r="A99" s="31" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -1962,7 +1971,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="21"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -1971,7 +1980,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="21"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -1980,7 +1989,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="21"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -1989,7 +1998,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="21"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -1998,7 +2007,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="21" t="str">
+      <c r="A104" s="31" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2007,30 +2016,36 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="21"/>
+      <c r="A105" s="31"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="21"/>
+      <c r="A106" s="31"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="21" t="str">
+      <c r="A107" s="31" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>143</v>
       </c>
+      <c r="C107" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="21"/>
+      <c r="A108" s="31"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
+      </c>
+      <c r="C108" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2043,11 +2058,35 @@
       </c>
       <c r="D109">
         <f>COUNTA(C79:C109)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2059,30 +2098,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Technically the end of Iteration 4.  There remain a few bugs, especially with the linking of track sections which needs to be redesigned.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,18 +2014,27 @@
       <c r="B104" s="9" t="s">
         <v>140</v>
       </c>
+      <c r="C104" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="31"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
+      <c r="C105" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="31"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
+      <c r="C106" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="str">
@@ -2056,9 +2065,12 @@
       <c r="B109" s="9" t="s">
         <v>145</v>
       </c>
+      <c r="C109" t="s">
+        <v>24</v>
+      </c>
       <c r="D109">
         <f>COUNTA(C79:C109)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separation of track sections and baubles.  Some bugs remain.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -13,13 +13,14 @@
     <sheet name="Stories 3" sheetId="6" r:id="rId4"/>
     <sheet name="Stories 4" sheetId="7" r:id="rId5"/>
     <sheet name="Stories 5" sheetId="9" r:id="rId6"/>
+    <sheet name="Stories 6" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="180">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -466,6 +467,99 @@
   </si>
   <si>
     <t>Get straight sections approximation of curve</t>
+  </si>
+  <si>
+    <t>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</t>
+  </si>
+  <si>
+    <t>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</t>
+  </si>
+  <si>
+    <t>I want to be able to create a new bauble partway around a curve.</t>
+  </si>
+  <si>
+    <t>Loading a map containing linked track sections should allow me to use the links correctly.</t>
+  </si>
+  <si>
+    <t>Saving and loading a map with buffer stops and compound curve sections should keep them</t>
+  </si>
+  <si>
+    <t>Iteration 5</t>
+  </si>
+  <si>
+    <t>Instantiate baubles independently of the section</t>
+  </si>
+  <si>
+    <t>bauble collider should only activate when section is finalized.</t>
+  </si>
+  <si>
+    <t>Rewrite track tool methods using only function calls to shape controlller</t>
+  </si>
+  <si>
+    <t>Have shape controller decide which end is which based on bauble links at each end</t>
+  </si>
+  <si>
+    <t>link baubles to each track section and vice versa.</t>
+  </si>
+  <si>
+    <t>The bauble's list of links should indicate direction, and also connection order</t>
+  </si>
+  <si>
+    <t>Create SaveLoadable for baubles</t>
+  </si>
+  <si>
+    <t>each track section should have a UID for bauble SaveLoadable to store</t>
+  </si>
+  <si>
+    <t>Once the file is completely loaded and deserialized, the track tool must go through the baubles and link to track section objects based on IDs.</t>
+  </si>
+  <si>
+    <t>Find equation to govern shape of a section with two transitions and an arc</t>
+  </si>
+  <si>
+    <t>Include third mode for track shape</t>
+  </si>
+  <si>
+    <t>"Rail" vectors should be goverened by the same function that adds creases to the bending model</t>
+  </si>
+  <si>
+    <t>Modify vertex bender to bend models in three parts</t>
+  </si>
+  <si>
+    <t>Track tool on a bauble will change curved track to arced.</t>
+  </si>
+  <si>
+    <t>Find a model for a buffer stop and link the prefab to the track tool</t>
+  </si>
+  <si>
+    <t>Add a sub-menu for the track tool; track by default with buffer stops</t>
+  </si>
+  <si>
+    <t>single-click sub-tool on a bauble with only one link will add buffer stop.</t>
+  </si>
+  <si>
+    <t>Catergorise or list box colliders for all track sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for collisions during finalization.  </t>
+  </si>
+  <si>
+    <t>If a collision occurs, prevent placement and give indication of error</t>
+  </si>
+  <si>
+    <t>Have exceptions for colliders in sections at either end of this section.</t>
+  </si>
+  <si>
+    <t>SaveLoadable for track sections needs to include data to recreate arced track</t>
+  </si>
+  <si>
+    <t>New Saveloadable for buffer stops; need track UIDs</t>
+  </si>
+  <si>
+    <t>Track tool must maintain list for making them visible/invisible</t>
+  </si>
+  <si>
+    <t>The post-save linking process should include buffer stops</t>
   </si>
 </sst>
 </file>
@@ -598,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -642,6 +736,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,9 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,14 +1104,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="str">
+      <c r="A3" s="25" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1020,7 +1123,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1029,7 +1132,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1141,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="str">
+      <c r="A6" s="25" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1050,7 +1153,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1162,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1171,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1180,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1189,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1198,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="25" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1107,7 +1210,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1219,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1125,7 +1228,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="str">
+      <c r="A15" s="25" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1137,7 +1240,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1249,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1155,7 +1258,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1267,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="str">
+      <c r="A19" s="25" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1176,7 +1279,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1288,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="str">
+      <c r="A21" s="25" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1197,7 +1300,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1210,11 +1313,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1229,7 +1332,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="str">
+      <c r="A25" s="25" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1241,7 +1344,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1250,7 +1353,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="str">
+      <c r="A27" s="25" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1262,7 +1365,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1271,7 +1374,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1383,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1289,7 +1392,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1401,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1307,7 +1410,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1316,7 +1419,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="str">
+      <c r="A34" s="25" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1328,7 +1431,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1337,7 +1440,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1346,7 +1449,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1355,7 +1458,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="str">
+      <c r="A38" s="25" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1367,7 +1470,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1491,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="str">
+      <c r="A41" s="25" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1400,7 +1503,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1409,7 +1512,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1418,7 +1521,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1427,7 +1530,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="str">
+      <c r="A45" s="25" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1439,7 +1542,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1448,7 +1551,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="str">
+      <c r="A47" s="25" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1460,7 +1563,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1469,7 +1572,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1482,14 +1585,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="str">
+      <c r="A51" s="25" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1501,7 +1604,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1510,7 +1613,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1519,7 +1622,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="str">
+      <c r="A54" s="25" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1531,7 +1634,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1540,7 +1643,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="str">
+      <c r="A56" s="25" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1552,7 +1655,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1561,7 +1664,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="str">
+      <c r="A58" s="25" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1573,7 +1676,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1582,7 +1685,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1591,7 +1694,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1600,7 +1703,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1609,7 +1712,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1618,7 +1721,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1627,7 +1730,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="str">
+      <c r="A65" s="25" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1637,7 +1740,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1646,7 +1749,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="str">
+      <c r="A67" s="25" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1658,7 +1761,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1667,7 +1770,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="str">
+      <c r="A69" s="25" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1679,21 +1782,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1702,7 +1805,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="str">
+      <c r="A73" s="25" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1714,7 +1817,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1723,7 +1826,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="str">
+      <c r="A75" s="25" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1735,7 +1838,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1744,7 +1847,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1757,315 +1860,316 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="str">
+      <c r="A79" s="25" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="str">
+      <c r="A81" s="25" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="str">
+      <c r="A83" s="25" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
+      <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="31" t="str">
+      <c r="A86" s="25" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="31"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="31" t="str">
+      <c r="A92" s="25" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="31"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="31"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="31" t="str">
+      <c r="A96" s="25" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31" t="str">
+      <c r="A99" s="25" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="31"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="31" t="str">
+      <c r="A104" s="25" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="31" t="str">
+      <c r="A107" s="25" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+      <c r="A108" s="25"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="str">
+      <c r="A109" s="21" t="str">
         <f>'Stories 4'!A10</f>
         <v>I want curved sections of track to save and load properly.</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D109">
@@ -2073,8 +2177,199 @@
         <v>30</v>
       </c>
     </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="24" t="str">
+        <f>'Stories 5'!A1</f>
+        <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="24"/>
+      <c r="B112" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="24"/>
+      <c r="B113" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="24"/>
+      <c r="B114" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="24"/>
+      <c r="B115" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C115" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="24" t="str">
+        <f>'Stories 5'!A2</f>
+        <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="24"/>
+      <c r="B117" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="24" t="str">
+        <f>'Stories 5'!A3</f>
+        <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="24"/>
+      <c r="B119" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="24"/>
+      <c r="B120" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="24" t="str">
+        <f>'Stories 5'!A4</f>
+        <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="24"/>
+      <c r="B122" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="24"/>
+      <c r="B123" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="24"/>
+      <c r="B124" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="24" t="str">
+        <f>'Stories 5'!A5</f>
+        <v>I want to be able to place a buffer stop at an existing track end.</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="24"/>
+      <c r="B126" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="24"/>
+      <c r="B127" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="24" t="str">
+        <f>'Stories 5'!A6</f>
+        <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="24"/>
+      <c r="B129" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="24"/>
+      <c r="B130" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="24"/>
+      <c r="B131" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="24" t="str">
+        <f>'Stories 5'!A7</f>
+        <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="24"/>
+      <c r="B133" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="24"/>
+      <c r="B134" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D134">
+        <f>COUNTA(C111:C134)</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="43">
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
     <mergeCell ref="A96:A98"/>
@@ -2110,6 +2405,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2360,9 +2663,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2371,17 +2676,65 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bauble link refactor almost done, just need to redo linking track to an existing section.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="180">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -745,16 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -777,6 +768,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1082,7 +1082,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,14 +1104,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
+      <c r="A3" s="24" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1123,7 +1123,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
+      <c r="A6" s="24" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1198,7 +1198,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
+      <c r="A12" s="24" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1228,7 +1228,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
+      <c r="A15" s="24" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1258,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1267,7 +1267,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="str">
+      <c r="A19" s="24" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="str">
+      <c r="A21" s="24" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1313,11 +1313,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="str">
+      <c r="A25" s="24" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="str">
+      <c r="A27" s="24" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="str">
+      <c r="A34" s="24" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="str">
+      <c r="A38" s="24" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="str">
+      <c r="A41" s="24" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1530,7 +1530,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="str">
+      <c r="A45" s="24" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="str">
+      <c r="A47" s="24" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1585,14 +1585,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="str">
+      <c r="A51" s="24" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1604,7 +1604,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1622,7 +1622,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="str">
+      <c r="A54" s="24" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="str">
+      <c r="A56" s="24" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="str">
+      <c r="A58" s="24" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="str">
+      <c r="A65" s="24" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="str">
+      <c r="A67" s="24" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="str">
+      <c r="A69" s="24" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1782,21 +1782,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="25" t="str">
+      <c r="A73" s="24" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="str">
+      <c r="A75" s="24" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1847,7 +1847,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1860,14 +1860,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="30"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="27"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="str">
+      <c r="A79" s="24" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1879,7 +1879,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="str">
+      <c r="A81" s="24" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
+      <c r="A82" s="24"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="str">
+      <c r="A83" s="24" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
+      <c r="A84" s="24"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1930,14 +1930,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="24"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="25" t="str">
+      <c r="A86" s="24" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
+      <c r="A87" s="24"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
+      <c r="A88" s="24"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="24"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
+      <c r="A90" s="24"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
+      <c r="A91" s="24"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="str">
+      <c r="A92" s="24" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
+      <c r="A93" s="24"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
+      <c r="A94" s="24"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
+      <c r="A95" s="24"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="str">
+      <c r="A96" s="24" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="24"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
+      <c r="A98" s="24"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="str">
+      <c r="A99" s="24" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
+      <c r="A100" s="24"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2084,7 +2084,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="24"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="24"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="str">
+      <c r="A104" s="24" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
+      <c r="A105" s="24"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2132,7 +2132,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
+      <c r="A106" s="24"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="str">
+      <c r="A107" s="24" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="25"/>
+      <c r="A108" s="24"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2178,14 +2178,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="24" t="s">
+      <c r="A110" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="24"/>
+      <c r="B110" s="34"/>
+      <c r="C110" s="34"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="24" t="str">
+      <c r="A111" s="34" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="24"/>
+      <c r="A112" s="34"/>
       <c r="B112" s="9" t="s">
         <v>178</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="24"/>
+      <c r="A113" s="34"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2215,13 +2215,16 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="24"/>
+      <c r="A114" s="34"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
+      <c r="C114" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="24"/>
+      <c r="A115" s="34"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2230,7 +2233,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="24" t="str">
+      <c r="A116" s="34" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2242,13 +2245,13 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="24"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="24" t="str">
+      <c r="A118" s="34" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2257,19 +2260,22 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="24"/>
+      <c r="A119" s="34"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
+      <c r="C119" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="24"/>
+      <c r="A120" s="34"/>
       <c r="B120" s="9" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="24" t="str">
+      <c r="A121" s="34" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2278,25 +2284,25 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="24"/>
+      <c r="A122" s="34"/>
       <c r="B122" s="9" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="24"/>
+      <c r="A123" s="34"/>
       <c r="B123" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="24"/>
+      <c r="A124" s="34"/>
       <c r="B124" s="9" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="24" t="str">
+      <c r="A125" s="34" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2305,19 +2311,19 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="24"/>
+      <c r="A126" s="34"/>
       <c r="B126" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="24"/>
+      <c r="A127" s="34"/>
       <c r="B127" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="24" t="str">
+      <c r="A128" s="34" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2326,25 +2332,25 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="24"/>
+      <c r="A129" s="34"/>
       <c r="B129" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="24"/>
+      <c r="A130" s="34"/>
       <c r="B130" s="9" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="24"/>
+      <c r="A131" s="34"/>
       <c r="B131" s="9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="24" t="str">
+      <c r="A132" s="34" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2353,47 +2359,31 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="24"/>
+      <c r="A133" s="34"/>
       <c r="B133" s="9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="24"/>
+      <c r="A134" s="34"/>
       <c r="B134" s="9" t="s">
         <v>179</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2405,14 +2395,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bauble refactoring is complete.  Partway through saving bauble data.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="180">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1082,7 +1082,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,6 +2249,9 @@
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="34" t="str">
@@ -2371,7 +2374,7 @@
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bauble links and track shapes are (finally) loading properly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="182">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -511,9 +511,6 @@
     <t>each track section should have a UID for bauble SaveLoadable to store</t>
   </si>
   <si>
-    <t>Once the file is completely loaded and deserialized, the track tool must go through the baubles and link to track section objects based on IDs.</t>
-  </si>
-  <si>
     <t>Find equation to govern shape of a section with two transitions and an arc</t>
   </si>
   <si>
@@ -560,6 +557,15 @@
   </si>
   <si>
     <t>The post-save linking process should include buffer stops</t>
+  </si>
+  <si>
+    <t>Once the file is completely loaded and deserialized, the track tool must go through the track sections and link to bauble objects based on IDs.</t>
+  </si>
+  <si>
+    <t>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</t>
+  </si>
+  <si>
+    <t>Upgrade to Unity 5</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2205,7 @@
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="34"/>
       <c r="B112" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C112" t="s">
         <v>24</v>
@@ -2261,6 +2267,9 @@
       <c r="B118" s="9" t="s">
         <v>161</v>
       </c>
+      <c r="C118" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="34"/>
@@ -2274,7 +2283,10 @@
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="34"/>
       <c r="B120" s="9" t="s">
-        <v>163</v>
+        <v>179</v>
+      </c>
+      <c r="C120" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,25 +2295,25 @@
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="34"/>
       <c r="B122" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="34"/>
       <c r="B123" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="34"/>
       <c r="B124" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2310,19 +2322,19 @@
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="34"/>
       <c r="B126" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="34"/>
       <c r="B127" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2331,25 +2343,25 @@
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="34"/>
       <c r="B129" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="34"/>
       <c r="B130" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="34"/>
       <c r="B131" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2358,23 +2370,23 @@
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="34"/>
       <c r="B133" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="34"/>
       <c r="B134" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2725,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2738,12 +2750,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>166</v>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Newton's method for finding A and theta in a compound curve is implemented, but not working 100%.  Need to find if problem with equations or if test scenarios are incorrect.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -511,21 +511,12 @@
     <t>each track section should have a UID for bauble SaveLoadable to store</t>
   </si>
   <si>
-    <t>Find equation to govern shape of a section with two transitions and an arc</t>
-  </si>
-  <si>
     <t>Include third mode for track shape</t>
   </si>
   <si>
     <t>"Rail" vectors should be goverened by the same function that adds creases to the bending model</t>
   </si>
   <si>
-    <t>Modify vertex bender to bend models in three parts</t>
-  </si>
-  <si>
-    <t>Track tool on a bauble will change curved track to arced.</t>
-  </si>
-  <si>
     <t>Find a model for a buffer stop and link the prefab to the track tool</t>
   </si>
   <si>
@@ -566,6 +557,18 @@
   </si>
   <si>
     <t>Upgrade to Unity 5</t>
+  </si>
+  <si>
+    <t>Design. Seriously.</t>
+  </si>
+  <si>
+    <t>Find equation to govern shape of a section with two different transitions</t>
+  </si>
+  <si>
+    <t>Modify vertex bender to bend models in two different parts</t>
+  </si>
+  <si>
+    <t>Track tool on a bauble will change curved track to compound curve</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
@@ -2205,7 +2208,7 @@
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="34"/>
       <c r="B112" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C112" t="s">
         <v>24</v>
@@ -2283,7 +2286,7 @@
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="34"/>
       <c r="B120" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C120" t="s">
         <v>24</v>
@@ -2295,25 +2298,25 @@
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="34"/>
       <c r="B122" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="34"/>
       <c r="B123" s="9" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="34"/>
       <c r="B124" s="9" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,19 +2325,19 @@
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="34"/>
       <c r="B126" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="34"/>
       <c r="B127" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2343,25 +2346,25 @@
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="34"/>
       <c r="B129" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="34"/>
       <c r="B130" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="34"/>
       <c r="B131" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2370,19 +2373,19 @@
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="34"/>
       <c r="B133" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="34"/>
       <c r="B134" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
@@ -2737,10 +2740,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2750,22 +2753,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>165</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>180</v>
+      <c r="A4" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compound curve math tested and constrains in place.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -754,7 +754,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -777,15 +786,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,14 +1113,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="str">
+      <c r="A3" s="25" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="str">
+      <c r="A6" s="25" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +1198,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1207,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="str">
+      <c r="A12" s="25" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1228,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1237,7 +1237,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="str">
+      <c r="A15" s="25" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1258,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1267,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1276,7 +1276,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="str">
+      <c r="A19" s="25" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="str">
+      <c r="A21" s="25" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1309,7 +1309,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1322,11 +1322,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1341,7 +1341,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="str">
+      <c r="A25" s="25" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="str">
+      <c r="A27" s="25" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1428,7 +1428,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="str">
+      <c r="A34" s="25" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="str">
+      <c r="A38" s="25" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1479,7 +1479,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1500,7 +1500,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="str">
+      <c r="A41" s="25" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1530,7 +1530,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="str">
+      <c r="A45" s="25" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="str">
+      <c r="A47" s="25" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1581,7 +1581,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1594,14 +1594,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="31"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="str">
+      <c r="A51" s="25" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1622,7 +1622,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="str">
+      <c r="A54" s="25" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="str">
+      <c r="A56" s="25" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1673,7 +1673,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="str">
+      <c r="A58" s="25" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="24"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="24"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="str">
+      <c r="A65" s="25" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="24"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="str">
+      <c r="A67" s="25" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="str">
+      <c r="A69" s="25" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1791,21 +1791,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="str">
+      <c r="A73" s="25" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="str">
+      <c r="A75" s="25" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1847,7 +1847,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="28"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1869,14 +1869,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="26"/>
-      <c r="C78" s="27"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="str">
+      <c r="A79" s="25" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="24"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1897,7 +1897,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="str">
+      <c r="A81" s="25" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="24"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="24" t="str">
+      <c r="A83" s="25" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1930,7 +1930,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1939,14 +1939,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="24"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="str">
+      <c r="A86" s="25" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="24"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="24"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="24"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="24" t="str">
+      <c r="A92" s="25" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2042,7 +2042,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="24" t="str">
+      <c r="A96" s="25" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="24"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="24"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="24" t="str">
+      <c r="A99" s="25" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2084,7 +2084,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="24"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="24"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="24"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="24"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="24" t="str">
+      <c r="A104" s="25" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2132,7 +2132,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="24"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="24"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="24" t="str">
+      <c r="A107" s="25" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2162,7 +2162,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="24"/>
+      <c r="A108" s="25"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2187,14 +2187,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="34" t="s">
+      <c r="A110" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="34"/>
-      <c r="C110" s="34"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="str">
+      <c r="A111" s="24" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
+      <c r="A112" s="24"/>
       <c r="B112" s="9" t="s">
         <v>174</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+      <c r="A113" s="24"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2224,7 +2224,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
+      <c r="A114" s="24"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2233,7 +2233,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
+      <c r="A115" s="24"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="34" t="str">
+      <c r="A116" s="24" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+      <c r="A117" s="24"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2263,7 +2263,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="34" t="str">
+      <c r="A118" s="24" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2275,7 +2275,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+      <c r="A119" s="24"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2284,7 +2284,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="34"/>
+      <c r="A120" s="24"/>
       <c r="B120" s="9" t="s">
         <v>176</v>
       </c>
@@ -2293,34 +2293,37 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="34" t="str">
+      <c r="A121" s="24" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>180</v>
       </c>
+      <c r="C121" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
-      <c r="B122" s="9" t="s">
+      <c r="A122" s="24"/>
+      <c r="B122" s="16" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+      <c r="A123" s="24"/>
       <c r="B123" s="9" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+      <c r="A124" s="24"/>
       <c r="B124" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="34" t="str">
+      <c r="A125" s="24" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2329,19 +2332,19 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+      <c r="A126" s="24"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+      <c r="A127" s="24"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="34" t="str">
+      <c r="A128" s="24" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2350,25 +2353,25 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+      <c r="A129" s="24"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="34"/>
+      <c r="A130" s="24"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="34"/>
+      <c r="A131" s="24"/>
       <c r="B131" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="34" t="str">
+      <c r="A132" s="24" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2377,31 +2380,47 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+      <c r="A133" s="24"/>
       <c r="B133" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+      <c r="A134" s="24"/>
       <c r="B134" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2413,30 +2432,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Compound curve code used for symmetrical curves and working correctly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -701,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -754,16 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -786,6 +777,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
+      <c r="A3" s="24" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1132,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
+      <c r="A6" s="24" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1162,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
+      <c r="A12" s="24" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1219,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1237,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
+      <c r="A15" s="24" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1249,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1276,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="str">
+      <c r="A19" s="24" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1288,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1297,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="str">
+      <c r="A21" s="24" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1309,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1322,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1341,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="str">
+      <c r="A25" s="24" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1353,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1362,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="str">
+      <c r="A27" s="24" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1374,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1401,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1410,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1419,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1428,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="str">
+      <c r="A34" s="24" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1440,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1458,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1467,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="str">
+      <c r="A38" s="24" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1479,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1500,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="str">
+      <c r="A41" s="24" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1512,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1521,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1530,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1539,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="str">
+      <c r="A45" s="24" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1551,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1560,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="str">
+      <c r="A47" s="24" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1572,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1581,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1594,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="str">
+      <c r="A51" s="24" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1613,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1622,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1631,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="str">
+      <c r="A54" s="24" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1643,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1652,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="str">
+      <c r="A56" s="24" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1664,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1673,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="str">
+      <c r="A58" s="24" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1685,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1694,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1703,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1712,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1721,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1730,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1739,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="str">
+      <c r="A65" s="24" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1749,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1758,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="str">
+      <c r="A67" s="24" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1770,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1779,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="str">
+      <c r="A69" s="24" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1791,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1814,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="25" t="str">
+      <c r="A73" s="24" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1826,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1835,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="str">
+      <c r="A75" s="24" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1847,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1856,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1869,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="30"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="27"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="str">
+      <c r="A79" s="24" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1888,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1897,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="str">
+      <c r="A81" s="24" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1909,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
+      <c r="A82" s="24"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1918,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="str">
+      <c r="A83" s="24" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1930,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
+      <c r="A84" s="24"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1939,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="24"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="25" t="str">
+      <c r="A86" s="24" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1958,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
+      <c r="A87" s="24"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1967,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
+      <c r="A88" s="24"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1976,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="24"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1985,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
+      <c r="A90" s="24"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1994,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
+      <c r="A91" s="24"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2003,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="str">
+      <c r="A92" s="24" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2015,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
+      <c r="A93" s="24"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2024,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
+      <c r="A94" s="24"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2033,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
+      <c r="A95" s="24"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2042,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="str">
+      <c r="A96" s="24" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2054,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="24"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2063,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
+      <c r="A98" s="24"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2072,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="str">
+      <c r="A99" s="24" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2084,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
+      <c r="A100" s="24"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2093,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="24"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2102,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="24"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2111,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2120,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="str">
+      <c r="A104" s="24" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2132,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
+      <c r="A105" s="24"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2141,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
+      <c r="A106" s="24"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2150,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="str">
+      <c r="A107" s="24" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2162,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="25"/>
+      <c r="A108" s="24"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2187,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="24" t="s">
+      <c r="A110" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="24"/>
+      <c r="B110" s="34"/>
+      <c r="C110" s="34"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="24" t="str">
+      <c r="A111" s="34" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2206,7 +2209,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="24"/>
+      <c r="A112" s="34"/>
       <c r="B112" s="9" t="s">
         <v>174</v>
       </c>
@@ -2215,7 +2218,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="24"/>
+      <c r="A113" s="34"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2224,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="24"/>
+      <c r="A114" s="34"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2233,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="24"/>
+      <c r="A115" s="34"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2242,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="24" t="str">
+      <c r="A116" s="34" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2254,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="24"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2263,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="24" t="str">
+      <c r="A118" s="34" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2275,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="24"/>
+      <c r="A119" s="34"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2284,7 +2287,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="24"/>
+      <c r="A120" s="34"/>
       <c r="B120" s="9" t="s">
         <v>176</v>
       </c>
@@ -2293,7 +2296,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="24" t="str">
+      <c r="A121" s="34" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2305,25 +2308,31 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="24"/>
-      <c r="B122" s="16" t="s">
+      <c r="A122" s="34"/>
+      <c r="B122" s="35" t="s">
         <v>163</v>
       </c>
+      <c r="C122" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="24"/>
+      <c r="A123" s="34"/>
       <c r="B123" s="9" t="s">
         <v>181</v>
       </c>
+      <c r="C123" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="24"/>
+      <c r="A124" s="34"/>
       <c r="B124" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="24" t="str">
+      <c r="A125" s="34" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2332,19 +2341,19 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="24"/>
+      <c r="A126" s="34"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="24"/>
+      <c r="A127" s="34"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="24" t="str">
+      <c r="A128" s="34" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2353,25 +2362,25 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="24"/>
+      <c r="A129" s="34"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="24"/>
+      <c r="A130" s="34"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="24"/>
+      <c r="A131" s="34"/>
       <c r="B131" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="24" t="str">
+      <c r="A132" s="34" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2380,47 +2389,31 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="24"/>
+      <c r="A133" s="34"/>
       <c r="B133" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="24"/>
+      <c r="A134" s="34"/>
       <c r="B134" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2432,14 +2425,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last few bugs with compound curves fixed.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -754,7 +754,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -777,18 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="str">
+      <c r="A3" s="26" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="str">
+      <c r="A6" s="26" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="str">
+      <c r="A12" s="26" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="str">
+      <c r="A15" s="26" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="str">
+      <c r="A19" s="26" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="str">
+      <c r="A21" s="26" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="str">
+      <c r="A25" s="26" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="str">
+      <c r="A27" s="26" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="str">
+      <c r="A34" s="26" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="str">
+      <c r="A38" s="26" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="str">
+      <c r="A41" s="26" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="str">
+      <c r="A45" s="26" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="str">
+      <c r="A47" s="26" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="31"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="str">
+      <c r="A51" s="26" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="str">
+      <c r="A54" s="26" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="str">
+      <c r="A56" s="26" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="str">
+      <c r="A58" s="26" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="24"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="24"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="str">
+      <c r="A65" s="26" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="24"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="str">
+      <c r="A67" s="26" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="str">
+      <c r="A69" s="26" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="str">
+      <c r="A73" s="26" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="str">
+      <c r="A75" s="26" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="28"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="26"/>
-      <c r="C78" s="27"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="str">
+      <c r="A79" s="26" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="24"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="str">
+      <c r="A81" s="26" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="24"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="24" t="str">
+      <c r="A83" s="26" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="24"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="str">
+      <c r="A86" s="26" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="24"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="24"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="24"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="24" t="str">
+      <c r="A92" s="26" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="24" t="str">
+      <c r="A96" s="26" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="24"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="24"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="24" t="str">
+      <c r="A99" s="26" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="24"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="24"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="24"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="24"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="24" t="str">
+      <c r="A104" s="26" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="24"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="24"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="24" t="str">
+      <c r="A107" s="26" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="24"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="34" t="s">
+      <c r="A110" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="34"/>
-      <c r="C110" s="34"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="str">
+      <c r="A111" s="25" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="9" t="s">
         <v>174</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
+      <c r="A113" s="25"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
+      <c r="A115" s="25"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="34" t="str">
+      <c r="A116" s="25" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+      <c r="A117" s="25"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="34" t="str">
+      <c r="A118" s="25" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="34"/>
+      <c r="A120" s="25"/>
       <c r="B120" s="9" t="s">
         <v>176</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="34" t="str">
+      <c r="A121" s="25" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2308,8 +2308,8 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
-      <c r="B122" s="35" t="s">
+      <c r="A122" s="25"/>
+      <c r="B122" s="24" t="s">
         <v>163</v>
       </c>
       <c r="C122" t="s">
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+      <c r="A123" s="25"/>
       <c r="B123" s="9" t="s">
         <v>181</v>
       </c>
@@ -2326,13 +2326,16 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+      <c r="A124" s="25"/>
       <c r="B124" s="9" t="s">
         <v>182</v>
       </c>
+      <c r="C124" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="34" t="str">
+      <c r="A125" s="25" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2341,19 +2344,19 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+      <c r="A126" s="25"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+      <c r="A127" s="25"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="34" t="str">
+      <c r="A128" s="25" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2362,25 +2365,25 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+      <c r="A129" s="25"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="34"/>
+      <c r="A130" s="25"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="34"/>
+      <c r="A131" s="25"/>
       <c r="B131" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="34" t="str">
+      <c r="A132" s="25" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2389,31 +2392,47 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+      <c r="A133" s="25"/>
       <c r="B133" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+      <c r="A134" s="25"/>
       <c r="B134" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2425,30 +2444,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Buffer stop tool added and working
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -757,16 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -789,6 +780,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="25" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="str">
+      <c r="A6" s="25" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="str">
+      <c r="A12" s="25" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="str">
+      <c r="A15" s="25" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="str">
+      <c r="A19" s="25" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="25" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
+      <c r="A25" s="25" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="str">
+      <c r="A27" s="25" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="str">
+      <c r="A34" s="25" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="str">
+      <c r="A38" s="25" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="str">
+      <c r="A41" s="25" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="str">
+      <c r="A45" s="25" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="str">
+      <c r="A47" s="25" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="str">
+      <c r="A51" s="25" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="str">
+      <c r="A54" s="25" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="str">
+      <c r="A56" s="25" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="str">
+      <c r="A58" s="25" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="str">
+      <c r="A65" s="25" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="str">
+      <c r="A67" s="25" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="str">
+      <c r="A69" s="25" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="str">
+      <c r="A73" s="25" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26" t="str">
+      <c r="A75" s="25" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="26" t="str">
+      <c r="A79" s="25" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="str">
+      <c r="A81" s="25" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="str">
+      <c r="A83" s="25" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26" t="str">
+      <c r="A86" s="25" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="26" t="str">
+      <c r="A92" s="25" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="26" t="str">
+      <c r="A96" s="25" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="26" t="str">
+      <c r="A99" s="25" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="26" t="str">
+      <c r="A104" s="25" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="26" t="str">
+      <c r="A107" s="25" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
+      <c r="A108" s="25"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="str">
+      <c r="A111" s="35" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
+      <c r="A112" s="35"/>
       <c r="B112" s="9" t="s">
         <v>174</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
+      <c r="A113" s="35"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
+      <c r="A114" s="35"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="25"/>
+      <c r="A115" s="35"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="25" t="str">
+      <c r="A116" s="35" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="25" t="str">
+      <c r="A118" s="35" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
+      <c r="A119" s="35"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
+      <c r="A120" s="35"/>
       <c r="B120" s="9" t="s">
         <v>176</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="25" t="str">
+      <c r="A121" s="35" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="24" t="s">
         <v>163</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="25"/>
+      <c r="A123" s="35"/>
       <c r="B123" s="9" t="s">
         <v>181</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
+      <c r="A124" s="35"/>
       <c r="B124" s="9" t="s">
         <v>182</v>
       </c>
@@ -2335,28 +2335,37 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="25" t="str">
+      <c r="A125" s="35" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>165</v>
       </c>
+      <c r="C125" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="25"/>
+      <c r="A126" s="35"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
+      <c r="C126" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="25"/>
+      <c r="A127" s="35"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
+      <c r="C127" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="25" t="str">
+      <c r="A128" s="35" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2365,25 +2374,25 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="25"/>
+      <c r="A129" s="35"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="25"/>
+      <c r="A130" s="35"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
+      <c r="A131" s="35"/>
       <c r="B131" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="str">
+      <c r="A132" s="35" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2392,47 +2401,31 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="25"/>
+      <c r="A133" s="35"/>
       <c r="B133" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="25"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2444,14 +2437,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tracks will no longer be placed if their colliders intersect another track's colliders.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -535,9 +535,6 @@
     <t>If a collision occurs, prevent placement and give indication of error</t>
   </si>
   <si>
-    <t>Have exceptions for colliders in sections at either end of this section.</t>
-  </si>
-  <si>
     <t>SaveLoadable for track sections needs to include data to recreate arced track</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>Track tool on a bauble will change curved track to compound curve</t>
+  </si>
+  <si>
+    <t>Have exceptions for tracks at the same level</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -780,15 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
+      <c r="A3" s="26" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
+      <c r="A6" s="26" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
+      <c r="A12" s="26" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
+      <c r="A15" s="26" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="str">
+      <c r="A19" s="26" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="str">
+      <c r="A21" s="26" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="str">
+      <c r="A25" s="26" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="str">
+      <c r="A27" s="26" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="str">
+      <c r="A34" s="26" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="str">
+      <c r="A38" s="26" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="str">
+      <c r="A41" s="26" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="str">
+      <c r="A45" s="26" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="str">
+      <c r="A47" s="26" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="str">
+      <c r="A51" s="26" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="str">
+      <c r="A54" s="26" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="str">
+      <c r="A56" s="26" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="str">
+      <c r="A58" s="26" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="str">
+      <c r="A65" s="26" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="str">
+      <c r="A67" s="26" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="str">
+      <c r="A69" s="26" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="25" t="str">
+      <c r="A73" s="26" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="str">
+      <c r="A75" s="26" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="str">
+      <c r="A79" s="26" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="str">
+      <c r="A81" s="26" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="str">
+      <c r="A83" s="26" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="25" t="str">
+      <c r="A86" s="26" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="str">
+      <c r="A92" s="26" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="str">
+      <c r="A96" s="26" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="str">
+      <c r="A99" s="26" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="str">
+      <c r="A104" s="26" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="str">
+      <c r="A107" s="26" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="25"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="35" t="s">
+      <c r="A110" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="35" t="str">
+      <c r="A111" s="25" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2209,16 +2209,16 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="35"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C112" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="35"/>
+      <c r="A113" s="25"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="35"/>
+      <c r="A115" s="25"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="35" t="str">
+      <c r="A116" s="25" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="35"/>
+      <c r="A117" s="25"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="35" t="str">
+      <c r="A118" s="25" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="35"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2287,28 +2287,28 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+      <c r="A120" s="25"/>
       <c r="B120" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C120" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="35" t="str">
+      <c r="A121" s="25" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C121" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="35"/>
+      <c r="A122" s="25"/>
       <c r="B122" s="24" t="s">
         <v>163</v>
       </c>
@@ -2317,25 +2317,25 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="35"/>
+      <c r="A123" s="25"/>
       <c r="B123" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="25"/>
+      <c r="B124" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C123" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="35"/>
-      <c r="B124" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="C124" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="35" t="str">
+      <c r="A125" s="25" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="35"/>
+      <c r="A126" s="25"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="35"/>
+      <c r="A127" s="25"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
@@ -2365,67 +2365,92 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="35" t="str">
+      <c r="A128" s="25" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
         <v>168</v>
       </c>
+      <c r="C128" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="35"/>
+      <c r="A129" s="25"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
+      <c r="C129" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+      <c r="A130" s="25"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="35"/>
+      <c r="A131" s="25"/>
       <c r="B131" s="9" t="s">
-        <v>171</v>
+        <v>182</v>
+      </c>
+      <c r="C131" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="35" t="str">
+      <c r="A132" s="25" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="25"/>
+      <c r="B133" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="35"/>
-      <c r="B133" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="35"/>
+      <c r="A134" s="25"/>
       <c r="B134" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2437,30 +2462,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2777,12 +2786,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -2797,7 +2806,7 @@
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Track sections will now highlight if placement is found to be invalid.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -757,16 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -789,6 +780,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="25" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="str">
+      <c r="A6" s="25" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="str">
+      <c r="A12" s="25" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="str">
+      <c r="A15" s="25" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="str">
+      <c r="A19" s="25" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="25" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
+      <c r="A25" s="25" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="str">
+      <c r="A27" s="25" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="str">
+      <c r="A34" s="25" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="str">
+      <c r="A38" s="25" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="str">
+      <c r="A41" s="25" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="str">
+      <c r="A45" s="25" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="str">
+      <c r="A47" s="25" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="str">
+      <c r="A51" s="25" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="str">
+      <c r="A54" s="25" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="str">
+      <c r="A56" s="25" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="str">
+      <c r="A58" s="25" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="str">
+      <c r="A65" s="25" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="str">
+      <c r="A67" s="25" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="str">
+      <c r="A69" s="25" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="str">
+      <c r="A73" s="25" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26" t="str">
+      <c r="A75" s="25" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="26" t="str">
+      <c r="A79" s="25" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="str">
+      <c r="A81" s="25" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="str">
+      <c r="A83" s="25" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26" t="str">
+      <c r="A86" s="25" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="26" t="str">
+      <c r="A92" s="25" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="26" t="str">
+      <c r="A96" s="25" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="26" t="str">
+      <c r="A99" s="25" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="26" t="str">
+      <c r="A104" s="25" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="26" t="str">
+      <c r="A107" s="25" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
+      <c r="A108" s="25"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="str">
+      <c r="A111" s="35" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
+      <c r="A112" s="35"/>
       <c r="B112" s="9" t="s">
         <v>173</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
+      <c r="A113" s="35"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
+      <c r="A114" s="35"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="25"/>
+      <c r="A115" s="35"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="25" t="str">
+      <c r="A116" s="35" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="25" t="str">
+      <c r="A118" s="35" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
+      <c r="A119" s="35"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
+      <c r="A120" s="35"/>
       <c r="B120" s="9" t="s">
         <v>175</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="25" t="str">
+      <c r="A121" s="35" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="24" t="s">
         <v>163</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="25"/>
+      <c r="A123" s="35"/>
       <c r="B123" s="9" t="s">
         <v>180</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
+      <c r="A124" s="35"/>
       <c r="B124" s="9" t="s">
         <v>181</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="25" t="str">
+      <c r="A125" s="35" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="25"/>
+      <c r="A126" s="35"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="25"/>
+      <c r="A127" s="35"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="25" t="str">
+      <c r="A128" s="35" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="25"/>
+      <c r="A129" s="35"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
@@ -2386,13 +2386,16 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="25"/>
+      <c r="A130" s="35"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
+      <c r="C130" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
+      <c r="A131" s="35"/>
       <c r="B131" s="9" t="s">
         <v>182</v>
       </c>
@@ -2401,7 +2404,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="str">
+      <c r="A132" s="35" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2410,47 +2413,31 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="25"/>
+      <c r="A133" s="35"/>
       <c r="B133" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="25"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="9" t="s">
         <v>174</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2462,14 +2449,30 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Buffer stops save, load and are linked to their baubles post-load.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="183">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -535,18 +535,12 @@
     <t>If a collision occurs, prevent placement and give indication of error</t>
   </si>
   <si>
-    <t>SaveLoadable for track sections needs to include data to recreate arced track</t>
-  </si>
-  <si>
     <t>New Saveloadable for buffer stops; need track UIDs</t>
   </si>
   <si>
     <t>Track tool must maintain list for making them visible/invisible</t>
   </si>
   <si>
-    <t>The post-save linking process should include buffer stops</t>
-  </si>
-  <si>
     <t>Once the file is completely loaded and deserialized, the track tool must go through the track sections and link to bauble objects based on IDs.</t>
   </si>
   <si>
@@ -569,6 +563,12 @@
   </si>
   <si>
     <t>Have exceptions for tracks at the same level</t>
+  </si>
+  <si>
+    <t>SaveLoadable for track sections needs to include data to recreate compound track</t>
+  </si>
+  <si>
+    <t>The post-load linking process should include buffer stops</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -780,15 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1116,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
+      <c r="A3" s="26" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
+      <c r="A6" s="26" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
+      <c r="A12" s="26" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
+      <c r="A15" s="26" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="str">
+      <c r="A19" s="26" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="str">
+      <c r="A21" s="26" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1344,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="str">
+      <c r="A25" s="26" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="str">
+      <c r="A27" s="26" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="str">
+      <c r="A34" s="26" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="str">
+      <c r="A38" s="26" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="str">
+      <c r="A41" s="26" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="str">
+      <c r="A45" s="26" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="str">
+      <c r="A47" s="26" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1597,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="str">
+      <c r="A51" s="26" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="str">
+      <c r="A54" s="26" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="str">
+      <c r="A56" s="26" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="str">
+      <c r="A58" s="26" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="str">
+      <c r="A65" s="26" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="str">
+      <c r="A67" s="26" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="str">
+      <c r="A69" s="26" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1794,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="25" t="str">
+      <c r="A73" s="26" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="str">
+      <c r="A75" s="26" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="str">
+      <c r="A79" s="26" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="str">
+      <c r="A81" s="26" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="str">
+      <c r="A83" s="26" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +1942,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="25" t="str">
+      <c r="A86" s="26" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="str">
+      <c r="A92" s="26" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="str">
+      <c r="A96" s="26" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="str">
+      <c r="A99" s="26" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="str">
+      <c r="A104" s="26" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2153,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="str">
+      <c r="A107" s="26" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="25"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,14 +2190,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="35" t="s">
+      <c r="A110" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="35" t="str">
+      <c r="A111" s="25" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2209,16 +2209,16 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="35"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="35"/>
+      <c r="A113" s="25"/>
       <c r="B113" s="9" t="s">
         <v>156</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="35"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="9" t="s">
         <v>159</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="35"/>
+      <c r="A115" s="25"/>
       <c r="B115" s="9" t="s">
         <v>160</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="35" t="str">
+      <c r="A116" s="25" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="35"/>
+      <c r="A117" s="25"/>
       <c r="B117" s="9" t="s">
         <v>158</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="35" t="str">
+      <c r="A118" s="25" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="35"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="9" t="s">
         <v>162</v>
       </c>
@@ -2287,28 +2287,28 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="35"/>
+      <c r="A120" s="25"/>
       <c r="B120" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C120" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="35" t="str">
+      <c r="A121" s="25" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C121" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="35"/>
+      <c r="A122" s="25"/>
       <c r="B122" s="24" t="s">
         <v>163</v>
       </c>
@@ -2317,25 +2317,25 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="35"/>
+      <c r="A123" s="25"/>
       <c r="B123" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C123" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="35"/>
+      <c r="A124" s="25"/>
       <c r="B124" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C124" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="35" t="str">
+      <c r="A125" s="25" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="35"/>
+      <c r="A126" s="25"/>
       <c r="B126" s="9" t="s">
         <v>166</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="35"/>
+      <c r="A127" s="25"/>
       <c r="B127" s="9" t="s">
         <v>167</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="35" t="str">
+      <c r="A128" s="25" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="35"/>
+      <c r="A129" s="25"/>
       <c r="B129" s="9" t="s">
         <v>169</v>
       </c>
@@ -2386,7 +2386,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+      <c r="A130" s="25"/>
       <c r="B130" s="9" t="s">
         <v>170</v>
       </c>
@@ -2395,49 +2395,74 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="35"/>
+      <c r="A131" s="25"/>
       <c r="B131" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C131" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="35" t="str">
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="25" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="25"/>
+      <c r="B133" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="35"/>
-      <c r="B133" s="9" t="s">
-        <v>172</v>
+      <c r="C133" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="35"/>
+      <c r="A134" s="25"/>
       <c r="B134" s="9" t="s">
-        <v>174</v>
+        <v>182</v>
+      </c>
+      <c r="C134" t="s">
+        <v>24</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2449,30 +2474,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2779,7 +2788,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2789,12 +2798,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -2809,7 +2818,7 @@
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated project to work with Unity version 5.0.0f4.  Includes some workarounds for Unity Test Tools bugs.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -14,13 +14,15 @@
     <sheet name="Stories 4" sheetId="7" r:id="rId5"/>
     <sheet name="Stories 5" sheetId="9" r:id="rId6"/>
     <sheet name="Stories 6" sheetId="10" r:id="rId7"/>
+    <sheet name="Stories 7" sheetId="11" r:id="rId8"/>
+    <sheet name="Stories 8" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="205">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -475,9 +477,6 @@
     <t>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</t>
   </si>
   <si>
-    <t>I want to be able to create a new bauble partway around a curve.</t>
-  </si>
-  <si>
     <t>Loading a map containing linked track sections should allow me to use the links correctly.</t>
   </si>
   <si>
@@ -550,9 +549,6 @@
     <t>Upgrade to Unity 5</t>
   </si>
   <si>
-    <t>Design. Seriously.</t>
-  </si>
-  <si>
     <t>Find equation to govern shape of a section with two different transitions</t>
   </si>
   <si>
@@ -569,6 +565,78 @@
   </si>
   <si>
     <t>The post-load linking process should include buffer stops</t>
+  </si>
+  <si>
+    <t>I want to be able to create a new bauble partway along straight track</t>
+  </si>
+  <si>
+    <t>Redesign whole project, including defining locomotives, carriages and props.</t>
+  </si>
+  <si>
+    <t>Refactor existing project components into new design.</t>
+  </si>
+  <si>
+    <t>Iteration 6</t>
+  </si>
+  <si>
+    <t>Download and install latest version of Unity</t>
+  </si>
+  <si>
+    <t>Update obsoleted API calls</t>
+  </si>
+  <si>
+    <t>Restore Test Tools icon functionality</t>
+  </si>
+  <si>
+    <t>Get rid of Test Tools-related warnings</t>
+  </si>
+  <si>
+    <t>Create UML of project in its current state.</t>
+  </si>
+  <si>
+    <t>Update project UML to desired state.</t>
+  </si>
+  <si>
+    <t>Add locomotives, carriages and props to UML</t>
+  </si>
+  <si>
+    <t>*tasks pending new design*</t>
+  </si>
+  <si>
+    <t>Project UML should have a place where this function results can be accessed by Vertex Bender and Track Section Controller.  If not, redesign.</t>
+  </si>
+  <si>
+    <t>Rewrite crease placement algorithm to accommodate compound curves</t>
+  </si>
+  <si>
+    <t>I want trains moving along the track to do so smoothly (Bezier curves and LeanTween)</t>
+  </si>
+  <si>
+    <t>Extant track section should split in half attaching each half to the new bauble</t>
+  </si>
+  <si>
+    <t>A new track section should be created starting from the new bauble</t>
+  </si>
+  <si>
+    <t>Hovering over straight track should highlight it as connectable</t>
+  </si>
+  <si>
+    <t>left-click on highlighted track should create a correctly-oriented bauble in the middle of the track nearest the cursor</t>
+  </si>
+  <si>
+    <t>TerrainController's line function should make some checks before writing to terrainData</t>
+  </si>
+  <si>
+    <t>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</t>
+  </si>
+  <si>
+    <t>Prevent spacebar from activating buttons.</t>
+  </si>
+  <si>
+    <t>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</t>
+  </si>
+  <si>
+    <t>I want to be able to create a new bauble partway along curved track.</t>
   </si>
 </sst>
 </file>
@@ -701,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -757,22 +825,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -789,6 +858,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,14 +1191,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="30" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1135,7 +1210,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1219,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1228,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="str">
+      <c r="A6" s="30" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1165,7 +1240,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1249,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1258,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1267,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1276,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1285,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="str">
+      <c r="A12" s="30" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1222,7 +1297,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1306,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1315,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="str">
+      <c r="A15" s="30" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1252,7 +1327,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1336,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1345,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1354,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="str">
+      <c r="A19" s="30" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1291,7 +1366,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1375,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="30" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1312,7 +1387,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,11 +1400,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1344,7 +1419,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
+      <c r="A25" s="30" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1356,7 +1431,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1365,7 +1440,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="str">
+      <c r="A27" s="30" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1377,7 +1452,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1461,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1470,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1404,7 +1479,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1488,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1497,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1506,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="str">
+      <c r="A34" s="30" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1443,7 +1518,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1527,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1536,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1545,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="str">
+      <c r="A38" s="30" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1482,7 +1557,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1578,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="str">
+      <c r="A41" s="30" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1515,7 +1590,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1599,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1608,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1542,7 +1617,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="str">
+      <c r="A45" s="30" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1554,7 +1629,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1638,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="str">
+      <c r="A47" s="30" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1575,7 +1650,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1659,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1597,14 +1672,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="str">
+      <c r="A51" s="30" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1616,7 +1691,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1700,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1709,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="str">
+      <c r="A54" s="30" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1646,7 +1721,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1655,7 +1730,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="str">
+      <c r="A56" s="30" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1667,7 +1742,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1676,7 +1751,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="str">
+      <c r="A58" s="30" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1688,7 +1763,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1697,7 +1772,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1706,7 +1781,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1790,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1799,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1733,7 +1808,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1742,7 +1817,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="str">
+      <c r="A65" s="30" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1752,7 +1827,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1761,7 +1836,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="str">
+      <c r="A67" s="30" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1773,7 +1848,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1782,7 +1857,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="str">
+      <c r="A69" s="30" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1794,21 +1869,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1817,7 +1892,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="str">
+      <c r="A73" s="30" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1829,7 +1904,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1838,7 +1913,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26" t="str">
+      <c r="A75" s="30" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1850,7 +1925,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1859,7 +1934,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1872,14 +1947,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="26" t="str">
+      <c r="A79" s="30" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1891,7 +1966,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1975,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="str">
+      <c r="A81" s="30" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1912,7 +1987,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -1921,7 +1996,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="str">
+      <c r="A83" s="30" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -1933,7 +2008,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -1942,14 +2017,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26" t="str">
+      <c r="A86" s="30" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -1961,7 +2036,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -1970,7 +2045,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +2054,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -1988,7 +2063,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -1997,7 +2072,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2081,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="26" t="str">
+      <c r="A92" s="30" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2018,7 +2093,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2102,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2036,7 +2111,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2120,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="26" t="str">
+      <c r="A96" s="30" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2057,7 +2132,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2141,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2075,7 +2150,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="26" t="str">
+      <c r="A99" s="30" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2087,7 +2162,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2096,7 +2171,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2105,7 +2180,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2114,7 +2189,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2198,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="26" t="str">
+      <c r="A104" s="30" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2135,7 +2210,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2219,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2153,7 +2228,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="26" t="str">
+      <c r="A107" s="30" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2165,7 +2240,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2190,246 +2265,246 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
+      <c r="A110" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="str">
+      <c r="A111" s="31" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="30"/>
+      <c r="B112" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="30"/>
+      <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
-      <c r="B112" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C112" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
-      <c r="B113" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="C113" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="30"/>
+      <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C114" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="25"/>
-      <c r="B115" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="C115" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="25" t="str">
+      <c r="A116" s="30" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
       <c r="B116" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="30"/>
+      <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C116" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
-      <c r="B117" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="C117" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="25" t="str">
+      <c r="A118" s="30" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
       <c r="B118" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="30"/>
+      <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C118" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
-      <c r="B119" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="C119" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
+      <c r="A120" s="30"/>
       <c r="B120" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C120" t="s">
+        <v>172</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="25" t="str">
+      <c r="A121" s="30" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="30"/>
+      <c r="B122" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="30"/>
+      <c r="B123" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="30"/>
+      <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C121" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
-      <c r="B122" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="C122" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="25"/>
-      <c r="B123" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C123" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
-      <c r="B124" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="C124" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="25" t="str">
+      <c r="A125" s="30" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="30"/>
+      <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C125" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="25"/>
-      <c r="B126" s="9" t="s">
+      <c r="C126" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="30"/>
+      <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C126" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="25"/>
-      <c r="B127" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C127" t="s">
+      <c r="C127" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="25" t="str">
+      <c r="A128" s="30" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="30"/>
+      <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C128" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="25"/>
-      <c r="B129" s="9" t="s">
+      <c r="C129" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="30"/>
+      <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C129" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="25"/>
-      <c r="B130" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="C130" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="str">
+      <c r="A132" s="30" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C132" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="25"/>
+      <c r="A133" s="30"/>
       <c r="B133" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C133" t="s">
+        <v>170</v>
+      </c>
+      <c r="C133" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="25"/>
-      <c r="B134" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C134" t="s">
+      <c r="A134" s="33"/>
+      <c r="B134" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D134">
@@ -2437,32 +2512,186 @@
         <v>24</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="28" t="str">
+        <f>'Stories 6'!A1</f>
+        <v>Upgrade to Unity 5</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="28"/>
+      <c r="B137" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="28"/>
+      <c r="B138" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="28"/>
+      <c r="B139" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="28"/>
+      <c r="B140" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="28" t="str">
+        <f>'Stories 6'!A2</f>
+        <v>Redesign whole project, including defining locomotives, carriages and props.</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="28"/>
+      <c r="B142" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="28"/>
+      <c r="B143" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="28" t="str">
+        <f>'Stories 6'!A3</f>
+        <v>Refactor existing project components into new design.</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="28"/>
+      <c r="B145" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="28"/>
+      <c r="B146" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="28"/>
+      <c r="B147" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="28"/>
+      <c r="B148" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="28" t="str">
+        <f>'Stories 6'!A4</f>
+        <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="28"/>
+      <c r="B150" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="28" t="str">
+        <f>'Stories 6'!A5</f>
+        <v>I want to be able to create a new bauble partway along straight track</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="28"/>
+      <c r="B152" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="28"/>
+      <c r="B153" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="28"/>
+      <c r="B154" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="27" t="str">
+        <f>'Stories 6'!A6</f>
+        <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D155">
+        <f>COUNTA(C136:C155)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="27"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+  <mergeCells count="49">
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2474,14 +2703,36 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A148"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2755,7 +3006,7 @@
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -2775,7 +3026,7 @@
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2785,10 +3036,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2798,28 +3049,95 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>174</v>
-      </c>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Addition of class relationship diagram in NClass. Includes minor changes to code structure.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="209">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>I want to be able to create a new bauble partway along curved track.</t>
+  </si>
+  <si>
+    <t>SaveLoad should be a superclass that all SaveLoads inherit</t>
+  </si>
+  <si>
+    <t>UID should be a part of SaveLoad</t>
+  </si>
+  <si>
+    <t>Itool should be an abstract class which inherits monobehaviour and implements some Tool functions</t>
+  </si>
+  <si>
+    <t>Replace inner wrapper classes with humble object pattern</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1181,7 @@
   <dimension ref="A1:D157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,6 +2587,9 @@
       <c r="B141" s="9" t="s">
         <v>189</v>
       </c>
+      <c r="C141" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="28"/>
@@ -2594,25 +2609,25 @@
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="28"/>
       <c r="B145" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="28"/>
       <c r="B146" s="9" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="28"/>
       <c r="B147" s="9" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2673,7 +2688,7 @@
       </c>
       <c r="D155">
         <f>COUNTA(C136:C155)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Class diagram now includes future structure improvements and some additional features.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="210">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -600,9 +600,6 @@
     <t>Add locomotives, carriages and props to UML</t>
   </si>
   <si>
-    <t>*tasks pending new design*</t>
-  </si>
-  <si>
     <t>Project UML should have a place where this function results can be accessed by Vertex Bender and Track Section Controller.  If not, redesign.</t>
   </si>
   <si>
@@ -649,6 +646,12 @@
   </si>
   <si>
     <t>Replace inner wrapper classes with humble object pattern</t>
+  </si>
+  <si>
+    <t>Control should hold lists of track sections etc. TrackPlacementTool should access objects through control, and object loading should be done by fileHandler</t>
+  </si>
+  <si>
+    <t>track sections, buffer stops and baubles should all add themselves to Control's lists ?through the SaveLoad abstract class?</t>
   </si>
 </sst>
 </file>
@@ -844,22 +847,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -870,12 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D157"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,14 +1206,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="str">
+      <c r="A3" s="28" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1222,7 +1225,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1231,7 +1234,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1240,7 +1243,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="str">
+      <c r="A6" s="28" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1252,7 +1255,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1261,7 +1264,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1273,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1282,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1288,7 +1291,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1300,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="28" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1309,7 +1312,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1318,7 +1321,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1327,7 +1330,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="28" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1339,7 +1342,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1348,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1360,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1366,7 +1369,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="28" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1378,7 +1381,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1387,7 +1390,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="28" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1399,7 +1402,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1415,8 +1418,8 @@
       <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1431,7 +1434,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="str">
+      <c r="A25" s="28" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1443,7 +1446,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1452,7 +1455,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="str">
+      <c r="A27" s="28" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1464,7 +1467,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1473,7 +1476,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1482,7 +1485,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1491,7 +1494,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1500,7 +1503,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1509,7 +1512,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1518,7 +1521,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="str">
+      <c r="A34" s="28" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1530,7 +1533,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1539,7 +1542,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1548,7 +1551,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1557,7 +1560,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="str">
+      <c r="A38" s="28" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1569,7 +1572,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1590,7 +1593,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="str">
+      <c r="A41" s="28" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1602,7 +1605,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1611,7 +1614,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1623,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1632,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="str">
+      <c r="A45" s="28" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1641,7 +1644,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1650,7 +1653,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="str">
+      <c r="A47" s="28" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1662,7 +1665,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1671,7 +1674,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1684,14 +1687,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="str">
+      <c r="A51" s="28" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1703,7 +1706,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1712,7 +1715,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1721,7 +1724,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="str">
+      <c r="A54" s="28" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1733,7 +1736,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1742,7 +1745,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="str">
+      <c r="A56" s="28" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1754,7 +1757,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1763,7 +1766,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="str">
+      <c r="A58" s="28" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1775,7 +1778,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1784,7 +1787,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1793,7 +1796,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1802,7 +1805,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1811,7 +1814,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1820,7 +1823,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1829,7 +1832,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="str">
+      <c r="A65" s="28" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="28"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1848,7 +1851,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="str">
+      <c r="A67" s="28" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1860,7 +1863,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1869,7 +1872,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="str">
+      <c r="A69" s="28" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1881,21 +1884,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="28"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1904,7 +1907,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="str">
+      <c r="A73" s="28" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1916,7 +1919,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1925,7 +1928,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="str">
+      <c r="A75" s="28" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1937,7 +1940,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1946,7 +1949,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1962,11 +1965,11 @@
       <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="32"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="35"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="str">
+      <c r="A79" s="28" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1978,7 +1981,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1987,7 +1990,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="str">
+      <c r="A81" s="28" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -1999,7 +2002,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="28"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2008,7 +2011,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="str">
+      <c r="A83" s="28" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2020,7 +2023,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2029,14 +2032,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="28"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="str">
+      <c r="A86" s="28" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2048,7 +2051,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2057,7 +2060,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="28"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2066,7 +2069,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="28"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2075,7 +2078,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="28"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2084,7 +2087,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="28"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2093,7 +2096,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="str">
+      <c r="A92" s="28" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2105,7 +2108,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="28"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2114,7 +2117,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="28"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2123,7 +2126,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="28"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2132,7 +2135,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="str">
+      <c r="A96" s="28" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2144,7 +2147,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="28"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2153,7 +2156,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="28"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2162,7 +2165,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="str">
+      <c r="A99" s="28" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2174,7 +2177,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="28"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2183,7 +2186,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="28"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2192,7 +2195,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="28"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2201,7 +2204,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="28"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2210,7 +2213,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="str">
+      <c r="A104" s="28" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2222,7 +2225,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="28"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2231,7 +2234,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="28"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2240,7 +2243,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="30" t="str">
+      <c r="A107" s="28" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2252,7 +2255,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="28"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2277,11 +2280,11 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="str">
@@ -2296,7 +2299,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="28"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2305,7 +2308,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="28"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2314,7 +2317,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="28"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2323,7 +2326,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="28"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2332,7 +2335,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="str">
+      <c r="A116" s="28" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2344,7 +2347,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="28"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2353,7 +2356,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="30" t="str">
+      <c r="A118" s="28" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2365,7 +2368,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="28"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2374,7 +2377,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="A120" s="28"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2383,7 +2386,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="str">
+      <c r="A121" s="28" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2395,7 +2398,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="28"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2404,7 +2407,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="28"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2413,7 +2416,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="28"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2422,7 +2425,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30" t="str">
+      <c r="A125" s="28" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2434,7 +2437,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="28"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2443,7 +2446,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="28"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2452,7 +2455,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30" t="str">
+      <c r="A128" s="28" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2464,7 +2467,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="28"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2473,7 +2476,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="28"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2482,7 +2485,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="28"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2491,7 +2494,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="str">
+      <c r="A132" s="28" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2503,7 +2506,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="28"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2512,7 +2515,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2525,14 +2528,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="29" t="s">
+      <c r="A135" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="29"/>
-      <c r="C135" s="29"/>
+      <c r="B135" s="34"/>
+      <c r="C135" s="34"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="28" t="str">
+      <c r="A136" s="30" t="str">
         <f>'Stories 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2544,7 +2547,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2553,16 +2556,16 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="28"/>
+      <c r="A138" s="30"/>
       <c r="B138" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="28"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2571,7 +2574,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="28"/>
+      <c r="A140" s="30"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2580,7 +2583,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="28" t="str">
+      <c r="A141" s="30" t="str">
         <f>'Stories 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2592,121 +2595,155 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="28"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
+      <c r="C142" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="28"/>
+      <c r="A143" s="30"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
+      <c r="C143" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="28" t="str">
+      <c r="A144" s="30" t="str">
         <f>'Stories 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="30"/>
+      <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="28"/>
-      <c r="B145" s="9" t="s">
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="30"/>
+      <c r="B146" s="9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="28"/>
-      <c r="B146" s="9" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="30"/>
+      <c r="B147" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="28"/>
-      <c r="B147" s="9" t="s">
+    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="30"/>
+      <c r="B148" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="28"/>
-      <c r="B148" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="28" t="str">
+      <c r="A149" s="30"/>
+      <c r="B149" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="30" t="str">
         <f>'Stories 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
-      <c r="B149" s="9" t="s">
+      <c r="B150" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="30"/>
+      <c r="B151" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="28"/>
-      <c r="B150" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="28" t="str">
+    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="30" t="str">
         <f>'Stories 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="B152" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="30"/>
+      <c r="B153" s="9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="28"/>
-      <c r="B152" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="28"/>
-      <c r="B153" s="9" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="30"/>
+      <c r="B154" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="30"/>
+      <c r="B155" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="28"/>
-      <c r="B154" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="27" t="str">
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="27" t="str">
         <f>'Stories 6'!A6</f>
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
-      <c r="B155" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D155">
-        <f>COUNTA(C136:C155)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="27"/>
+      <c r="B156" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D156">
+        <f>COUNTA(C136:C156)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="27"/>
     </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A152:A155"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2718,36 +2755,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3112,7 +3127,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,7 +3135,7 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3143,12 +3158,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
The first few tasks in the process of refactoring to a more favourable design are complete.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="210">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -642,9 +642,6 @@
     <t>UID should be a part of SaveLoad</t>
   </si>
   <si>
-    <t>Itool should be an abstract class which inherits monobehaviour and implements some Tool functions</t>
-  </si>
-  <si>
     <t>Replace inner wrapper classes with humble object pattern</t>
   </si>
   <si>
@@ -652,6 +649,9 @@
   </si>
   <si>
     <t>track sections, buffer stops and baubles should all add themselves to Control's lists ?through the SaveLoad abstract class?</t>
+  </si>
+  <si>
+    <t>Itool should be a superclass which inherits monobehaviour and implements Tool functions as defualts</t>
   </si>
 </sst>
 </file>
@@ -847,28 +847,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,6 +873,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,14 +1206,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="str">
+      <c r="A3" s="30" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1225,7 +1225,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="str">
+      <c r="A6" s="30" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1282,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="str">
+      <c r="A12" s="30" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1330,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="str">
+      <c r="A15" s="30" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="str">
+      <c r="A19" s="30" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1381,7 +1381,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="str">
+      <c r="A21" s="30" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1402,7 +1402,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1418,8 +1418,8 @@
       <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1434,7 +1434,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="str">
+      <c r="A25" s="30" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="str">
+      <c r="A27" s="30" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="str">
+      <c r="A34" s="30" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="str">
+      <c r="A38" s="30" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1593,7 +1593,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="str">
+      <c r="A41" s="30" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1623,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="str">
+      <c r="A45" s="30" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="str">
+      <c r="A47" s="30" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1687,14 +1687,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="str">
+      <c r="A51" s="30" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="str">
+      <c r="A54" s="30" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1745,7 +1745,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="str">
+      <c r="A56" s="30" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1757,7 +1757,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="str">
+      <c r="A58" s="30" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="28"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="28"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="str">
+      <c r="A65" s="30" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="28"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="str">
+      <c r="A67" s="30" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="28"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="str">
+      <c r="A69" s="30" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1884,21 +1884,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="28"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="28"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="str">
+      <c r="A73" s="30" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1928,7 +1928,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="str">
+      <c r="A75" s="30" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1965,11 +1965,11 @@
       <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="34"/>
-      <c r="C78" s="35"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="str">
+      <c r="A79" s="30" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1990,7 +1990,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="str">
+      <c r="A81" s="30" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="28"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2011,7 +2011,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="str">
+      <c r="A83" s="30" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="28"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2032,14 +2032,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="str">
+      <c r="A86" s="30" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="28"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="str">
+      <c r="A92" s="30" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2108,7 +2108,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2117,7 +2117,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="str">
+      <c r="A96" s="30" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="28"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="28"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="str">
+      <c r="A99" s="30" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2186,7 +2186,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="28"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="28"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="str">
+      <c r="A104" s="30" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="28"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2243,7 +2243,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="28" t="str">
+      <c r="A107" s="30" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2255,7 +2255,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="28"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2280,11 +2280,11 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="30"/>
-      <c r="C110" s="30"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="str">
@@ -2299,7 +2299,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="28"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="28"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="28"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
+      <c r="A115" s="30"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="str">
+      <c r="A116" s="30" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
+      <c r="A117" s="30"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="28" t="str">
+      <c r="A118" s="30" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2368,7 +2368,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
+      <c r="A119" s="30"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="28"/>
+      <c r="A120" s="30"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2386,7 +2386,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="28" t="str">
+      <c r="A121" s="30" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="28"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2407,7 +2407,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="28"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="28"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2425,7 +2425,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="28" t="str">
+      <c r="A125" s="30" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="28"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="28"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2455,7 +2455,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="28" t="str">
+      <c r="A128" s="30" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2467,7 +2467,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="28"/>
+      <c r="A129" s="30"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="28"/>
+      <c r="A130" s="30"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2485,7 +2485,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2494,7 +2494,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="28" t="str">
+      <c r="A132" s="30" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="28"/>
+      <c r="A133" s="30"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2515,7 +2515,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="33"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2528,14 +2528,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="34" t="s">
+      <c r="A135" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="34"/>
-      <c r="C135" s="34"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="28" t="str">
         <f>'Stories 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="30"/>
+      <c r="A137" s="28"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="30"/>
+      <c r="A138" s="28"/>
       <c r="B138" s="9" t="s">
         <v>201</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
+      <c r="A139" s="28"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="30"/>
+      <c r="A140" s="28"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2583,7 +2583,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="str">
+      <c r="A141" s="28" t="str">
         <f>'Stories 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2595,7 +2595,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="30"/>
+      <c r="A142" s="28"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2604,7 +2604,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="30"/>
+      <c r="A143" s="28"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2613,46 +2613,58 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="30" t="str">
+      <c r="A144" s="28" t="str">
         <f>'Stories 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
         <v>204</v>
       </c>
+      <c r="C144" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="30"/>
+      <c r="A145" s="28"/>
       <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
+      <c r="C145" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="30"/>
+      <c r="A146" s="28"/>
       <c r="B146" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="28"/>
+      <c r="B147" s="9" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="30"/>
-      <c r="B147" s="9" t="s">
+      <c r="C147" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="28"/>
+      <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
-      <c r="B148" s="9" t="s">
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="28"/>
+      <c r="B149" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
-      <c r="B149" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="30" t="str">
+      <c r="A150" s="28" t="str">
         <f>'Stories 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -2661,13 +2673,13 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
+      <c r="A151" s="28"/>
       <c r="B151" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="30" t="str">
+      <c r="A152" s="28" t="str">
         <f>'Stories 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -2676,19 +2688,19 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="30"/>
+      <c r="A153" s="28"/>
       <c r="B153" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="30"/>
+      <c r="A154" s="28"/>
       <c r="B154" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="30"/>
+      <c r="A155" s="28"/>
       <c r="B155" s="9" t="s">
         <v>196</v>
       </c>
@@ -2703,7 +2715,7 @@
       </c>
       <c r="D156">
         <f>COUNTA(C136:C156)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,36 +2726,14 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A152:A155"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2755,14 +2745,36 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A152:A155"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
The remainder of major refactoring this iteration; less work is done by the track placement tool, some of which is picked up by the Control and FileHandler classes.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -645,13 +645,13 @@
     <t>Replace inner wrapper classes with humble object pattern</t>
   </si>
   <si>
-    <t>Control should hold lists of track sections etc. TrackPlacementTool should access objects through control, and object loading should be done by fileHandler</t>
-  </si>
-  <si>
     <t>track sections, buffer stops and baubles should all add themselves to Control's lists ?through the SaveLoad abstract class?</t>
   </si>
   <si>
     <t>Itool should be a superclass which inherits monobehaviour and implements Tool functions as defualts</t>
+  </si>
+  <si>
+    <t>Control should hold lists of track sections etc. TrackPlacementTool should access objects through control, and object loading and linking should be done by fileHandler</t>
   </si>
 </sst>
 </file>
@@ -847,22 +847,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -873,12 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:D158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,14 +1206,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="str">
+      <c r="A3" s="28" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1225,7 +1225,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="str">
+      <c r="A6" s="28" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1282,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="28" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1330,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="28" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="28" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1381,7 +1381,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="28" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1402,7 +1402,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1418,8 +1418,8 @@
       <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1434,7 +1434,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="str">
+      <c r="A25" s="28" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="str">
+      <c r="A27" s="28" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="str">
+      <c r="A34" s="28" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="str">
+      <c r="A38" s="28" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1593,7 +1593,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="str">
+      <c r="A41" s="28" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1623,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="str">
+      <c r="A45" s="28" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="str">
+      <c r="A47" s="28" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1687,14 +1687,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="str">
+      <c r="A51" s="28" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="str">
+      <c r="A54" s="28" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1745,7 +1745,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="str">
+      <c r="A56" s="28" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1757,7 +1757,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="str">
+      <c r="A58" s="28" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="str">
+      <c r="A65" s="28" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="28"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="str">
+      <c r="A67" s="28" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="str">
+      <c r="A69" s="28" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1884,21 +1884,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="28"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="str">
+      <c r="A73" s="28" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1928,7 +1928,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="str">
+      <c r="A75" s="28" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1965,11 +1965,11 @@
       <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="32"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="35"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="str">
+      <c r="A79" s="28" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1990,7 +1990,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="str">
+      <c r="A81" s="28" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="28"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2011,7 +2011,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="str">
+      <c r="A83" s="28" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2032,14 +2032,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="28"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="str">
+      <c r="A86" s="28" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="28"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="28"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="28"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="28"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="str">
+      <c r="A92" s="28" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2108,7 +2108,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="28"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2117,7 +2117,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="28"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="28"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="str">
+      <c r="A96" s="28" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="28"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="28"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="str">
+      <c r="A99" s="28" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="28"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2186,7 +2186,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="28"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="28"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="28"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="str">
+      <c r="A104" s="28" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="28"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="28"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2243,7 +2243,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="30" t="str">
+      <c r="A107" s="28" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2255,7 +2255,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="28"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2280,11 +2280,11 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="str">
@@ -2299,7 +2299,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="28"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="28"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="28"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="28"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="str">
+      <c r="A116" s="28" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="28"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="30" t="str">
+      <c r="A118" s="28" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2368,7 +2368,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="28"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="A120" s="28"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2386,7 +2386,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="str">
+      <c r="A121" s="28" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="28"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2407,7 +2407,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="28"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="28"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2425,7 +2425,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30" t="str">
+      <c r="A125" s="28" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="28"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="28"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2455,7 +2455,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30" t="str">
+      <c r="A128" s="28" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2467,7 +2467,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="28"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="28"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2485,7 +2485,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="28"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2494,7 +2494,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="str">
+      <c r="A132" s="28" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="28"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2515,7 +2515,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2528,14 +2528,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="29" t="s">
+      <c r="A135" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="29"/>
-      <c r="C135" s="29"/>
+      <c r="B135" s="34"/>
+      <c r="C135" s="34"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="28" t="str">
+      <c r="A136" s="30" t="str">
         <f>'Stories 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="28"/>
+      <c r="A138" s="30"/>
       <c r="B138" s="9" t="s">
         <v>201</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="28"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="28"/>
+      <c r="A140" s="30"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2583,7 +2583,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="28" t="str">
+      <c r="A141" s="30" t="str">
         <f>'Stories 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2595,7 +2595,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="28"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2604,7 +2604,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="28"/>
+      <c r="A143" s="30"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="28" t="str">
+      <c r="A144" s="30" t="str">
         <f>'Stories 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -2625,7 +2625,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="28"/>
+      <c r="A145" s="30"/>
       <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
@@ -2634,16 +2634,16 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="28"/>
+      <c r="A146" s="30"/>
       <c r="B146" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C146" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="28"/>
+      <c r="A147" s="30"/>
       <c r="B147" s="9" t="s">
         <v>206</v>
       </c>
@@ -2652,19 +2652,25 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="28"/>
+      <c r="A148" s="30"/>
       <c r="B148" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="30"/>
+      <c r="B149" s="9" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="28"/>
-      <c r="B149" s="9" t="s">
-        <v>208</v>
+      <c r="C149" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="28" t="str">
+      <c r="A150" s="30" t="str">
         <f>'Stories 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -2673,13 +2679,13 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="28"/>
+      <c r="A151" s="30"/>
       <c r="B151" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="28" t="str">
+      <c r="A152" s="30" t="str">
         <f>'Stories 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -2688,19 +2694,19 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="28"/>
+      <c r="A153" s="30"/>
       <c r="B153" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="28"/>
+      <c r="A154" s="30"/>
       <c r="B154" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="28"/>
+      <c r="A155" s="30"/>
       <c r="B155" s="9" t="s">
         <v>196</v>
       </c>
@@ -2715,7 +2721,7 @@
       </c>
       <c r="D156">
         <f>COUNTA(C136:C156)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,14 +2732,36 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A152:A155"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2745,36 +2773,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A152:A155"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rail vectors moved, are now also responsible for creases, and match compound curves better.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="212">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t>Control should hold lists of track sections etc. TrackPlacementTool should access objects through control, and object loading and linking should be done by fileHandler</t>
+  </si>
+  <si>
+    <t>Use rail vectors to determine creases</t>
+  </si>
+  <si>
+    <t>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</t>
   </si>
 </sst>
 </file>
@@ -847,28 +853,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,6 +879,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,14 +1212,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="str">
+      <c r="A3" s="30" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1225,7 +1231,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1240,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1243,7 +1249,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="str">
+      <c r="A6" s="30" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1255,7 +1261,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1270,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1279,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1288,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1291,7 +1297,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1306,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="str">
+      <c r="A12" s="30" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1312,7 +1318,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1327,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1336,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="str">
+      <c r="A15" s="30" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1342,7 +1348,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1357,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1360,7 +1366,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1375,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="str">
+      <c r="A19" s="30" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1381,7 +1387,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1390,7 +1396,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="str">
+      <c r="A21" s="30" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1402,7 +1408,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1418,8 +1424,8 @@
       <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1434,7 +1440,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="str">
+      <c r="A25" s="30" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1446,7 +1452,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1455,7 +1461,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="str">
+      <c r="A27" s="30" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1467,7 +1473,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1476,7 +1482,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1485,7 +1491,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1494,7 +1500,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1503,7 +1509,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1518,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1521,7 +1527,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="str">
+      <c r="A34" s="30" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1533,7 +1539,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1542,7 +1548,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1551,7 +1557,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1560,7 +1566,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="str">
+      <c r="A38" s="30" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1572,7 +1578,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1593,7 +1599,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="str">
+      <c r="A41" s="30" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1605,7 +1611,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1620,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1629,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1638,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="str">
+      <c r="A45" s="30" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1644,7 +1650,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1653,7 +1659,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="str">
+      <c r="A47" s="30" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1665,7 +1671,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1680,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1687,14 +1693,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="str">
+      <c r="A51" s="30" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1706,7 +1712,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1715,7 +1721,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1724,7 +1730,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="str">
+      <c r="A54" s="30" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1736,7 +1742,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1745,7 +1751,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="str">
+      <c r="A56" s="30" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1757,7 +1763,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1766,7 +1772,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="str">
+      <c r="A58" s="30" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1778,7 +1784,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1787,7 +1793,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1796,7 +1802,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +1811,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1814,7 +1820,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="28"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1823,7 +1829,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="28"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1832,7 +1838,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="str">
+      <c r="A65" s="30" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1842,7 +1848,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="28"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1851,7 +1857,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="str">
+      <c r="A67" s="30" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1863,7 +1869,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="28"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1872,7 +1878,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="str">
+      <c r="A69" s="30" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1884,21 +1890,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="28"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="28"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1907,7 +1913,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="str">
+      <c r="A73" s="30" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1919,7 +1925,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1928,7 +1934,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="str">
+      <c r="A75" s="30" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1940,7 +1946,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1949,7 +1955,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1965,11 +1971,11 @@
       <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="34"/>
-      <c r="C78" s="35"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="str">
+      <c r="A79" s="30" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1981,7 +1987,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1990,7 +1996,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="str">
+      <c r="A81" s="30" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2002,7 +2008,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="28"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2011,7 +2017,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="str">
+      <c r="A83" s="30" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2023,7 +2029,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="28"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2032,14 +2038,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="str">
+      <c r="A86" s="30" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2051,7 +2057,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2060,7 +2066,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2069,7 +2075,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2078,7 +2084,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2087,7 +2093,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="28"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2096,7 +2102,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="str">
+      <c r="A92" s="30" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2108,7 +2114,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2117,7 +2123,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2126,7 +2132,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2135,7 +2141,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="str">
+      <c r="A96" s="30" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2147,7 +2153,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="28"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2156,7 +2162,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="28"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2165,7 +2171,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="str">
+      <c r="A99" s="30" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2177,7 +2183,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2186,7 +2192,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="28"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2195,7 +2201,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="28"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2204,7 +2210,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2213,7 +2219,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="str">
+      <c r="A104" s="30" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2225,7 +2231,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="28"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2234,7 +2240,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2243,7 +2249,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="28" t="str">
+      <c r="A107" s="30" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2255,7 +2261,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="28"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2280,11 +2286,11 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="30"/>
-      <c r="C110" s="30"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="str">
@@ -2299,7 +2305,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="28"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2308,7 +2314,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="28"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2317,7 +2323,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="28"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2326,7 +2332,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
+      <c r="A115" s="30"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2335,7 +2341,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="str">
+      <c r="A116" s="30" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2347,7 +2353,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
+      <c r="A117" s="30"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2356,7 +2362,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="28" t="str">
+      <c r="A118" s="30" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2368,7 +2374,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
+      <c r="A119" s="30"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2377,7 +2383,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="28"/>
+      <c r="A120" s="30"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2386,7 +2392,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="28" t="str">
+      <c r="A121" s="30" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2398,7 +2404,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="28"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2407,7 +2413,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="28"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2416,7 +2422,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="28"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2425,7 +2431,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="28" t="str">
+      <c r="A125" s="30" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2437,7 +2443,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="28"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2446,7 +2452,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="28"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2455,7 +2461,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="28" t="str">
+      <c r="A128" s="30" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2467,7 +2473,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="28"/>
+      <c r="A129" s="30"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2476,7 +2482,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="28"/>
+      <c r="A130" s="30"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2485,7 +2491,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2494,7 +2500,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="28" t="str">
+      <c r="A132" s="30" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2506,7 +2512,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="28"/>
+      <c r="A133" s="30"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2515,7 +2521,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="33"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2528,14 +2534,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="34" t="s">
+      <c r="A135" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="34"/>
-      <c r="C135" s="34"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="28" t="str">
         <f>'Stories 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2547,7 +2553,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="30"/>
+      <c r="A137" s="28"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2556,7 +2562,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="30"/>
+      <c r="A138" s="28"/>
       <c r="B138" s="9" t="s">
         <v>201</v>
       </c>
@@ -2565,7 +2571,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
+      <c r="A139" s="28"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2574,7 +2580,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="30"/>
+      <c r="A140" s="28"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2583,7 +2589,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="str">
+      <c r="A141" s="28" t="str">
         <f>'Stories 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2595,7 +2601,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="30"/>
+      <c r="A142" s="28"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2604,7 +2610,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="30"/>
+      <c r="A143" s="28"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2613,7 +2619,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="30" t="str">
+      <c r="A144" s="28" t="str">
         <f>'Stories 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -2625,7 +2631,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="30"/>
+      <c r="A145" s="28"/>
       <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
@@ -2634,7 +2640,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="30"/>
+      <c r="A146" s="28"/>
       <c r="B146" s="9" t="s">
         <v>208</v>
       </c>
@@ -2643,7 +2649,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="30"/>
+      <c r="A147" s="28"/>
       <c r="B147" s="9" t="s">
         <v>206</v>
       </c>
@@ -2652,7 +2658,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
+      <c r="A148" s="28"/>
       <c r="B148" s="9" t="s">
         <v>209</v>
       </c>
@@ -2661,7 +2667,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
+      <c r="A149" s="28"/>
       <c r="B149" s="9" t="s">
         <v>207</v>
       </c>
@@ -2670,98 +2676,88 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="30" t="str">
+      <c r="A150" s="28" t="str">
         <f>'Stories 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
-      <c r="B150" s="9" t="s">
+      <c r="B150" s="24" t="s">
         <v>192</v>
       </c>
+      <c r="C150" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
-      <c r="B151" s="9" t="s">
+      <c r="A151" s="28"/>
+      <c r="B151" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C151" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="28"/>
+      <c r="B152" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="30" t="str">
+    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="28" t="str">
         <f>'Stories 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B153" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="30"/>
-      <c r="B153" s="9" t="s">
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="28"/>
+      <c r="B154" s="9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="30"/>
-      <c r="B154" s="9" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="28"/>
+      <c r="B155" s="9" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="30"/>
-      <c r="B155" s="9" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="28"/>
+      <c r="B156" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="27" t="str">
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="27" t="str">
         <f>'Stories 6'!A6</f>
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
-      <c r="B156" s="9" t="s">
+      <c r="B157" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D156">
-        <f>COUNTA(C136:C156)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="27"/>
+      <c r="D157">
+        <f>COUNTA(C136:C157)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="27"/>
     </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A152:A155"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2773,14 +2769,36 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A153:A156"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3132,10 +3150,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3143,6 +3161,11 @@
     <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
Allowed a straight track to split if another track begins or ends in its middle, and improved ballast adjustment efficiency slightly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="216">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -658,6 +658,18 @@
   </si>
   <si>
     <t>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</t>
+  </si>
+  <si>
+    <t>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</t>
+  </si>
+  <si>
+    <t>The behaviour should be the same when dragging a track to a track</t>
+  </si>
+  <si>
+    <t>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</t>
+  </si>
+  <si>
+    <t>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</t>
   </si>
 </sst>
 </file>
@@ -790,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -856,19 +868,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,12 +900,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,14 +1227,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="str">
+      <c r="A3" s="29" t="str">
         <f>'Stories 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1231,7 +1246,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1240,7 +1255,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1249,7 +1264,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="str">
+      <c r="A6" s="29" t="str">
         <f>'Stories 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1261,7 +1276,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1285,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1279,7 +1294,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1288,7 +1303,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1312,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1321,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="29" t="str">
         <f>'Stories 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1318,7 +1333,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1342,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1351,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="29" t="str">
         <f>'Stories 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1348,7 +1363,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1357,7 +1372,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1366,7 +1381,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1375,7 +1390,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="29" t="str">
         <f>'Stories 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1387,7 +1402,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1396,7 +1411,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="29" t="str">
         <f>'Stories 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1408,7 +1423,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1421,11 +1436,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1440,7 +1455,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="str">
+      <c r="A25" s="29" t="str">
         <f>'Stories 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1452,7 +1467,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1461,7 +1476,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="str">
+      <c r="A27" s="29" t="str">
         <f>'Stories 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1473,7 +1488,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1482,7 +1497,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1491,7 +1506,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1500,7 +1515,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1509,7 +1524,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1518,7 +1533,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1527,7 +1542,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="str">
+      <c r="A34" s="29" t="str">
         <f>'Stories 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1539,7 +1554,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1548,7 +1563,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1557,7 +1572,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1566,7 +1581,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="str">
+      <c r="A38" s="29" t="str">
         <f>'Stories 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1578,7 +1593,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1599,7 +1614,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="str">
+      <c r="A41" s="29" t="str">
         <f>'Stories 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1611,7 +1626,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1620,7 +1635,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1629,7 +1644,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1638,7 +1653,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="str">
+      <c r="A45" s="29" t="str">
         <f>'Stories 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1650,7 +1665,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1659,7 +1674,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="str">
+      <c r="A47" s="29" t="str">
         <f>'Stories 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1671,7 +1686,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1680,7 +1695,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1693,14 +1708,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="str">
+      <c r="A51" s="29" t="str">
         <f>'Stories 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1712,7 +1727,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1721,7 +1736,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1730,7 +1745,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="str">
+      <c r="A54" s="29" t="str">
         <f>'Stories 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1742,7 +1757,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1751,7 +1766,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="str">
+      <c r="A56" s="29" t="str">
         <f>'Stories 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1763,7 +1778,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1772,7 +1787,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="str">
+      <c r="A58" s="29" t="str">
         <f>'Stories 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1784,7 +1799,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1793,7 +1808,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1802,7 +1817,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1811,7 +1826,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1820,7 +1835,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="29"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1829,7 +1844,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="29"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1838,7 +1853,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="str">
+      <c r="A65" s="29" t="str">
         <f>'Stories 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1848,7 +1863,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="29"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1857,7 +1872,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="str">
+      <c r="A67" s="29" t="str">
         <f>'Stories 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1869,7 +1884,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="29"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1878,7 +1893,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="str">
+      <c r="A69" s="29" t="str">
         <f>'Stories 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -1890,21 +1905,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="29"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -1913,7 +1928,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="str">
+      <c r="A73" s="29" t="str">
         <f>'Stories 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -1925,7 +1940,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -1934,7 +1949,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="str">
+      <c r="A75" s="29" t="str">
         <f>'Stories 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -1946,7 +1961,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="29"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -1955,7 +1970,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1968,14 +1983,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="32"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="36"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="str">
+      <c r="A79" s="29" t="str">
         <f>'Stories 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -1987,7 +2002,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -1996,7 +2011,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="str">
+      <c r="A81" s="29" t="str">
         <f>'Stories 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2008,7 +2023,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="29"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2017,7 +2032,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="str">
+      <c r="A83" s="29" t="str">
         <f>'Stories 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2029,7 +2044,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2038,14 +2053,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="str">
+      <c r="A86" s="29" t="str">
         <f>'Stories 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2057,7 +2072,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2066,7 +2081,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="29"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2075,7 +2090,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2084,7 +2099,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2093,7 +2108,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2102,7 +2117,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="str">
+      <c r="A92" s="29" t="str">
         <f>'Stories 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2114,7 +2129,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2123,7 +2138,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2132,7 +2147,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2141,7 +2156,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="str">
+      <c r="A96" s="29" t="str">
         <f>'Stories 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2153,7 +2168,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2162,7 +2177,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2171,7 +2186,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="str">
+      <c r="A99" s="29" t="str">
         <f>'Stories 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2183,7 +2198,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2192,7 +2207,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2201,7 +2216,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2210,7 +2225,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2219,7 +2234,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="str">
+      <c r="A104" s="29" t="str">
         <f>'Stories 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2231,7 +2246,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2240,7 +2255,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2249,7 +2264,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="30" t="str">
+      <c r="A107" s="29" t="str">
         <f>'Stories 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2261,7 +2276,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2286,14 +2301,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="31"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="31" t="str">
+      <c r="A111" s="32" t="str">
         <f>'Stories 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2305,7 +2320,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2314,7 +2329,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="29"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2323,7 +2338,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="29"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2332,7 +2347,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2341,7 +2356,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="str">
+      <c r="A116" s="29" t="str">
         <f>'Stories 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2353,7 +2368,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="29"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2362,7 +2377,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="30" t="str">
+      <c r="A118" s="29" t="str">
         <f>'Stories 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2374,7 +2389,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2383,7 +2398,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="A120" s="29"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2392,7 +2407,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="str">
+      <c r="A121" s="29" t="str">
         <f>'Stories 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2404,7 +2419,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2413,7 +2428,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2422,7 +2437,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2431,7 +2446,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30" t="str">
+      <c r="A125" s="29" t="str">
         <f>'Stories 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2443,7 +2458,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2452,7 +2467,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2461,7 +2476,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30" t="str">
+      <c r="A128" s="29" t="str">
         <f>'Stories 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2473,7 +2488,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2482,7 +2497,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2491,7 +2506,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2500,7 +2515,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="str">
+      <c r="A132" s="29" t="str">
         <f>'Stories 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2512,7 +2527,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="29"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2521,7 +2536,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="30"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2534,14 +2549,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="29" t="s">
+      <c r="A135" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="29"/>
-      <c r="C135" s="29"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="35"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="28" t="str">
+      <c r="A136" s="31" t="str">
         <f>'Stories 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2553,7 +2568,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2562,7 +2577,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="28"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="9" t="s">
         <v>201</v>
       </c>
@@ -2571,7 +2586,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="28"/>
+      <c r="A139" s="31"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2580,7 +2595,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="28"/>
+      <c r="A140" s="31"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2589,7 +2604,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="28" t="str">
+      <c r="A141" s="31" t="str">
         <f>'Stories 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2601,7 +2616,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="28"/>
+      <c r="A142" s="31"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2610,7 +2625,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="28"/>
+      <c r="A143" s="31"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2619,7 +2634,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="28" t="str">
+      <c r="A144" s="31" t="str">
         <f>'Stories 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -2631,7 +2646,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="28"/>
+      <c r="A145" s="31"/>
       <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
@@ -2640,7 +2655,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="28"/>
+      <c r="A146" s="31"/>
       <c r="B146" s="9" t="s">
         <v>208</v>
       </c>
@@ -2649,7 +2664,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="28"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="9" t="s">
         <v>206</v>
       </c>
@@ -2658,7 +2673,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="28"/>
+      <c r="A148" s="31"/>
       <c r="B148" s="9" t="s">
         <v>209</v>
       </c>
@@ -2667,7 +2682,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="28"/>
+      <c r="A149" s="31"/>
       <c r="B149" s="9" t="s">
         <v>207</v>
       </c>
@@ -2676,7 +2691,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="28" t="str">
+      <c r="A150" s="31" t="str">
         <f>'Stories 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -2688,7 +2703,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="28"/>
+      <c r="A151" s="31"/>
       <c r="B151" s="24" t="s">
         <v>210</v>
       </c>
@@ -2697,67 +2712,113 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="28"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="16" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="28" t="str">
+      <c r="A153" s="31" t="str">
         <f>'Stories 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
       <c r="B153" s="9" t="s">
         <v>197</v>
       </c>
+      <c r="C153" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="28"/>
+      <c r="A154" s="31"/>
       <c r="B154" s="9" t="s">
         <v>198</v>
       </c>
+      <c r="C154" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="28"/>
+      <c r="A155" s="31"/>
       <c r="B155" s="9" t="s">
         <v>195</v>
       </c>
+      <c r="C155" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="28"/>
+      <c r="A156" s="31"/>
       <c r="B156" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="27" t="str">
+      <c r="C156" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="31"/>
+      <c r="B157" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C157" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="28" t="str">
         <f>'Stories 6'!A6</f>
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
-      <c r="B157" s="9" t="s">
+      <c r="B158" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D157">
-        <f>COUNTA(C136:C157)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="27"/>
+      <c r="C158" t="s">
+        <v>24</v>
+      </c>
+      <c r="D158">
+        <f>COUNTA(C136:C158)</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="27"/>
     </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2769,36 +2830,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A153:A156"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3152,9 +3191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3168,11 +3205,18 @@
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -3189,7 +3233,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3207,6 +3251,11 @@
         <v>203</v>
       </c>
     </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
     </row>

</xml_diff>

<commit_message>
The task list for iteration 7.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -8,21 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
-    <sheet name="Stories 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Stories 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Stories 3" sheetId="6" r:id="rId4"/>
-    <sheet name="Stories 4" sheetId="7" r:id="rId5"/>
-    <sheet name="Stories 5" sheetId="9" r:id="rId6"/>
-    <sheet name="Stories 6" sheetId="10" r:id="rId7"/>
-    <sheet name="Stories 7" sheetId="11" r:id="rId8"/>
-    <sheet name="Stories 8" sheetId="12" r:id="rId9"/>
+    <sheet name="S 1" sheetId="1" r:id="rId2"/>
+    <sheet name="S 2" sheetId="4" r:id="rId3"/>
+    <sheet name="S 3" sheetId="6" r:id="rId4"/>
+    <sheet name="S 4" sheetId="7" r:id="rId5"/>
+    <sheet name="S 5" sheetId="9" r:id="rId6"/>
+    <sheet name="S 6" sheetId="10" r:id="rId7"/>
+    <sheet name="S 7" sheetId="11" r:id="rId8"/>
+    <sheet name="S 8" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="251">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -670,6 +670,111 @@
   </si>
   <si>
     <t>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</t>
+  </si>
+  <si>
+    <t>Iteration 7</t>
+  </si>
+  <si>
+    <t>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</t>
+  </si>
+  <si>
+    <t>When I select a bauble to move it, it should move the whole bauble, with all attached track sections moving with it.  If a track section can't meet the bauble, the bauble transitions backwards to where all track sections can meet it.</t>
+  </si>
+  <si>
+    <t>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</t>
+  </si>
+  <si>
+    <t>Make all curve parameters private variables of Shape Controller</t>
+  </si>
+  <si>
+    <t>Rewrite rail vector function to calculate minimum angle etc</t>
+  </si>
+  <si>
+    <t>Rotate ends based on fixedness, then calculate params.</t>
+  </si>
+  <si>
+    <t>Call testable rail vector function from Curve() after params are calculated</t>
+  </si>
+  <si>
+    <t>Modify parameter calculations to put L1 = 0; A1 = 0 for straight track</t>
+  </si>
+  <si>
+    <t>Modify length and curve calculations to correctly handle L1 = 0</t>
+  </si>
+  <si>
+    <t>Baubles should notice when they've been moved and update all their attached track sections</t>
+  </si>
+  <si>
+    <t>SetEndPoint should be private and called from UpdateShape()</t>
+  </si>
+  <si>
+    <t>Track Sections should update their own shape when linked to a bauble.  Shape should be meaningless without a bauble at each end.</t>
+  </si>
+  <si>
+    <t>Make parameter calculations function called from ShapeController.Curve()</t>
+  </si>
+  <si>
+    <t>Create new Tool for placing train parts</t>
+  </si>
+  <si>
+    <t>Have minimum track length if ends are too close together.</t>
+  </si>
+  <si>
+    <t>CursorLight should snap to track.  Some indication of locomotive orientation should appear.  Arrow textured quad?</t>
+  </si>
+  <si>
+    <t>Update code where SetEndpoint or similar has been used.  Lighten track saveload data to contain only UID and bauble UIDs</t>
+  </si>
+  <si>
+    <t>Left-click on track to place locomotive in default orientation, left-click-drag to place locomotive oriented in drag direction. Directions must lock to rail directions.</t>
+  </si>
+  <si>
+    <t>Subtool should be locomotive.  Find a locomotive placeholder model.</t>
+  </si>
+  <si>
+    <t>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</t>
+  </si>
+  <si>
+    <t>Give LocomotiveController (see UML) a public float between 0 and 1.</t>
+  </si>
+  <si>
+    <t>Have Locomotive reference a track section and its progress along it.</t>
+  </si>
+  <si>
+    <t>Apply a force to locomotive based on power level.  Apply drag/friction force based on speed.</t>
+  </si>
+  <si>
+    <t>Lock locomotive to rail, re-orienting where necessary.</t>
+  </si>
+  <si>
+    <t>Locomotive should find next track section from bauble track link baubles.</t>
+  </si>
+  <si>
+    <t>Find Bezier curve equivalent of Euler spirals</t>
+  </si>
+  <si>
+    <t>Lock locomotive to bezier curves instead of rail vectors.</t>
+  </si>
+  <si>
+    <t>Download and install LeanTween.</t>
+  </si>
+  <si>
+    <t>Update FileHandler to accept Locomotives</t>
+  </si>
+  <si>
+    <t>Genericise Instantiate functions in FileHandler</t>
+  </si>
+  <si>
+    <t>Create SaveLoad and Data.  Data must have UID for track.</t>
+  </si>
+  <si>
+    <t>Update post-load linker to link locomotives to track.</t>
+  </si>
+  <si>
+    <t>Baubles should remember where they were before they moved, and revert to that position if any track section updates fail</t>
+  </si>
+  <si>
+    <t>Move length calculations to tssc after params, but before vert bending</t>
   </si>
 </sst>
 </file>
@@ -802,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -862,8 +967,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -871,25 +976,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -900,6 +996,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,10 +1304,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="615" topLeftCell="A159" activePane="bottomLeft"/>
+      <selection activeCell="A164" sqref="A164"/>
+      <selection pane="bottomLeft" activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,12 +1334,12 @@
       <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="str">
-        <f>'Stories 1'!A1</f>
+        <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1265,7 +1369,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="str">
-        <f>'Stories 1'!A2</f>
+        <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1322,7 +1426,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="str">
-        <f>'Stories 1'!A3</f>
+        <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1352,7 +1456,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="str">
-        <f>'Stories 1'!A4</f>
+        <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1391,7 +1495,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="str">
-        <f>'Stories 1'!A5</f>
+        <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1412,7 +1516,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="str">
-        <f>'Stories 1'!A6</f>
+        <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1423,7 +1527,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1436,15 +1540,15 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
-        <f>'Stories 2'!A1</f>
+        <f>'S 2'!A1</f>
         <v>I want a button on the toolbar for utilities.</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1456,7 +1560,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="str">
-        <f>'Stories 2'!A2</f>
+        <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -1477,7 +1581,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="str">
-        <f>'Stories 2'!A3</f>
+        <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -1543,7 +1647,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="str">
-        <f>'Stories 2'!A4</f>
+        <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -1582,7 +1686,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="str">
-        <f>'Stories 2'!A5</f>
+        <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -1603,7 +1707,7 @@
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="str">
-        <f>'Stories 2'!A6</f>
+        <f>'S 2'!A6</f>
         <v>The rotate camera function should take the pivot from the centre of the view, not from the mouse location.</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -1615,7 +1719,7 @@
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="str">
-        <f>'Stories 2'!A7</f>
+        <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -1654,7 +1758,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="str">
-        <f>'Stories 2'!A8</f>
+        <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -1675,7 +1779,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="str">
-        <f>'Stories 2'!A9</f>
+        <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
       <c r="B47" s="10" t="s">
@@ -1695,7 +1799,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1708,15 +1812,15 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="str">
-        <f>'Stories 3'!A1</f>
+        <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -1746,7 +1850,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="str">
-        <f>'Stories 3'!A2</f>
+        <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
       <c r="B54" s="10" t="s">
@@ -1767,7 +1871,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="str">
-        <f>'Stories 3'!A3</f>
+        <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
       <c r="B56" s="10" t="s">
@@ -1788,7 +1892,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="str">
-        <f>'Stories 3'!A4</f>
+        <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -1854,7 +1958,7 @@
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="str">
-        <f>'Stories 3'!A5</f>
+        <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
       <c r="B65" s="16" t="s">
@@ -1873,7 +1977,7 @@
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="str">
-        <f>'Stories 3'!A6</f>
+        <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -1894,7 +1998,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="str">
-        <f>'Stories 3'!A7</f>
+        <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -1929,7 +2033,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="str">
-        <f>'Stories 3'!A8</f>
+        <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -1950,7 +2054,7 @@
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="str">
-        <f>'Stories 3'!A9</f>
+        <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
       <c r="B75" s="19" t="s">
@@ -1970,7 +2074,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -1983,15 +2087,15 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="36"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="str">
-        <f>'Stories 4'!A1</f>
+        <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
       <c r="B79" s="9" t="s">
@@ -2012,7 +2116,7 @@
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="str">
-        <f>'Stories 4'!A2</f>
+        <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
       <c r="B81" s="9" t="s">
@@ -2033,7 +2137,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="str">
-        <f>'Stories 4'!A3</f>
+        <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
       <c r="B83" s="9" t="s">
@@ -2061,7 +2165,7 @@
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="str">
-        <f>'Stories 4'!A4</f>
+        <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
       <c r="B86" s="9" t="s">
@@ -2118,7 +2222,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="29" t="str">
-        <f>'Stories 4'!A5</f>
+        <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
       <c r="B92" s="9" t="s">
@@ -2157,7 +2261,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="str">
-        <f>'Stories 4'!A6</f>
+        <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
@@ -2187,7 +2291,7 @@
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="str">
-        <f>'Stories 4'!A7</f>
+        <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
       <c r="B99" s="9" t="s">
@@ -2235,7 +2339,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="str">
-        <f>'Stories 4'!A8</f>
+        <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
       <c r="B104" s="9" t="s">
@@ -2265,7 +2369,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="str">
-        <f>'Stories 4'!A9</f>
+        <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
       <c r="B107" s="9" t="s">
@@ -2286,7 +2390,7 @@
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="str">
-        <f>'Stories 4'!A10</f>
+        <f>'S 4'!A10</f>
         <v>I want curved sections of track to save and load properly.</v>
       </c>
       <c r="B109" s="22" t="s">
@@ -2301,15 +2405,15 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="31" t="s">
+      <c r="A110" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="31"/>
-      <c r="C110" s="31"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="str">
-        <f>'Stories 5'!A1</f>
+      <c r="A111" s="30" t="str">
+        <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
       <c r="B111" s="25" t="s">
@@ -2357,7 +2461,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="29" t="str">
-        <f>'Stories 5'!A2</f>
+        <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
       <c r="B116" s="9" t="s">
@@ -2378,7 +2482,7 @@
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="str">
-        <f>'Stories 5'!A3</f>
+        <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
       <c r="B118" s="9" t="s">
@@ -2408,7 +2512,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="str">
-        <f>'Stories 5'!A4</f>
+        <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
@@ -2447,7 +2551,7 @@
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="29" t="str">
-        <f>'Stories 5'!A5</f>
+        <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
@@ -2477,7 +2581,7 @@
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="str">
-        <f>'Stories 5'!A6</f>
+        <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
@@ -2516,7 +2620,7 @@
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="str">
-        <f>'Stories 5'!A7</f>
+        <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
@@ -2536,7 +2640,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="30"/>
+      <c r="A134" s="33"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2549,231 +2653,232 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="35" t="s">
+      <c r="A135" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="35"/>
-      <c r="C135" s="35"/>
+      <c r="B135" s="31"/>
+      <c r="C135" s="31"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="31" t="str">
-        <f>'Stories 6'!A1</f>
+      <c r="A136" s="30" t="str">
+        <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
-      <c r="B136" s="9" t="s">
+      <c r="B136" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C136" s="8" t="s">
+      <c r="C136" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
+      <c r="A137" s="29"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="C137" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
+      <c r="A138" s="29"/>
       <c r="B138" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C138" s="8" t="s">
+      <c r="C138" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="31"/>
+      <c r="A139" s="29"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C139" s="8" t="s">
+      <c r="C139" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="31"/>
+      <c r="A140" s="29"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C140" s="8" t="s">
+      <c r="C140" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="31" t="str">
-        <f>'Stories 6'!A2</f>
+      <c r="A141" s="29" t="str">
+        <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
       <c r="B141" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C141" s="8" t="s">
+      <c r="C141" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="31"/>
+      <c r="A142" s="29"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C142" s="8" t="s">
+      <c r="C142" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="31"/>
+      <c r="A143" s="29"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C143" s="8" t="s">
+      <c r="C143" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="31" t="str">
-        <f>'Stories 6'!A3</f>
+      <c r="A144" s="29" t="str">
+        <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C144" s="8" t="s">
+      <c r="C144" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="31"/>
+      <c r="A145" s="29"/>
       <c r="B145" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="31"/>
+      <c r="A146" s="29"/>
       <c r="B146" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="31"/>
+      <c r="A147" s="29"/>
       <c r="B147" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="31"/>
+      <c r="A148" s="29"/>
       <c r="B148" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="31"/>
+      <c r="A149" s="29"/>
       <c r="B149" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="31" t="str">
-        <f>'Stories 6'!A4</f>
+      <c r="A150" s="29" t="str">
+        <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
       <c r="B150" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="31"/>
+      <c r="A151" s="29"/>
       <c r="B151" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="31"/>
+      <c r="A152" s="29"/>
       <c r="B152" s="16" t="s">
         <v>193</v>
       </c>
+      <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="31" t="str">
-        <f>'Stories 6'!A5</f>
+      <c r="A153" s="29" t="str">
+        <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
       <c r="B153" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="31"/>
+      <c r="A154" s="29"/>
       <c r="B154" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="31"/>
+      <c r="A155" s="29"/>
       <c r="B155" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="31"/>
+      <c r="A156" s="29"/>
       <c r="B156" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="31"/>
+      <c r="A157" s="29"/>
       <c r="B157" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="28" t="str">
-        <f>'Stories 6'!A6</f>
+      <c r="A158" s="27" t="str">
+        <f>'S 6'!A6</f>
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
-      <c r="B158" s="9" t="s">
+      <c r="B158" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D158">
@@ -2782,43 +2887,230 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="27"/>
+      <c r="A159" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="B159" s="31"/>
+      <c r="C159" s="31"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="27"/>
+      <c r="A160" s="28" t="str">
+        <f>'S 7'!A1</f>
+        <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="28"/>
+      <c r="B161" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="28"/>
+      <c r="B162" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="28"/>
+      <c r="B163" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="28"/>
+      <c r="B164" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="28" t="str">
+        <f>'S 7'!A2</f>
+        <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="28"/>
+      <c r="B166" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="28"/>
+      <c r="B167" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="28"/>
+      <c r="B168" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="28" t="str">
+        <f>'S 7'!A3</f>
+        <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="28"/>
+      <c r="B170" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="28"/>
+      <c r="B171" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="28"/>
+      <c r="B172" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="28"/>
+      <c r="B173" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="28" t="str">
+        <f>'S 7'!A4</f>
+        <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
+      </c>
+      <c r="B174" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="28"/>
+      <c r="B175" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="28"/>
+      <c r="B176" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A177" s="28"/>
+      <c r="B177" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="28" t="str">
+        <f>'S 7'!A5</f>
+        <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="28"/>
+      <c r="B179" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="28"/>
+      <c r="B180" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="28"/>
+      <c r="B181" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="28"/>
+      <c r="B182" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="28" t="str">
+        <f>'S 7'!A6</f>
+        <v>I want trains moving along the track to do so smoothly (Bezier curves and LeanTween)</v>
+      </c>
+      <c r="B183" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="28"/>
+      <c r="B184" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="28"/>
+      <c r="B185" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="28" t="str">
+        <f>'S 7'!A7</f>
+        <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="28"/>
+      <c r="B187" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="28"/>
+      <c r="B188" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="28"/>
+      <c r="B189" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D189">
+        <f>COUNTA(C160:C189)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="A150:A152"/>
+  <mergeCells count="57">
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
     <mergeCell ref="A153:A157"/>
     <mergeCell ref="A135:C135"/>
     <mergeCell ref="A136:A140"/>
     <mergeCell ref="A141:A143"/>
     <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:A26"/>
@@ -2830,14 +3122,41 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A160:A164"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A159:C159"/>
     <mergeCell ref="A132:A134"/>
     <mergeCell ref="A121:A124"/>
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A150:A152"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3023,7 +3342,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3189,9 +3508,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3218,9 +3539,19 @@
         <v>200</v>
       </c>
     </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3230,10 +3561,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3257,7 +3588,14 @@
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Track section shape parameters refactored, and rail vector list rewritten to be more evenly spread.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="251">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -705,9 +705,6 @@
     <t>Baubles should notice when they've been moved and update all their attached track sections</t>
   </si>
   <si>
-    <t>SetEndPoint should be private and called from UpdateShape()</t>
-  </si>
-  <si>
     <t>Track Sections should update their own shape when linked to a bauble.  Shape should be meaningless without a bauble at each end.</t>
   </si>
   <si>
@@ -735,9 +732,6 @@
     <t>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</t>
   </si>
   <si>
-    <t>Give LocomotiveController (see UML) a public float between 0 and 1.</t>
-  </si>
-  <si>
     <t>Have Locomotive reference a track section and its progress along it.</t>
   </si>
   <si>
@@ -775,6 +769,12 @@
   </si>
   <si>
     <t>Move length calculations to tssc after params, but before vert bending</t>
+  </si>
+  <si>
+    <t>Curve, SetEndPoint should be private, SetEndPoint called from UpdateShape</t>
+  </si>
+  <si>
+    <t>Give LocomotiveController (see UML) a public float between -1 and 1.</t>
   </si>
 </sst>
 </file>
@@ -982,10 +982,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1309,7 +1309,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A159" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="B163" sqref="B163"/>
+      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1527,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
+      <c r="C23" s="33"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>106</v>
       </c>
       <c r="B78" s="31"/>
-      <c r="C78" s="32"/>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="str">
@@ -2640,7 +2640,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2901,32 +2901,47 @@
       <c r="B160" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="28"/>
       <c r="B161" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="28"/>
       <c r="B162" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="28"/>
       <c r="B163" s="9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="28"/>
       <c r="B164" s="9" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C164" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="28" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
@@ -2935,82 +2950,82 @@
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="28"/>
       <c r="B166" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="28"/>
       <c r="B167" s="9" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="28"/>
       <c r="B168" s="9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="28" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="28"/>
       <c r="B170" s="9" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="28"/>
       <c r="B171" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="28"/>
       <c r="B172" s="9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="28"/>
       <c r="B173" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="28" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="28"/>
       <c r="B175" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="28"/>
       <c r="B176" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="28"/>
       <c r="B177" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3019,31 +3034,31 @@
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="28"/>
       <c r="B179" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="28"/>
       <c r="B180" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="28"/>
       <c r="B181" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="28"/>
       <c r="B182" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3052,19 +3067,19 @@
         <v>I want trains moving along the track to do so smoothly (Bezier curves and LeanTween)</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="28"/>
       <c r="B184" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="28"/>
       <c r="B185" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3073,29 +3088,29 @@
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="28"/>
       <c r="B187" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="28"/>
       <c r="B188" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="28"/>
       <c r="B189" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D189">
         <f>COUNTA(C160:C189)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3551,7 +3566,7 @@
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bauble-track section relationship has been refactored and neatened.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="251">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1307,9 +1307,9 @@
   <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A159" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A165" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
+      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,24 +2949,36 @@
       <c r="B165" s="9" t="s">
         <v>222</v>
       </c>
+      <c r="C165" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="28"/>
       <c r="B166" s="9" t="s">
         <v>230</v>
       </c>
+      <c r="C166" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="28"/>
       <c r="B167" s="9" t="s">
         <v>224</v>
       </c>
+      <c r="C167" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="28"/>
       <c r="B168" s="9" t="s">
         <v>225</v>
       </c>
+      <c r="C168" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="28" t="str">
@@ -2976,16 +2988,22 @@
       <c r="B169" s="9" t="s">
         <v>227</v>
       </c>
+      <c r="C169" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="28"/>
       <c r="B170" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="C170" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="28"/>
-      <c r="B171" s="9" t="s">
+      <c r="B171" s="16" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2994,12 +3012,18 @@
       <c r="B172" s="9" t="s">
         <v>249</v>
       </c>
+      <c r="C172" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="28"/>
       <c r="B173" s="9" t="s">
         <v>232</v>
       </c>
+      <c r="C173" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="28" t="str">
@@ -3110,7 +3134,7 @@
       </c>
       <c r="D189">
         <f>COUNTA(C160:C189)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Locomotive can now be placed in the world.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="251">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -976,16 +976,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,12 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,9 +1307,9 @@
   <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A165" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A168" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
+      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,8 +1334,8 @@
       <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="str">
@@ -1527,7 +1527,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1540,11 +1540,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="33"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="34"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1812,11 +1812,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="str">
@@ -2074,7 +2074,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2087,11 +2087,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="33"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="34"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="str">
@@ -2412,7 +2412,7 @@
       <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="str">
+      <c r="A111" s="31" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2640,7 +2640,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2653,14 +2653,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="31" t="s">
+      <c r="A135" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="31"/>
-      <c r="C135" s="31"/>
+      <c r="B135" s="30"/>
+      <c r="C135" s="30"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="31" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2887,11 +2887,11 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="31" t="s">
+      <c r="A159" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="B159" s="31"/>
-      <c r="C159" s="31"/>
+      <c r="B159" s="30"/>
+      <c r="C159" s="30"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="28" t="str">
@@ -3033,24 +3033,36 @@
       <c r="B174" s="9" t="s">
         <v>229</v>
       </c>
+      <c r="C174" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="28"/>
       <c r="B175" s="9" t="s">
         <v>234</v>
       </c>
+      <c r="C175" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="28"/>
       <c r="B176" s="9" t="s">
         <v>231</v>
       </c>
+      <c r="C176" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="28"/>
       <c r="B177" s="9" t="s">
         <v>233</v>
       </c>
+      <c r="C177" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="28" t="str">
@@ -3134,52 +3146,11 @@
       </c>
       <c r="D189">
         <f>COUNTA(C160:C189)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3196,6 +3167,47 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Locomotive will move along the track according to its power setting.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="250">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -606,9 +606,6 @@
     <t>Rewrite crease placement algorithm to accommodate compound curves</t>
   </si>
   <si>
-    <t>I want trains moving along the track to do so smoothly (Bezier curves and LeanTween)</t>
-  </si>
-  <si>
     <t>Extant track section should split in half attaching each half to the new bauble</t>
   </si>
   <si>
@@ -732,9 +729,6 @@
     <t>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</t>
   </si>
   <si>
-    <t>Have Locomotive reference a track section and its progress along it.</t>
-  </si>
-  <si>
     <t>Apply a force to locomotive based on power level.  Apply drag/friction force based on speed.</t>
   </si>
   <si>
@@ -744,15 +738,6 @@
     <t>Locomotive should find next track section from bauble track link baubles.</t>
   </si>
   <si>
-    <t>Find Bezier curve equivalent of Euler spirals</t>
-  </si>
-  <si>
-    <t>Lock locomotive to bezier curves instead of rail vectors.</t>
-  </si>
-  <si>
-    <t>Download and install LeanTween.</t>
-  </si>
-  <si>
     <t>Update FileHandler to accept Locomotives</t>
   </si>
   <si>
@@ -775,6 +760,18 @@
   </si>
   <si>
     <t>Give LocomotiveController (see UML) a public float between -1 and 1.</t>
+  </si>
+  <si>
+    <t>Have TrackVehicle reference a track section</t>
+  </si>
+  <si>
+    <t>I want to be able to create large curved sections without the rails bugging out.</t>
+  </si>
+  <si>
+    <t>I want trains moving along the track to do so smoothly</t>
+  </si>
+  <si>
+    <t>Function for position and direction along track should use Euler curve params</t>
   </si>
 </sst>
 </file>
@@ -907,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -976,22 +973,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1002,6 +993,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,9 +1307,9 @@
   <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A168" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A160" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
+      <selection pane="bottomLeft" activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,8 +1334,8 @@
       <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="str">
@@ -1527,7 +1527,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1540,11 +1540,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="33"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1812,11 +1812,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="str">
@@ -2074,7 +2074,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="35"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2087,11 +2087,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="30"/>
-      <c r="C78" s="34"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="str">
@@ -2412,7 +2412,7 @@
       <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="31" t="str">
+      <c r="A111" s="30" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2640,7 +2640,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="35"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2653,14 +2653,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="30" t="s">
+      <c r="A135" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="30"/>
-      <c r="C135" s="30"/>
+      <c r="B135" s="31"/>
+      <c r="C135" s="31"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="31" t="str">
+      <c r="A136" s="30" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2683,7 +2683,7 @@
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
       <c r="B138" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>24</v>
@@ -2743,7 +2743,7 @@
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>24</v>
@@ -2752,7 +2752,7 @@
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
       <c r="B145" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>24</v>
@@ -2761,7 +2761,7 @@
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="29"/>
       <c r="B146" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>24</v>
@@ -2770,7 +2770,7 @@
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
       <c r="B147" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>24</v>
@@ -2779,7 +2779,7 @@
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
       <c r="B148" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>24</v>
@@ -2788,7 +2788,7 @@
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
       <c r="B149" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>24</v>
@@ -2809,7 +2809,7 @@
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
       <c r="B151" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>24</v>
@@ -2828,7 +2828,7 @@
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>24</v>
@@ -2837,7 +2837,7 @@
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="29"/>
       <c r="B154" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>24</v>
@@ -2846,7 +2846,7 @@
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="29"/>
       <c r="B155" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>24</v>
@@ -2855,7 +2855,7 @@
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="29"/>
       <c r="B156" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>24</v>
@@ -2864,7 +2864,7 @@
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
       <c r="B157" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>24</v>
@@ -2876,7 +2876,7 @@
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>24</v>
@@ -2887,11 +2887,11 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="B159" s="30"/>
-      <c r="C159" s="30"/>
+      <c r="A159" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B159" s="31"/>
+      <c r="C159" s="31"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="28" t="str">
@@ -2899,7 +2899,7 @@
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>24</v>
@@ -2908,7 +2908,7 @@
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="28"/>
       <c r="B161" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>24</v>
@@ -2917,7 +2917,7 @@
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="28"/>
       <c r="B162" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>24</v>
@@ -2926,7 +2926,7 @@
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="28"/>
       <c r="B163" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C163" s="8" t="s">
         <v>24</v>
@@ -2935,7 +2935,7 @@
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="28"/>
       <c r="B164" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C164" s="8" t="s">
         <v>24</v>
@@ -2947,7 +2947,7 @@
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C165" s="8" t="s">
         <v>24</v>
@@ -2956,7 +2956,7 @@
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="28"/>
       <c r="B166" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>24</v>
@@ -2965,7 +2965,7 @@
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="28"/>
       <c r="B167" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C167" s="8" t="s">
         <v>24</v>
@@ -2974,7 +2974,7 @@
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="28"/>
       <c r="B168" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C168" s="8" t="s">
         <v>24</v>
@@ -2986,7 +2986,7 @@
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C169" s="8" t="s">
         <v>24</v>
@@ -2995,7 +2995,7 @@
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="28"/>
       <c r="B170" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>24</v>
@@ -3004,13 +3004,13 @@
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="28"/>
       <c r="B171" s="16" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="28"/>
       <c r="B172" s="9" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C172" t="s">
         <v>24</v>
@@ -3019,7 +3019,7 @@
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="28"/>
       <c r="B173" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C173" t="s">
         <v>24</v>
@@ -3031,7 +3031,7 @@
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C174" t="s">
         <v>24</v>
@@ -3040,7 +3040,7 @@
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="28"/>
       <c r="B175" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C175" t="s">
         <v>24</v>
@@ -3049,7 +3049,7 @@
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="28"/>
       <c r="B176" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C176" t="s">
         <v>24</v>
@@ -3058,7 +3058,7 @@
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="28"/>
       <c r="B177" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C177" t="s">
         <v>24</v>
@@ -3070,87 +3070,136 @@
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>250</v>
+        <v>245</v>
+      </c>
+      <c r="C178" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="28"/>
       <c r="B179" s="9" t="s">
-        <v>236</v>
+        <v>246</v>
+      </c>
+      <c r="C179" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="28"/>
       <c r="B180" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="C180" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="28"/>
       <c r="B181" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
+      </c>
+      <c r="C181" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="28"/>
       <c r="B182" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
+      </c>
+      <c r="C182" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="28" t="str">
+      <c r="A183" s="39" t="str">
         <f>'S 7'!A6</f>
-        <v>I want trains moving along the track to do so smoothly (Bezier curves and LeanTween)</v>
+        <v>I want trains moving along the track to do so smoothly</v>
       </c>
       <c r="B183" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="28" t="str">
+        <f>'S 7'!A7</f>
+        <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
+      </c>
+      <c r="B184" s="9" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="28"/>
-      <c r="B184" s="9" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="28"/>
       <c r="B185" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="28"/>
+      <c r="B186" s="9" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="28" t="str">
-        <f>'S 7'!A7</f>
-        <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
-      </c>
-      <c r="B186" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="28"/>
       <c r="B187" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
+      </c>
+      <c r="D187">
+        <f>COUNTA(C160:C187)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="28"/>
-      <c r="B188" s="9" t="s">
-        <v>246</v>
-      </c>
+      <c r="A188" s="39"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="28"/>
-      <c r="B189" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D189">
-        <f>COUNTA(C160:C189)</f>
-        <v>17</v>
-      </c>
+      <c r="A189" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="56">
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A184:A187"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3167,47 +3216,6 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3562,7 +3570,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3572,37 +3580,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3612,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3625,27 +3633,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trains movement and placement will now position the vehicle smoothly on the curve using the Euler Spiral parameters.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="252">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -771,7 +771,13 @@
     <t>I want trains moving along the track to do so smoothly</t>
   </si>
   <si>
-    <t>Function for position and direction along track should use Euler curve params</t>
+    <t>function for position and direction along track should use Euler curve params</t>
+  </si>
+  <si>
+    <t>FindTrackCentre should use Euler curve params</t>
+  </si>
+  <si>
+    <t>GetTravelDistance should use Euler curve params</t>
   </si>
 </sst>
 </file>
@@ -968,21 +974,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,15 +1008,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1304,12 +1310,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D189"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A160" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A175" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C183" sqref="C183"/>
+      <selection pane="bottomLeft" activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,14 +1337,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="str">
+      <c r="A3" s="30" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1350,7 +1356,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1359,7 +1365,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1368,7 +1374,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="str">
+      <c r="A6" s="30" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1380,7 +1386,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1395,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1398,7 +1404,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1407,7 +1413,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1416,7 +1422,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1425,7 +1431,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="str">
+      <c r="A12" s="30" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1437,7 +1443,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1446,7 +1452,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1455,7 +1461,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="str">
+      <c r="A15" s="30" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1467,7 +1473,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1476,7 +1482,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1485,7 +1491,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1494,7 +1500,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="str">
+      <c r="A19" s="30" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1506,7 +1512,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1515,7 +1521,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="str">
+      <c r="A21" s="30" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1527,7 +1533,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1540,11 +1546,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="32" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="31"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1559,7 +1565,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="str">
+      <c r="A25" s="30" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1571,7 +1577,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1580,7 +1586,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="str">
+      <c r="A27" s="30" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1592,7 +1598,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1601,7 +1607,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1610,7 +1616,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1619,7 +1625,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1628,7 +1634,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1637,7 +1643,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1646,7 +1652,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="str">
+      <c r="A34" s="30" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1658,7 +1664,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1667,7 +1673,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1676,7 +1682,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1685,7 +1691,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="str">
+      <c r="A38" s="30" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1697,7 +1703,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1718,7 +1724,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="str">
+      <c r="A41" s="30" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1730,7 +1736,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1739,7 +1745,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1754,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1757,7 +1763,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="str">
+      <c r="A45" s="30" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1769,7 +1775,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1778,7 +1784,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="str">
+      <c r="A47" s="30" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1790,7 +1796,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1799,7 +1805,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="36"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1812,14 +1818,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="str">
+      <c r="A51" s="30" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1831,7 +1837,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1840,7 +1846,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1849,7 +1855,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="str">
+      <c r="A54" s="30" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1861,7 +1867,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1870,7 +1876,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="str">
+      <c r="A56" s="30" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1882,7 +1888,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1891,7 +1897,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="str">
+      <c r="A58" s="30" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1903,7 +1909,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1912,7 +1918,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1921,7 +1927,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1930,7 +1936,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -1939,7 +1945,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -1948,7 +1954,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -1957,7 +1963,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="str">
+      <c r="A65" s="30" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -1967,7 +1973,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -1976,7 +1982,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="str">
+      <c r="A67" s="30" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -1988,7 +1994,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -1997,7 +2003,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="29" t="str">
+      <c r="A69" s="30" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2009,21 +2015,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -2032,7 +2038,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="str">
+      <c r="A73" s="30" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2044,7 +2050,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -2053,7 +2059,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="29" t="str">
+      <c r="A75" s="30" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2065,7 +2071,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -2074,7 +2080,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="36"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2087,14 +2093,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="32" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="31"/>
-      <c r="C78" s="33"/>
+      <c r="C78" s="35"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="str">
+      <c r="A79" s="30" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2106,7 +2112,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -2115,7 +2121,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="29" t="str">
+      <c r="A81" s="30" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2127,7 +2133,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2136,7 +2142,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="29" t="str">
+      <c r="A83" s="30" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2148,7 +2154,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2157,14 +2163,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29" t="str">
+      <c r="A86" s="30" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2176,7 +2182,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2185,7 +2191,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2194,7 +2200,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2203,7 +2209,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2212,7 +2218,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2221,7 +2227,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="29" t="str">
+      <c r="A92" s="30" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2233,7 +2239,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2242,7 +2248,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2251,7 +2257,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2260,7 +2266,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="29" t="str">
+      <c r="A96" s="30" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2272,7 +2278,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2281,7 +2287,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2290,7 +2296,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="29" t="str">
+      <c r="A99" s="30" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2302,7 +2308,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2311,7 +2317,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2320,7 +2326,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2329,7 +2335,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2338,7 +2344,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="29" t="str">
+      <c r="A104" s="30" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2350,7 +2356,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2359,7 +2365,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2368,7 +2374,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="29" t="str">
+      <c r="A107" s="30" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2380,7 +2386,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="29"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2405,14 +2411,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="str">
+      <c r="A111" s="32" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2424,7 +2430,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2433,7 +2439,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="29"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2442,7 +2448,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="29"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2451,7 +2457,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="29"/>
+      <c r="A115" s="30"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2460,7 +2466,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="29" t="str">
+      <c r="A116" s="30" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2472,7 +2478,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
+      <c r="A117" s="30"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2481,7 +2487,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="29" t="str">
+      <c r="A118" s="30" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2493,7 +2499,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
+      <c r="A119" s="30"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2502,7 +2508,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="29"/>
+      <c r="A120" s="30"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2511,7 +2517,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="29" t="str">
+      <c r="A121" s="30" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2523,7 +2529,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2532,7 +2538,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2541,7 +2547,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2550,7 +2556,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="29" t="str">
+      <c r="A125" s="30" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2562,7 +2568,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2571,7 +2577,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2580,7 +2586,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="29" t="str">
+      <c r="A128" s="30" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2592,7 +2598,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
+      <c r="A129" s="30"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2601,7 +2607,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="30"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2610,7 +2616,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="29"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2619,7 +2625,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="29" t="str">
+      <c r="A132" s="30" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2631,7 +2637,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
+      <c r="A133" s="30"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2640,7 +2646,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="36"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2660,7 +2666,7 @@
       <c r="C135" s="31"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="32" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2672,7 +2678,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="29"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2681,7 +2687,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
+      <c r="A138" s="30"/>
       <c r="B138" s="9" t="s">
         <v>200</v>
       </c>
@@ -2690,7 +2696,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="29"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2699,7 +2705,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
+      <c r="A140" s="30"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2708,7 +2714,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="29" t="str">
+      <c r="A141" s="30" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2720,7 +2726,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2729,7 +2735,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="29"/>
+      <c r="A143" s="30"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2738,7 +2744,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="29" t="str">
+      <c r="A144" s="30" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -2750,7 +2756,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="29"/>
+      <c r="A145" s="30"/>
       <c r="B145" s="9" t="s">
         <v>204</v>
       </c>
@@ -2759,7 +2765,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="29"/>
+      <c r="A146" s="30"/>
       <c r="B146" s="9" t="s">
         <v>207</v>
       </c>
@@ -2768,7 +2774,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="29"/>
+      <c r="A147" s="30"/>
       <c r="B147" s="9" t="s">
         <v>205</v>
       </c>
@@ -2777,7 +2783,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="29"/>
+      <c r="A148" s="30"/>
       <c r="B148" s="9" t="s">
         <v>208</v>
       </c>
@@ -2786,7 +2792,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="29"/>
+      <c r="A149" s="30"/>
       <c r="B149" s="9" t="s">
         <v>206</v>
       </c>
@@ -2795,7 +2801,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="29" t="str">
+      <c r="A150" s="30" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -2807,7 +2813,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="29"/>
+      <c r="A151" s="30"/>
       <c r="B151" s="24" t="s">
         <v>209</v>
       </c>
@@ -2816,14 +2822,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="29"/>
+      <c r="A152" s="30"/>
       <c r="B152" s="16" t="s">
         <v>193</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="29" t="str">
+      <c r="A153" s="30" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -2835,7 +2841,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="29"/>
+      <c r="A154" s="30"/>
       <c r="B154" s="9" t="s">
         <v>197</v>
       </c>
@@ -2844,7 +2850,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="29"/>
+      <c r="A155" s="30"/>
       <c r="B155" s="9" t="s">
         <v>194</v>
       </c>
@@ -2853,7 +2859,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="29"/>
+      <c r="A156" s="30"/>
       <c r="B156" s="9" t="s">
         <v>195</v>
       </c>
@@ -2862,7 +2868,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="29"/>
+      <c r="A157" s="30"/>
       <c r="B157" s="9" t="s">
         <v>212</v>
       </c>
@@ -2894,7 +2900,7 @@
       <c r="C159" s="31"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="28" t="str">
+      <c r="A160" s="29" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -2906,7 +2912,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="28"/>
+      <c r="A161" s="29"/>
       <c r="B161" s="9" t="s">
         <v>227</v>
       </c>
@@ -2915,7 +2921,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="28"/>
+      <c r="A162" s="29"/>
       <c r="B162" s="9" t="s">
         <v>243</v>
       </c>
@@ -2924,7 +2930,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="28"/>
+      <c r="A163" s="29"/>
       <c r="B163" s="9" t="s">
         <v>222</v>
       </c>
@@ -2933,7 +2939,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="28"/>
+      <c r="A164" s="29"/>
       <c r="B164" s="9" t="s">
         <v>220</v>
       </c>
@@ -2942,7 +2948,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="28" t="str">
+      <c r="A165" s="29" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -2954,7 +2960,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="28"/>
+      <c r="A166" s="29"/>
       <c r="B166" s="9" t="s">
         <v>229</v>
       </c>
@@ -2963,7 +2969,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="28"/>
+      <c r="A167" s="29"/>
       <c r="B167" s="9" t="s">
         <v>223</v>
       </c>
@@ -2972,7 +2978,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="28"/>
+      <c r="A168" s="29"/>
       <c r="B168" s="9" t="s">
         <v>224</v>
       </c>
@@ -2981,7 +2987,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="28" t="str">
+      <c r="A169" s="29" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -2993,7 +2999,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="28"/>
+      <c r="A170" s="29"/>
       <c r="B170" s="9" t="s">
         <v>225</v>
       </c>
@@ -3002,13 +3008,13 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="28"/>
+      <c r="A171" s="29"/>
       <c r="B171" s="16" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="28"/>
+      <c r="A172" s="29"/>
       <c r="B172" s="9" t="s">
         <v>244</v>
       </c>
@@ -3017,7 +3023,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="28"/>
+      <c r="A173" s="29"/>
       <c r="B173" s="9" t="s">
         <v>231</v>
       </c>
@@ -3026,7 +3032,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="28" t="str">
+      <c r="A174" s="29" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3038,7 +3044,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="28"/>
+      <c r="A175" s="29"/>
       <c r="B175" s="9" t="s">
         <v>233</v>
       </c>
@@ -3047,7 +3053,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="28"/>
+      <c r="A176" s="29"/>
       <c r="B176" s="9" t="s">
         <v>230</v>
       </c>
@@ -3056,7 +3062,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="28"/>
+      <c r="A177" s="29"/>
       <c r="B177" s="9" t="s">
         <v>232</v>
       </c>
@@ -3065,7 +3071,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="28" t="str">
+      <c r="A178" s="29" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3077,7 +3083,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="28"/>
+      <c r="A179" s="29"/>
       <c r="B179" s="9" t="s">
         <v>246</v>
       </c>
@@ -3086,7 +3092,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="28"/>
+      <c r="A180" s="29"/>
       <c r="B180" s="9" t="s">
         <v>235</v>
       </c>
@@ -3095,7 +3101,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="28"/>
+      <c r="A181" s="29"/>
       <c r="B181" s="9" t="s">
         <v>236</v>
       </c>
@@ -3104,7 +3110,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="28"/>
+      <c r="A182" s="29"/>
       <c r="B182" s="9" t="s">
         <v>237</v>
       </c>
@@ -3112,94 +3118,75 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="39" t="str">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="29" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
       <c r="B183" s="9" t="s">
         <v>249</v>
       </c>
+      <c r="C183" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="28" t="str">
+      <c r="A184" s="29"/>
+      <c r="B184" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C184" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="29"/>
+      <c r="B185" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C185" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="29" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
-      <c r="B184" s="9" t="s">
+      <c r="B186" s="9" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="28"/>
-      <c r="B185" s="9" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="29"/>
+      <c r="B187" s="9" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="28"/>
-      <c r="B186" s="9" t="s">
+    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="29"/>
+      <c r="B188" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="28"/>
-      <c r="B187" s="9" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="29"/>
+      <c r="B189" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="D187">
-        <f>COUNTA(C160:C187)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="39"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="39"/>
+      <c r="D189">
+        <f>COUNTA(C160:C189)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="28"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A184:A187"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
+  <mergeCells count="57">
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3216,6 +3203,47 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Locomotive info is saved and loaded, and saving and loading refactored slightly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="253">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -778,6 +778,9 @@
   </si>
   <si>
     <t>GetTravelDistance should use Euler curve params</t>
+  </si>
+  <si>
+    <t>I want a way to remove a locomotive from the track.</t>
   </si>
 </sst>
 </file>
@@ -1313,9 +1316,9 @@
   <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A175" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A166" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C186" sqref="C186"/>
+      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,27 +3159,39 @@
       <c r="B186" s="9" t="s">
         <v>240</v>
       </c>
+      <c r="C186" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="29"/>
       <c r="B187" s="9" t="s">
         <v>238</v>
       </c>
+      <c r="C187" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="29"/>
       <c r="B188" s="9" t="s">
         <v>241</v>
       </c>
+      <c r="C188" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="29"/>
       <c r="B189" s="9" t="s">
         <v>239</v>
       </c>
+      <c r="C189" t="s">
+        <v>24</v>
+      </c>
       <c r="D189">
         <f>COUNTA(C160:C189)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,11 +3663,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3666,26 +3679,31 @@
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor fixes and task list for Iteration 8
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -16,13 +16,14 @@
     <sheet name="S 6" sheetId="10" r:id="rId7"/>
     <sheet name="S 7" sheetId="11" r:id="rId8"/>
     <sheet name="S 8" sheetId="12" r:id="rId9"/>
+    <sheet name="S 9" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="272">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -765,9 +766,6 @@
     <t>Have TrackVehicle reference a track section</t>
   </si>
   <si>
-    <t>I want to be able to create large curved sections without the rails bugging out.</t>
-  </si>
-  <si>
     <t>I want trains moving along the track to do so smoothly</t>
   </si>
   <si>
@@ -780,7 +778,67 @@
     <t>GetTravelDistance should use Euler curve params</t>
   </si>
   <si>
-    <t>I want a way to remove a locomotive from the track.</t>
+    <t>Iteration 8</t>
+  </si>
+  <si>
+    <t>If a track vehicle runs off the end of the track, it should derail properly.</t>
+  </si>
+  <si>
+    <t>I want a way to remove a locomotive from the world.</t>
+  </si>
+  <si>
+    <t>Fix that bug</t>
+  </si>
+  <si>
+    <t>I want to be able to create large curved sections without the colliders bugging out.</t>
+  </si>
+  <si>
+    <t>Add right-click to TrainPlacementTool to delete vehicle under cursor</t>
+  </si>
+  <si>
+    <t>Bauble needs radius property for Track Shaper to use during update.</t>
+  </si>
+  <si>
+    <t>Key presses while moving bauble changes radius. Default = inf.</t>
+  </si>
+  <si>
+    <t>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</t>
+  </si>
+  <si>
+    <t>Allow for exceptional case where a bauble is right on the apex</t>
+  </si>
+  <si>
+    <t>Find equation for projecting endpoint if a given location has given curvature</t>
+  </si>
+  <si>
+    <t>Make track section bend to curved end bauble</t>
+  </si>
+  <si>
+    <t>Make track section bend to curved start bauble.</t>
+  </si>
+  <si>
+    <t>Remove condition for the track to be straight before splitting it</t>
+  </si>
+  <si>
+    <t>On a curved section, the created bauble must have correct curvature.</t>
+  </si>
+  <si>
+    <t>Fix remaining issues from straight section implementation if any</t>
+  </si>
+  <si>
+    <t>Calculate correct position for the bauble to be in based on radius of bauble at other end.</t>
+  </si>
+  <si>
+    <t>Lock bauble's curvature to that of other bauble.</t>
+  </si>
+  <si>
+    <t>Correctly handle fixed radius curves.  Transition params will be irrelevant.</t>
+  </si>
+  <si>
+    <t>Ensure physics engine works properly.  Reduce friction for cooler crash.</t>
+  </si>
+  <si>
+    <t>Fix rigidbody velocity and stop traversing if trackSection becomes null</t>
   </si>
 </sst>
 </file>
@@ -985,22 +1043,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1011,6 +1063,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1313,18 +1371,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A166" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A184" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
+      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="2" max="2" width="71.28515625" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1343,8 +1401,8 @@
       <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="str">
@@ -1536,7 +1594,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1549,11 +1607,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="35"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="34"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1808,7 +1866,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1821,11 +1879,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="str">
@@ -2083,7 +2141,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="36"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2096,11 +2154,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="35"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="34"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="str">
@@ -2421,7 +2479,7 @@
       <c r="C110" s="29"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="str">
+      <c r="A111" s="31" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2649,7 +2707,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="36"/>
+      <c r="A134" s="33"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2662,14 +2720,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="31" t="s">
+      <c r="A135" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="31"/>
-      <c r="C135" s="31"/>
+      <c r="B135" s="32"/>
+      <c r="C135" s="32"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="32" t="str">
+      <c r="A136" s="31" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2896,297 +2954,298 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="31" t="s">
+      <c r="A159" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="B159" s="31"/>
-      <c r="C159" s="31"/>
+      <c r="B159" s="32"/>
+      <c r="C159" s="32"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="29" t="str">
+      <c r="A160" s="31" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
-      <c r="B160" s="9" t="s">
+      <c r="B160" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="C160" s="8" t="s">
+      <c r="C160" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="29"/>
+      <c r="A161" s="30"/>
       <c r="B161" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C161" s="8" t="s">
+      <c r="C161" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="29"/>
+      <c r="A162" s="30"/>
       <c r="B162" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C162" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="29"/>
+      <c r="A163" s="30"/>
       <c r="B163" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="29"/>
+      <c r="A164" s="30"/>
       <c r="B164" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="C164" s="8" t="s">
+      <c r="C164" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="29" t="str">
+      <c r="A165" s="30" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
       <c r="B165" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C165" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="29"/>
+      <c r="A166" s="30"/>
       <c r="B166" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C166" s="8" t="s">
+      <c r="C166" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="29"/>
+      <c r="A167" s="30"/>
       <c r="B167" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C167" s="8" t="s">
+      <c r="C167" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="29"/>
+      <c r="A168" s="30"/>
       <c r="B168" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C168" s="8" t="s">
+      <c r="C168" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="29" t="str">
+      <c r="A169" s="30" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C169" s="8" t="s">
+      <c r="C169" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="29"/>
+      <c r="A170" s="30"/>
       <c r="B170" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C170" s="8" t="s">
+      <c r="C170" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="29"/>
+      <c r="A171" s="30"/>
       <c r="B171" s="16" t="s">
         <v>242</v>
       </c>
+      <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="29"/>
+      <c r="A172" s="30"/>
       <c r="B172" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
+      <c r="A173" s="30"/>
       <c r="B173" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="29" t="str">
+      <c r="A174" s="30" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
       <c r="B174" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="29"/>
+      <c r="A175" s="30"/>
       <c r="B175" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="29"/>
+      <c r="A176" s="30"/>
       <c r="B176" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="29"/>
+      <c r="A177" s="30"/>
       <c r="B177" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="29" t="str">
+      <c r="A178" s="30" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
       <c r="B178" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="29"/>
+      <c r="A179" s="30"/>
       <c r="B179" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="29"/>
+      <c r="A180" s="30"/>
       <c r="B180" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="29"/>
+      <c r="A181" s="30"/>
       <c r="B181" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="29"/>
+      <c r="A182" s="30"/>
       <c r="B182" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="29" t="str">
+      <c r="A183" s="30" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
       <c r="B183" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="30"/>
+      <c r="B184" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C183" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="29"/>
-      <c r="B184" s="9" t="s">
+      <c r="C184" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="30"/>
+      <c r="B185" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C184" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="29"/>
-      <c r="B185" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="C185" t="s">
+      <c r="C185" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="29" t="str">
+      <c r="A186" s="30" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
       <c r="B186" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="29"/>
+      <c r="A187" s="30"/>
       <c r="B187" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="29"/>
+      <c r="A188" s="30"/>
       <c r="B188" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="29"/>
-      <c r="B189" s="9" t="s">
+      <c r="A189" s="33"/>
+      <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D189">
@@ -3195,13 +3254,177 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="28"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="28"/>
+      <c r="A190" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B190" s="29"/>
+      <c r="C190" s="29"/>
+    </row>
+    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="28" t="str">
+        <f>'S 8'!A1</f>
+        <v>I want to be able to create large curved sections without the colliders bugging out.</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="str">
+        <f>'S 8'!A2</f>
+        <v>I want a way to remove a locomotive from the world.</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="29" t="str">
+        <f>'S 8'!A3</f>
+        <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="29"/>
+      <c r="B194" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="29"/>
+      <c r="B195" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="29"/>
+      <c r="B196" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="29"/>
+      <c r="B197" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="29"/>
+      <c r="B198" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="29" t="str">
+        <f>'S 8'!A4</f>
+        <v>I want to be able to create a new bauble partway along curved track.</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="29"/>
+      <c r="B200" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="29"/>
+      <c r="B201" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="29" t="str">
+        <f>'S 8'!A5</f>
+        <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="29"/>
+      <c r="B203" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="29"/>
+      <c r="B204" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="29" t="str">
+        <f>'S 8'!A6</f>
+        <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
+      </c>
+      <c r="B205" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="29"/>
+      <c r="B206" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="62">
+    <mergeCell ref="A202:A204"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A198"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3218,50 +3441,45 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3270,7 +3488,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3565,7 +3783,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3648,7 +3866,7 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -3663,9 +3881,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3674,12 +3894,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -3698,13 +3918,8 @@
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>218</v>
+      <c r="A6" s="14" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug with rail vector bending, and locomotives can be deleted and derailed better.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="272">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1043,13 +1043,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1063,12 +1069,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1376,7 +1376,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A184" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
+      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,8 +1401,8 @@
       <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="str">
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1607,11 +1607,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="33" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="32"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1866,7 +1866,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1879,11 +1879,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="str">
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2154,11 +2154,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="33" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="32"/>
-      <c r="C78" s="34"/>
+      <c r="C78" s="36"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="str">
@@ -2479,7 +2479,7 @@
       <c r="C110" s="29"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="31" t="str">
+      <c r="A111" s="33" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="31"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="C135" s="32"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="31" t="str">
+      <c r="A136" s="33" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="C159" s="32"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="31" t="str">
+      <c r="A160" s="33" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="33"/>
+      <c r="A189" s="31"/>
       <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
@@ -3268,6 +3268,9 @@
       <c r="B191" s="9" t="s">
         <v>254</v>
       </c>
+      <c r="C191" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="str">
@@ -3277,8 +3280,11 @@
       <c r="B192" s="9" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C192" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
@@ -3287,37 +3293,37 @@
         <v>257</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="29"/>
       <c r="B195" s="9" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="29"/>
       <c r="B196" s="9" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="29"/>
       <c r="B197" s="9" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="29"/>
       <c r="B198" s="9" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="29" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
@@ -3326,19 +3332,19 @@
         <v>264</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="29"/>
       <c r="B200" s="9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="29"/>
       <c r="B201" s="9" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
@@ -3347,19 +3353,19 @@
         <v>267</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="29"/>
       <c r="B203" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="29"/>
       <c r="B204" s="9" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
@@ -3367,64 +3373,28 @@
       <c r="B205" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C205" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="29"/>
       <c r="B206" s="9" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C206" t="s">
+        <v>24</v>
+      </c>
+      <c r="D206">
+        <f>COUNTA(C191:C206)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A202:A204"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A198"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3441,6 +3411,52 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A202:A204"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A198"/>
+    <mergeCell ref="A199:A201"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3452,7 +3468,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed math functions for computing partial transition at one end.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="272">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -814,9 +814,6 @@
     <t>Make track section bend to curved end bauble</t>
   </si>
   <si>
-    <t>Make track section bend to curved start bauble.</t>
-  </si>
-  <si>
     <t>Remove condition for the track to be straight before splitting it</t>
   </si>
   <si>
@@ -839,6 +836,9 @@
   </si>
   <si>
     <t>Fix rigidbody velocity and stop traversing if trackSection becomes null</t>
+  </si>
+  <si>
+    <t>Make track section bend to curved start and end bauble.</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1036,6 +1036,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1376,7 +1379,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A184" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
+      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,14 +1401,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="str">
+      <c r="A3" s="31" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1417,7 +1420,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1429,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1435,7 +1438,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="str">
+      <c r="A6" s="31" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1447,7 +1450,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1459,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1465,7 +1468,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1474,7 +1477,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1483,7 +1486,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1492,7 +1495,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="31" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1504,7 +1507,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1513,7 +1516,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1522,7 +1525,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="31" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1534,7 +1537,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1543,7 +1546,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1552,7 +1555,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1561,7 +1564,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="31" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1573,7 +1576,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1582,7 +1585,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="31" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1594,7 +1597,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1607,11 +1610,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="37"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1626,7 +1629,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="str">
+      <c r="A25" s="31" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1638,7 +1641,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
@@ -1647,7 +1650,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="str">
+      <c r="A27" s="31" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1659,7 +1662,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1668,7 +1671,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1677,7 +1680,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1686,7 +1689,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
@@ -1695,7 +1698,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="10" t="s">
         <v>46</v>
       </c>
@@ -1704,7 +1707,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
@@ -1713,7 +1716,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="str">
+      <c r="A34" s="31" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -1725,7 +1728,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
@@ -1734,7 +1737,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="10" t="s">
         <v>51</v>
       </c>
@@ -1743,7 +1746,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -1752,7 +1755,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="str">
+      <c r="A38" s="31" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -1764,7 +1767,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
@@ -1785,7 +1788,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="str">
+      <c r="A41" s="31" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -1797,7 +1800,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
@@ -1806,7 +1809,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="10" t="s">
         <v>58</v>
       </c>
@@ -1815,7 +1818,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
@@ -1824,7 +1827,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="str">
+      <c r="A45" s="31" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -1836,7 +1839,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1845,7 +1848,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="str">
+      <c r="A47" s="31" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -1857,7 +1860,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1866,7 +1869,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1879,14 +1882,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="40"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="str">
+      <c r="A51" s="31" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -1898,7 +1901,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="10" t="s">
         <v>77</v>
       </c>
@@ -1907,7 +1910,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="10" t="s">
         <v>78</v>
       </c>
@@ -1916,7 +1919,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="str">
+      <c r="A54" s="31" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -1928,7 +1931,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="31"/>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -1937,7 +1940,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="str">
+      <c r="A56" s="31" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -1949,7 +1952,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="10" t="s">
         <v>82</v>
       </c>
@@ -1958,7 +1961,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="str">
+      <c r="A58" s="31" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -1970,7 +1973,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="9" t="s">
         <v>99</v>
       </c>
@@ -1979,7 +1982,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="10" t="s">
         <v>84</v>
       </c>
@@ -1988,7 +1991,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="10" t="s">
         <v>85</v>
       </c>
@@ -1997,7 +2000,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="15" t="s">
         <v>86</v>
       </c>
@@ -2006,7 +2009,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="9" t="s">
         <v>105</v>
       </c>
@@ -2015,7 +2018,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="10" t="s">
         <v>91</v>
       </c>
@@ -2024,7 +2027,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="str">
+      <c r="A65" s="31" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -2034,7 +2037,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="5" t="s">
         <v>88</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="str">
+      <c r="A67" s="31" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -2055,7 +2058,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="5" t="s">
         <v>90</v>
       </c>
@@ -2064,7 +2067,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="str">
+      <c r="A69" s="31" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2076,21 +2079,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="5" t="s">
         <v>95</v>
       </c>
@@ -2099,7 +2102,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="str">
+      <c r="A73" s="31" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2111,7 +2114,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="19" t="s">
         <v>97</v>
       </c>
@@ -2120,7 +2123,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="str">
+      <c r="A75" s="31" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2132,7 +2135,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="19" t="s">
         <v>103</v>
       </c>
@@ -2141,7 +2144,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2154,14 +2157,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="36"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="37"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="str">
+      <c r="A79" s="31" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2173,7 +2176,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="9" t="s">
         <v>119</v>
       </c>
@@ -2182,7 +2185,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="str">
+      <c r="A81" s="31" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2194,7 +2197,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="31"/>
       <c r="B82" s="9" t="s">
         <v>120</v>
       </c>
@@ -2203,7 +2206,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="str">
+      <c r="A83" s="31" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2215,7 +2218,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="31"/>
       <c r="B84" s="9" t="s">
         <v>122</v>
       </c>
@@ -2224,14 +2227,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="31"/>
       <c r="B85" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="str">
+      <c r="A86" s="31" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2243,7 +2246,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="31"/>
       <c r="B87" s="9" t="s">
         <v>125</v>
       </c>
@@ -2252,7 +2255,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="31"/>
       <c r="B88" s="9" t="s">
         <v>126</v>
       </c>
@@ -2261,7 +2264,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="9" t="s">
         <v>127</v>
       </c>
@@ -2270,7 +2273,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="9" t="s">
         <v>128</v>
       </c>
@@ -2279,7 +2282,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="9" t="s">
         <v>129</v>
       </c>
@@ -2288,7 +2291,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="str">
+      <c r="A92" s="31" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2300,7 +2303,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="9" t="s">
         <v>131</v>
       </c>
@@ -2309,7 +2312,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="9" t="s">
         <v>132</v>
       </c>
@@ -2318,7 +2321,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="9" t="s">
         <v>133</v>
       </c>
@@ -2327,7 +2330,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="str">
+      <c r="A96" s="31" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2339,7 +2342,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="9" t="s">
         <v>134</v>
       </c>
@@ -2348,7 +2351,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="9" t="s">
         <v>135</v>
       </c>
@@ -2357,7 +2360,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="str">
+      <c r="A99" s="31" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2369,7 +2372,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="9" t="s">
         <v>138</v>
       </c>
@@ -2378,7 +2381,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="9" t="s">
         <v>137</v>
       </c>
@@ -2387,7 +2390,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="9" t="s">
         <v>139</v>
       </c>
@@ -2396,7 +2399,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="9" t="s">
         <v>147</v>
       </c>
@@ -2405,7 +2408,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="str">
+      <c r="A104" s="31" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2417,7 +2420,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="31"/>
       <c r="B105" s="9" t="s">
         <v>141</v>
       </c>
@@ -2426,7 +2429,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="31"/>
       <c r="B106" s="9" t="s">
         <v>142</v>
       </c>
@@ -2435,7 +2438,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="30" t="str">
+      <c r="A107" s="31" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2447,7 +2450,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="31"/>
       <c r="B108" s="9" t="s">
         <v>144</v>
       </c>
@@ -2472,14 +2475,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="29" t="s">
+      <c r="A110" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="29"/>
-      <c r="C110" s="29"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="33" t="str">
+      <c r="A111" s="34" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2491,7 +2494,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="31"/>
       <c r="B112" s="9" t="s">
         <v>171</v>
       </c>
@@ -2500,7 +2503,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="31"/>
       <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
@@ -2509,7 +2512,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="31"/>
       <c r="B114" s="9" t="s">
         <v>158</v>
       </c>
@@ -2518,7 +2521,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="31"/>
       <c r="B115" s="9" t="s">
         <v>159</v>
       </c>
@@ -2527,7 +2530,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="str">
+      <c r="A116" s="31" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2539,7 +2542,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="31"/>
       <c r="B117" s="9" t="s">
         <v>157</v>
       </c>
@@ -2548,7 +2551,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="30" t="str">
+      <c r="A118" s="31" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2560,7 +2563,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="31"/>
       <c r="B119" s="9" t="s">
         <v>161</v>
       </c>
@@ -2569,7 +2572,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="A120" s="31"/>
       <c r="B120" s="9" t="s">
         <v>172</v>
       </c>
@@ -2578,7 +2581,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="str">
+      <c r="A121" s="31" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2590,7 +2593,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="31"/>
       <c r="B122" s="24" t="s">
         <v>162</v>
       </c>
@@ -2599,7 +2602,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="31"/>
       <c r="B123" s="9" t="s">
         <v>176</v>
       </c>
@@ -2608,7 +2611,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="31"/>
       <c r="B124" s="9" t="s">
         <v>177</v>
       </c>
@@ -2617,7 +2620,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30" t="str">
+      <c r="A125" s="31" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2629,7 +2632,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="31"/>
       <c r="B126" s="9" t="s">
         <v>165</v>
       </c>
@@ -2638,7 +2641,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="31"/>
       <c r="B127" s="9" t="s">
         <v>166</v>
       </c>
@@ -2647,7 +2650,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30" t="str">
+      <c r="A128" s="31" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2659,7 +2662,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="31"/>
       <c r="B129" s="9" t="s">
         <v>168</v>
       </c>
@@ -2668,7 +2671,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="31"/>
       <c r="B130" s="9" t="s">
         <v>169</v>
       </c>
@@ -2677,7 +2680,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="31"/>
       <c r="B131" s="9" t="s">
         <v>178</v>
       </c>
@@ -2686,7 +2689,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="30" t="str">
+      <c r="A132" s="31" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -2698,7 +2701,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="31"/>
       <c r="B133" s="9" t="s">
         <v>170</v>
       </c>
@@ -2707,7 +2710,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="31"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2720,14 +2723,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="32" t="s">
+      <c r="A135" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="B135" s="32"/>
-      <c r="C135" s="32"/>
+      <c r="B135" s="33"/>
+      <c r="C135" s="33"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="str">
+      <c r="A136" s="34" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2739,7 +2742,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="30"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="9" t="s">
         <v>186</v>
       </c>
@@ -2748,7 +2751,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="30"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="9" t="s">
         <v>200</v>
       </c>
@@ -2757,7 +2760,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
+      <c r="A139" s="31"/>
       <c r="B139" s="9" t="s">
         <v>187</v>
       </c>
@@ -2766,7 +2769,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="30"/>
+      <c r="A140" s="31"/>
       <c r="B140" s="9" t="s">
         <v>188</v>
       </c>
@@ -2775,7 +2778,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="str">
+      <c r="A141" s="31" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="30"/>
+      <c r="A142" s="31"/>
       <c r="B142" s="9" t="s">
         <v>190</v>
       </c>
@@ -2796,7 +2799,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="30"/>
+      <c r="A143" s="31"/>
       <c r="B143" s="9" t="s">
         <v>191</v>
       </c>
@@ -2805,7 +2808,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="30" t="str">
+      <c r="A144" s="31" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -2817,7 +2820,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="30"/>
+      <c r="A145" s="31"/>
       <c r="B145" s="9" t="s">
         <v>204</v>
       </c>
@@ -2826,7 +2829,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="30"/>
+      <c r="A146" s="31"/>
       <c r="B146" s="9" t="s">
         <v>207</v>
       </c>
@@ -2835,7 +2838,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="30"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="9" t="s">
         <v>205</v>
       </c>
@@ -2844,7 +2847,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
+      <c r="A148" s="31"/>
       <c r="B148" s="9" t="s">
         <v>208</v>
       </c>
@@ -2853,7 +2856,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
+      <c r="A149" s="31"/>
       <c r="B149" s="9" t="s">
         <v>206</v>
       </c>
@@ -2862,7 +2865,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="30" t="str">
+      <c r="A150" s="31" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -2874,7 +2877,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
+      <c r="A151" s="31"/>
       <c r="B151" s="24" t="s">
         <v>209</v>
       </c>
@@ -2883,14 +2886,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="30"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="16" t="s">
         <v>193</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="30" t="str">
+      <c r="A153" s="31" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -2902,7 +2905,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="30"/>
+      <c r="A154" s="31"/>
       <c r="B154" s="9" t="s">
         <v>197</v>
       </c>
@@ -2911,7 +2914,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="30"/>
+      <c r="A155" s="31"/>
       <c r="B155" s="9" t="s">
         <v>194</v>
       </c>
@@ -2920,7 +2923,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="30"/>
+      <c r="A156" s="31"/>
       <c r="B156" s="9" t="s">
         <v>195</v>
       </c>
@@ -2929,7 +2932,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="30"/>
+      <c r="A157" s="31"/>
       <c r="B157" s="9" t="s">
         <v>212</v>
       </c>
@@ -2954,14 +2957,14 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="32" t="s">
+      <c r="A159" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="B159" s="32"/>
-      <c r="C159" s="32"/>
+      <c r="B159" s="33"/>
+      <c r="C159" s="33"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="33" t="str">
+      <c r="A160" s="34" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -2973,7 +2976,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="30"/>
+      <c r="A161" s="31"/>
       <c r="B161" s="9" t="s">
         <v>227</v>
       </c>
@@ -2982,7 +2985,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="30"/>
+      <c r="A162" s="31"/>
       <c r="B162" s="9" t="s">
         <v>243</v>
       </c>
@@ -2991,7 +2994,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="30"/>
+      <c r="A163" s="31"/>
       <c r="B163" s="9" t="s">
         <v>222</v>
       </c>
@@ -3000,7 +3003,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="30"/>
+      <c r="A164" s="31"/>
       <c r="B164" s="9" t="s">
         <v>220</v>
       </c>
@@ -3009,7 +3012,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="30" t="str">
+      <c r="A165" s="31" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -3021,7 +3024,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="30"/>
+      <c r="A166" s="31"/>
       <c r="B166" s="9" t="s">
         <v>229</v>
       </c>
@@ -3030,7 +3033,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="30"/>
+      <c r="A167" s="31"/>
       <c r="B167" s="9" t="s">
         <v>223</v>
       </c>
@@ -3039,7 +3042,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="30"/>
+      <c r="A168" s="31"/>
       <c r="B168" s="9" t="s">
         <v>224</v>
       </c>
@@ -3048,7 +3051,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="30" t="str">
+      <c r="A169" s="31" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -3060,7 +3063,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="30"/>
+      <c r="A170" s="31"/>
       <c r="B170" s="9" t="s">
         <v>225</v>
       </c>
@@ -3069,14 +3072,14 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="30"/>
+      <c r="A171" s="31"/>
       <c r="B171" s="16" t="s">
         <v>242</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="30"/>
+      <c r="A172" s="31"/>
       <c r="B172" s="9" t="s">
         <v>244</v>
       </c>
@@ -3085,7 +3088,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="30"/>
+      <c r="A173" s="31"/>
       <c r="B173" s="9" t="s">
         <v>231</v>
       </c>
@@ -3094,7 +3097,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="30" t="str">
+      <c r="A174" s="31" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3106,7 +3109,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="30"/>
+      <c r="A175" s="31"/>
       <c r="B175" s="9" t="s">
         <v>233</v>
       </c>
@@ -3115,7 +3118,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="30"/>
+      <c r="A176" s="31"/>
       <c r="B176" s="9" t="s">
         <v>230</v>
       </c>
@@ -3124,7 +3127,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="30"/>
+      <c r="A177" s="31"/>
       <c r="B177" s="9" t="s">
         <v>232</v>
       </c>
@@ -3133,7 +3136,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="30" t="str">
+      <c r="A178" s="31" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3145,7 +3148,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="30"/>
+      <c r="A179" s="31"/>
       <c r="B179" s="9" t="s">
         <v>246</v>
       </c>
@@ -3154,7 +3157,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="30"/>
+      <c r="A180" s="31"/>
       <c r="B180" s="9" t="s">
         <v>235</v>
       </c>
@@ -3163,7 +3166,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="30"/>
+      <c r="A181" s="31"/>
       <c r="B181" s="9" t="s">
         <v>236</v>
       </c>
@@ -3172,7 +3175,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="30"/>
+      <c r="A182" s="31"/>
       <c r="B182" s="9" t="s">
         <v>237</v>
       </c>
@@ -3181,7 +3184,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="30" t="str">
+      <c r="A183" s="31" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
@@ -3193,7 +3196,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="30"/>
+      <c r="A184" s="31"/>
       <c r="B184" s="9" t="s">
         <v>249</v>
       </c>
@@ -3202,7 +3205,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="30"/>
+      <c r="A185" s="31"/>
       <c r="B185" s="9" t="s">
         <v>250</v>
       </c>
@@ -3211,7 +3214,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="30" t="str">
+      <c r="A186" s="31" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
@@ -3223,7 +3226,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="30"/>
+      <c r="A187" s="31"/>
       <c r="B187" s="9" t="s">
         <v>238</v>
       </c>
@@ -3232,7 +3235,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="30"/>
+      <c r="A188" s="31"/>
       <c r="B188" s="9" t="s">
         <v>241</v>
       </c>
@@ -3241,7 +3244,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="31"/>
+      <c r="A189" s="32"/>
       <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
@@ -3254,14 +3257,14 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="29" t="s">
+      <c r="A190" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="B190" s="29"/>
-      <c r="C190" s="29"/>
+      <c r="B190" s="30"/>
+      <c r="C190" s="30"/>
     </row>
     <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="28" t="str">
+      <c r="A191" s="29" t="str">
         <f>'S 8'!A1</f>
         <v>I want to be able to create large curved sections without the colliders bugging out.</v>
       </c>
@@ -3285,109 +3288,118 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="29" t="str">
+      <c r="A193" s="30" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>257</v>
       </c>
+      <c r="C193" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="29"/>
+      <c r="A194" s="30"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
       </c>
+      <c r="C194" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="29"/>
+      <c r="A195" s="30"/>
       <c r="B195" s="9" t="s">
         <v>261</v>
       </c>
+      <c r="C195" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="29"/>
+      <c r="A196" s="30"/>
       <c r="B196" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="29"/>
+      <c r="A197" s="30"/>
       <c r="B197" s="9" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="29"/>
+      <c r="A198" s="30"/>
       <c r="B198" s="9" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="29" t="str">
+      <c r="A199" s="30" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
       <c r="B199" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="30"/>
+      <c r="B200" s="9" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="29"/>
-      <c r="B200" s="9" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="30"/>
+      <c r="B201" s="9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
-      <c r="B201" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
     <row r="202" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="29" t="str">
+      <c r="A202" s="30" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
       <c r="B202" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="30"/>
+      <c r="B203" s="9" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="29"/>
-      <c r="B203" s="9" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="30"/>
+      <c r="B204" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
-      <c r="B204" s="9" t="s">
-        <v>269</v>
-      </c>
-    </row>
     <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="29" t="str">
+      <c r="A205" s="30" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C205" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="29"/>
+      <c r="A206" s="30"/>
       <c r="B206" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C206" t="s">
         <v>24</v>
       </c>
       <c r="D206">
         <f>COUNTA(C191:C206)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Partial transitions at a single free end work.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="276">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -805,15 +805,9 @@
     <t>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</t>
   </si>
   <si>
-    <t>Allow for exceptional case where a bauble is right on the apex</t>
-  </si>
-  <si>
     <t>Find equation for projecting endpoint if a given location has given curvature</t>
   </si>
   <si>
-    <t>Make track section bend to curved end bauble</t>
-  </si>
-  <si>
     <t>Remove condition for the track to be straight before splitting it</t>
   </si>
   <si>
@@ -838,7 +832,25 @@
     <t>Fix rigidbody velocity and stop traversing if trackSection becomes null</t>
   </si>
   <si>
-    <t>Make track section bend to curved start and end bauble.</t>
+    <t>Calc. Params for rotate -&gt; rotate/radius</t>
+  </si>
+  <si>
+    <t>fixed -&gt; rotate/radius</t>
+  </si>
+  <si>
+    <t>rotate/radius -&gt; rotate/radius</t>
+  </si>
+  <si>
+    <t>fixed/radius -&gt; rotate/radius</t>
+  </si>
+  <si>
+    <t>rotate -&gt; fixed/radius</t>
+  </si>
+  <si>
+    <t>fixed/radius -&gt; fixed/radius</t>
+  </si>
+  <si>
+    <t>fixed -&gt; fixed/radius</t>
   </si>
 </sst>
 </file>
@@ -1374,12 +1386,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A184" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A183" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
+      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,7 +3299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="30" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
@@ -3299,7 +3311,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="30"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
@@ -3308,102 +3320,134 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="30"/>
       <c r="B195" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C195" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="30"/>
       <c r="B196" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="C196" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="30"/>
       <c r="B197" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="30"/>
       <c r="B198" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="30" t="str">
+        <v>271</v>
+      </c>
+      <c r="C198" s="8"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="30"/>
+      <c r="B199" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C199" s="8"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="30"/>
+      <c r="B200" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="30"/>
+      <c r="B201" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="30"/>
+      <c r="B202" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="30" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
-      <c r="B199" s="9" t="s">
+      <c r="B203" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="30"/>
+      <c r="B204" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="30"/>
+      <c r="B205" s="9" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="30"/>
-      <c r="B200" s="9" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="30"/>
-      <c r="B201" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="30" t="str">
+    <row r="206" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="30" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
-      <c r="B202" s="9" t="s">
+      <c r="B206" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="30"/>
+      <c r="B207" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="30"/>
+      <c r="B208" s="9" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="30"/>
-      <c r="B203" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="30"/>
-      <c r="B204" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="30" t="str">
+    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="30" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
-      <c r="B205" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="C205" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="30"/>
-      <c r="B206" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C206" t="s">
-        <v>24</v>
-      </c>
-      <c r="D206">
-        <f>COUNTA(C191:C206)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="28"/>
+      <c r="B209" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C209" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="30"/>
+      <c r="B210" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C210" t="s">
+        <v>24</v>
+      </c>
+      <c r="D210">
+        <f>COUNTA(C191:C210)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="62">
@@ -3464,11 +3508,11 @@
     <mergeCell ref="A178:A182"/>
     <mergeCell ref="A186:A189"/>
     <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A202:A204"/>
-    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
     <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A198"/>
-    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed some glaring issues with the previous two commits.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -1052,25 +1052,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1084,6 +1078,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,7 +1391,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A183" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C197" sqref="C197"/>
+      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,8 +1416,8 @@
       <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="str">
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1622,11 +1622,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="33"/>
-      <c r="C23" s="37"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1894,11 +1894,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="str">
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="34"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2169,11 +2169,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="30" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="33"/>
-      <c r="C78" s="37"/>
+      <c r="C78" s="35"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="str">
@@ -2487,14 +2487,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="30"/>
-      <c r="C110" s="30"/>
+      <c r="B110" s="32"/>
+      <c r="C110" s="32"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="str">
+      <c r="A111" s="30" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="34"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="C135" s="33"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="34" t="str">
+      <c r="A136" s="30" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="C159" s="33"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="34" t="str">
+      <c r="A160" s="30" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3256,7 +3256,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="32"/>
+      <c r="A189" s="34"/>
       <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
@@ -3269,11 +3269,11 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="30" t="s">
+      <c r="A190" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="B190" s="30"/>
-      <c r="C190" s="30"/>
+      <c r="B190" s="32"/>
+      <c r="C190" s="32"/>
     </row>
     <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="str">
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="30" t="str">
+      <c r="A193" s="32" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3312,7 +3312,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="30"/>
+      <c r="A194" s="32"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
       </c>
@@ -3321,7 +3321,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="30"/>
+      <c r="A195" s="32"/>
       <c r="B195" s="9" t="s">
         <v>260</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="30"/>
+      <c r="A196" s="32"/>
       <c r="B196" s="9" t="s">
         <v>269</v>
       </c>
@@ -3339,7 +3339,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="30"/>
+      <c r="A197" s="32"/>
       <c r="B197" s="9" t="s">
         <v>270</v>
       </c>
@@ -3348,39 +3348,39 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="30"/>
+      <c r="A198" s="32"/>
       <c r="B198" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C198" s="8"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="30"/>
+      <c r="A199" s="32"/>
       <c r="B199" s="9" t="s">
         <v>272</v>
       </c>
       <c r="C199" s="8"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="30"/>
+      <c r="A200" s="32"/>
       <c r="B200" s="9" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="30"/>
+      <c r="A201" s="32"/>
       <c r="B201" s="9" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="30"/>
+      <c r="A202" s="32"/>
       <c r="B202" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="30" t="str">
+      <c r="A203" s="32" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3389,19 +3389,19 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="30"/>
+      <c r="A204" s="32"/>
       <c r="B204" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="30"/>
+      <c r="A205" s="32"/>
       <c r="B205" s="9" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="30" t="str">
+      <c r="A206" s="32" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3410,19 +3410,19 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="30"/>
+      <c r="A207" s="32"/>
       <c r="B207" s="9" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="30"/>
+      <c r="A208" s="32"/>
       <c r="B208" s="9" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="30" t="str">
+      <c r="A209" s="32" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3434,7 +3434,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="30"/>
+      <c r="A210" s="32"/>
       <c r="B210" s="9" t="s">
         <v>267</v>
       </c>
@@ -3451,6 +3451,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3467,52 +3513,6 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
A free piece of track can now have curvature at both ends.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="276">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1052,19 +1052,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1078,12 +1084,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,7 +1391,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A183" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
+      <selection pane="bottomLeft" activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,8 +1416,8 @@
       <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="str">
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1622,11 +1622,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="34" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="33"/>
-      <c r="C23" s="35"/>
+      <c r="C23" s="37"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1894,11 +1894,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="40"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="str">
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2169,11 +2169,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="34" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="33"/>
-      <c r="C78" s="35"/>
+      <c r="C78" s="37"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="str">
@@ -2487,14 +2487,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="32" t="s">
+      <c r="A110" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="str">
+      <c r="A111" s="34" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="C135" s="33"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="34" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="C159" s="33"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="30" t="str">
+      <c r="A160" s="34" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3256,7 +3256,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="34"/>
+      <c r="A189" s="32"/>
       <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
@@ -3269,11 +3269,11 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="32" t="s">
+      <c r="A190" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="B190" s="32"/>
-      <c r="C190" s="32"/>
+      <c r="B190" s="30"/>
+      <c r="C190" s="30"/>
     </row>
     <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="str">
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="32" t="str">
+      <c r="A193" s="30" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3312,7 +3312,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="32"/>
+      <c r="A194" s="30"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
       </c>
@@ -3321,7 +3321,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="32"/>
+      <c r="A195" s="30"/>
       <c r="B195" s="9" t="s">
         <v>260</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="32"/>
+      <c r="A196" s="30"/>
       <c r="B196" s="9" t="s">
         <v>269</v>
       </c>
@@ -3339,7 +3339,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="32"/>
+      <c r="A197" s="30"/>
       <c r="B197" s="9" t="s">
         <v>270</v>
       </c>
@@ -3348,39 +3348,41 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="32"/>
+      <c r="A198" s="30"/>
       <c r="B198" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="C198" s="8"/>
+      <c r="C198" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="32"/>
+      <c r="A199" s="30"/>
       <c r="B199" s="9" t="s">
         <v>272</v>
       </c>
       <c r="C199" s="8"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="32"/>
+      <c r="A200" s="30"/>
       <c r="B200" s="9" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="32"/>
+      <c r="A201" s="30"/>
       <c r="B201" s="9" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="32"/>
+      <c r="A202" s="30"/>
       <c r="B202" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="32" t="str">
+      <c r="A203" s="30" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3389,19 +3391,19 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="32"/>
+      <c r="A204" s="30"/>
       <c r="B204" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="32"/>
+      <c r="A205" s="30"/>
       <c r="B205" s="9" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="32" t="str">
+      <c r="A206" s="30" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3410,19 +3412,19 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="32"/>
+      <c r="A207" s="30"/>
       <c r="B207" s="9" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="32"/>
+      <c r="A208" s="30"/>
       <c r="B208" s="9" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="32" t="str">
+      <c r="A209" s="30" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3434,7 +3436,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="32"/>
+      <c r="A210" s="30"/>
       <c r="B210" s="9" t="s">
         <v>267</v>
       </c>
@@ -3443,7 +3445,7 @@
       </c>
       <c r="D210">
         <f>COUNTA(C191:C210)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3451,52 +3453,6 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3513,6 +3469,52 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed/Radius -> Free curves now used properly by shape controller, and a small fix for partial curves not giving position properly.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="276">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1052,25 +1052,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1084,6 +1078,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,7 +1391,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A183" activePane="bottomLeft"/>
       <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C199" sqref="C199"/>
+      <selection pane="bottomLeft" activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,8 +1416,8 @@
       <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="str">
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1622,11 +1622,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="33"/>
-      <c r="C23" s="37"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
@@ -1894,11 +1894,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="str">
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="34"/>
       <c r="B77" s="20" t="s">
         <v>104</v>
       </c>
@@ -2169,11 +2169,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="30" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="33"/>
-      <c r="C78" s="37"/>
+      <c r="C78" s="35"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="str">
@@ -2487,14 +2487,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="30"/>
-      <c r="C110" s="30"/>
+      <c r="B110" s="32"/>
+      <c r="C110" s="32"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="str">
+      <c r="A111" s="30" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="34"/>
       <c r="B134" s="22" t="s">
         <v>180</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="C135" s="33"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="34" t="str">
+      <c r="A136" s="30" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="C159" s="33"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="34" t="str">
+      <c r="A160" s="30" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3256,7 +3256,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="32"/>
+      <c r="A189" s="34"/>
       <c r="B189" s="22" t="s">
         <v>239</v>
       </c>
@@ -3269,11 +3269,11 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="30" t="s">
+      <c r="A190" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="B190" s="30"/>
-      <c r="C190" s="30"/>
+      <c r="B190" s="32"/>
+      <c r="C190" s="32"/>
     </row>
     <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="str">
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="30" t="str">
+      <c r="A193" s="32" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3312,7 +3312,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="30"/>
+      <c r="A194" s="32"/>
       <c r="B194" s="9" t="s">
         <v>258</v>
       </c>
@@ -3321,7 +3321,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="30"/>
+      <c r="A195" s="32"/>
       <c r="B195" s="9" t="s">
         <v>260</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="30"/>
+      <c r="A196" s="32"/>
       <c r="B196" s="9" t="s">
         <v>269</v>
       </c>
@@ -3339,7 +3339,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="30"/>
+      <c r="A197" s="32"/>
       <c r="B197" s="9" t="s">
         <v>270</v>
       </c>
@@ -3348,7 +3348,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="30"/>
+      <c r="A198" s="32"/>
       <c r="B198" s="9" t="s">
         <v>271</v>
       </c>
@@ -3357,32 +3357,35 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="30"/>
+      <c r="A199" s="32"/>
       <c r="B199" s="9" t="s">
         <v>272</v>
       </c>
       <c r="C199" s="8"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="30"/>
+      <c r="A200" s="32"/>
       <c r="B200" s="9" t="s">
         <v>273</v>
       </c>
+      <c r="C200" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="30"/>
+      <c r="A201" s="32"/>
       <c r="B201" s="9" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="30"/>
+      <c r="A202" s="32"/>
       <c r="B202" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="30" t="str">
+      <c r="A203" s="32" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3391,19 +3394,19 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="30"/>
+      <c r="A204" s="32"/>
       <c r="B204" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="30"/>
+      <c r="A205" s="32"/>
       <c r="B205" s="9" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="30" t="str">
+      <c r="A206" s="32" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3412,19 +3415,19 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="30"/>
+      <c r="A207" s="32"/>
       <c r="B207" s="9" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="30"/>
+      <c r="A208" s="32"/>
       <c r="B208" s="9" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="30" t="str">
+      <c r="A209" s="32" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3436,7 +3439,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="30"/>
+      <c r="A210" s="32"/>
       <c r="B210" s="9" t="s">
         <v>267</v>
       </c>
@@ -3445,7 +3448,7 @@
       </c>
       <c r="D210">
         <f>COUNTA(C191:C210)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,6 +3456,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3469,52 +3518,6 @@
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
     <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated User Stories for Iteration 9, removed race condition for loading Control vs Terrain, and stopped a lot of Unity Test Tools from building outside the editor.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="S 7" sheetId="11" r:id="rId8"/>
     <sheet name="S 8" sheetId="12" r:id="rId9"/>
     <sheet name="S 9" sheetId="14" r:id="rId10"/>
+    <sheet name="S 10" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="288">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -46,9 +47,6 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Init  Camera angle, implement click-drag panning</t>
   </si>
   <si>
@@ -851,13 +849,52 @@
   </si>
   <si>
     <t>fixed -&gt; fixed/radius</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>[S]tarted</t>
+  </si>
+  <si>
+    <t>[C]omplete</t>
+  </si>
+  <si>
+    <t>[R]eview</t>
+  </si>
+  <si>
+    <t>[P]ostponed</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Iteration 9</t>
+  </si>
+  <si>
+    <t>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</t>
+  </si>
+  <si>
+    <t>I want the track to be able to transition [Fixed -&gt; Rotate/Radius]</t>
+  </si>
+  <si>
+    <t>I want the track to be able to transition [Fixed/Radius -&gt; Fixed/Radius]</t>
+  </si>
+  <si>
+    <t>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</t>
+  </si>
+  <si>
+    <t>I want a bauble to retain its curvature after saving and reloading a map.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -873,16 +910,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6161"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD961"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2DE82"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF61D6FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -979,11 +1046,155 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1046,10 +1257,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1085,12 +1310,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D6FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD961"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D6FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD961"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6161"/>
+      <color rgb="FF61D6FF"/>
+      <color rgb="FFFFD961"/>
+      <color rgb="FFB2DE82"/>
+      <color rgb="FFFF6464"/>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1386,22 +1693,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D211"/>
+  <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A183" activePane="bottomLeft"/>
-      <selection activeCell="A164" sqref="A164"/>
-      <selection pane="bottomLeft" activeCell="C201" sqref="C201"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="615" topLeftCell="A187" activePane="bottomLeft"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A211" sqref="A211:B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1409,212 +1720,224 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="str">
+        <v>275</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="5" t="s">
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="str">
+      <c r="A19" s="41" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="C20" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="str">
+      <c r="A21" s="41" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <f>COUNTA(C3:C22)</f>
@@ -1622,11 +1945,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="35"/>
+      <c r="A23" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="43"/>
+      <c r="C23" s="45"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1634,157 +1957,157 @@
         <v>I want a button on the toolbar for utilities.</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="str">
+      <c r="A25" s="41" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="C26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="str">
+      <c r="A27" s="41" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="41"/>
+      <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="41"/>
+      <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="str">
+      <c r="A34" s="41" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="41"/>
+      <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="10" t="s">
+      <c r="C36" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="C37" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="str">
+      <c r="A38" s="41" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="41"/>
+      <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="C39" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1793,100 +2116,100 @@
         <v>The rotate camera function should take the pivot from the centre of the view, not from the mouse location.</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="str">
+      <c r="A41" s="41" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
       <c r="B41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="C42" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="41"/>
+      <c r="B44" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="C44" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="str">
+      <c r="A45" s="41" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="str">
+      <c r="A47" s="41" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
       <c r="B47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="41"/>
+      <c r="B48" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="10" t="s">
+      <c r="C48" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="44"/>
+      <c r="B49" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="C49" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D49">
         <f>COUNTA(C24:C49)</f>
@@ -1894,274 +2217,274 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="47"/>
+      <c r="C50" s="48"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="str">
+      <c r="A51" s="41" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
       <c r="B51" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="10" t="s">
+      <c r="C52" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="41"/>
+      <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="C53" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="str">
+      <c r="A54" s="41" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
       <c r="B54" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="41"/>
+      <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
-      <c r="B55" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="C55" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="31" t="str">
+      <c r="A56" s="41" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
       <c r="B56" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="41"/>
+      <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
-      <c r="B57" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="C57" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31" t="str">
+      <c r="A58" s="41" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
       <c r="B58" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="41"/>
+      <c r="B59" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="41"/>
+      <c r="B60" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
-      <c r="B59" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
-      <c r="B60" s="10" t="s">
+      <c r="C60" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="41"/>
+      <c r="B61" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="31"/>
-      <c r="B61" s="10" t="s">
+      <c r="C61" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="41"/>
+      <c r="B62" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
-      <c r="B62" s="15" t="s">
-        <v>86</v>
-      </c>
       <c r="C62" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+      <c r="A63" s="41"/>
       <c r="B63" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+      <c r="A64" s="41"/>
       <c r="B64" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="31" t="str">
+      <c r="A65" s="41" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
       <c r="B65" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="41"/>
+      <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="6"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
-      <c r="B66" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="C66" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="31" t="str">
+      <c r="A67" s="41" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="41"/>
+      <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C67" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
-      <c r="B68" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="C68" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="31" t="str">
+      <c r="A69" s="41" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="41"/>
+      <c r="B70" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
-      <c r="B70" s="18" t="s">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="41"/>
+      <c r="B71" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="6"/>
-    </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
-      <c r="B71" s="18" t="s">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="41"/>
+      <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
-      <c r="B72" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C72" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="31" t="str">
+      <c r="A73" s="41" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="41"/>
+      <c r="B74" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
-      <c r="B74" s="19" t="s">
-        <v>97</v>
-      </c>
       <c r="C74" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="str">
+      <c r="A75" s="41" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
       <c r="B75" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="41"/>
+      <c r="B76" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="31"/>
-      <c r="B76" s="19" t="s">
+      <c r="C76" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="44"/>
+      <c r="B77" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
-      <c r="B77" s="20" t="s">
-        <v>104</v>
-      </c>
       <c r="C77" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D77">
         <f>COUNTA(C51:C77)</f>
@@ -2169,305 +2492,305 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="35"/>
+      <c r="A78" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="43"/>
+      <c r="C78" s="45"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="str">
+      <c r="A79" s="41" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="41"/>
+      <c r="B80" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
-      <c r="B80" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="C80" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="str">
+      <c r="A81" s="41" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
+      <c r="A82" s="41"/>
       <c r="B82" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="str">
+      <c r="A83" s="41" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
       <c r="B83" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="41"/>
+      <c r="B84" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C83" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
-      <c r="B84" s="9" t="s">
+      <c r="C84" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="41"/>
+      <c r="B85" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C84" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
-      <c r="B85" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="31" t="str">
+      <c r="A86" s="41" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
       <c r="B86" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="41"/>
+      <c r="B87" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="31"/>
-      <c r="B87" s="9" t="s">
+      <c r="C87" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="41"/>
+      <c r="B88" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
-      <c r="B88" s="9" t="s">
+      <c r="C88" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="41"/>
+      <c r="B89" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="31"/>
-      <c r="B89" s="9" t="s">
+      <c r="C89" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="41"/>
+      <c r="B90" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C89" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="31"/>
-      <c r="B90" s="9" t="s">
+      <c r="C90" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="41"/>
+      <c r="B91" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
-      <c r="B91" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="C91" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="31" t="str">
+      <c r="A92" s="41" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
       <c r="B92" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="41"/>
+      <c r="B93" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
-      <c r="B93" s="9" t="s">
+      <c r="C93" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="41"/>
+      <c r="B94" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="31"/>
-      <c r="B94" s="9" t="s">
+      <c r="C94" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="41"/>
+      <c r="B95" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="31"/>
-      <c r="B95" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="C95" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="31" t="str">
+      <c r="A96" s="41" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="41"/>
       <c r="B97" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="41"/>
+      <c r="B98" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C97" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
-      <c r="B98" s="9" t="s">
-        <v>135</v>
-      </c>
       <c r="C98" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31" t="str">
+      <c r="A99" s="41" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
       <c r="B99" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="41"/>
+      <c r="B100" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="41"/>
+      <c r="B101" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C99" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="31"/>
-      <c r="B100" s="9" t="s">
+      <c r="C101" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="41"/>
+      <c r="B102" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C100" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="31"/>
-      <c r="B101" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
-      <c r="B102" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="C102" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
+      <c r="A103" s="41"/>
       <c r="B103" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="31" t="str">
+      <c r="A104" s="41" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
       <c r="B104" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="41"/>
+      <c r="B105" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C104" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
-      <c r="B105" s="9" t="s">
+      <c r="C105" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="41"/>
+      <c r="B106" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
-      <c r="B106" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="C106" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="31" t="str">
+      <c r="A107" s="41" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
       <c r="B107" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="41"/>
+      <c r="B108" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
-      <c r="B108" s="9" t="s">
-        <v>144</v>
-      </c>
       <c r="C108" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2476,10 +2799,10 @@
         <v>I want curved sections of track to save and load properly.</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D109">
         <f>COUNTA(C79:C109)</f>
@@ -2487,247 +2810,247 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
+      <c r="A110" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="B110" s="42"/>
+      <c r="C110" s="42"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="str">
+      <c r="A111" s="40" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
       <c r="B111" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="41"/>
+      <c r="B112" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="41"/>
+      <c r="B113" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C111" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="31"/>
-      <c r="B112" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
-      <c r="B113" s="9" t="s">
-        <v>155</v>
-      </c>
       <c r="C113" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="31"/>
+      <c r="A114" s="41"/>
       <c r="B114" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="41"/>
+      <c r="B115" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C114" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="31"/>
-      <c r="B115" s="9" t="s">
-        <v>159</v>
-      </c>
       <c r="C115" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="31" t="str">
+      <c r="A116" s="41" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
       <c r="B116" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="41"/>
+      <c r="B117" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C116" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
-      <c r="B117" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="C117" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="31" t="str">
+      <c r="A118" s="41" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
       <c r="B118" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="41"/>
+      <c r="B119" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C118" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
-      <c r="B119" s="9" t="s">
-        <v>161</v>
-      </c>
       <c r="C119" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="31"/>
+      <c r="A120" s="41"/>
       <c r="B120" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="31" t="str">
+      <c r="A121" s="41" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
       <c r="B121" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="41"/>
+      <c r="B122" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="41"/>
+      <c r="B123" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C121" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
-      <c r="B122" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="31"/>
-      <c r="B123" s="9" t="s">
+      <c r="C123" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="41"/>
+      <c r="B124" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C123" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="31"/>
-      <c r="B124" s="9" t="s">
-        <v>177</v>
-      </c>
       <c r="C124" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="31" t="str">
+      <c r="A125" s="41" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="41"/>
+      <c r="B126" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C125" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="31"/>
-      <c r="B126" s="9" t="s">
+      <c r="C126" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="41"/>
+      <c r="B127" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C126" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="31"/>
-      <c r="B127" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="C127" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="31" t="str">
+      <c r="A128" s="41" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="41"/>
+      <c r="B129" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C128" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="31"/>
-      <c r="B129" s="9" t="s">
+      <c r="C129" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="41"/>
+      <c r="B130" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C129" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="31"/>
-      <c r="B130" s="9" t="s">
-        <v>169</v>
-      </c>
       <c r="C130" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="31"/>
+      <c r="A131" s="41"/>
       <c r="B131" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="31" t="str">
+      <c r="A132" s="41" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="41"/>
+      <c r="B133" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="44"/>
+      <c r="B134" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C132" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="31"/>
-      <c r="B133" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
-      <c r="B134" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="C134" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D134">
         <f>COUNTA(C111:C134)</f>
@@ -2735,221 +3058,221 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="B135" s="33"/>
-      <c r="C135" s="33"/>
+      <c r="A135" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B135" s="43"/>
+      <c r="C135" s="43"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="30" t="str">
+      <c r="A136" s="40" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
       <c r="B136" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C136" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="41"/>
+      <c r="B137" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C136" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="31"/>
-      <c r="B137" s="9" t="s">
+      <c r="C137" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="41"/>
+      <c r="B138" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="41"/>
+      <c r="B139" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C137" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
-      <c r="B138" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="31"/>
-      <c r="B139" s="9" t="s">
+      <c r="C139" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="41"/>
+      <c r="B140" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="31"/>
-      <c r="B140" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="C140" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="31" t="str">
+      <c r="A141" s="41" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
       <c r="B141" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="41"/>
+      <c r="B142" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C141" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="31"/>
-      <c r="B142" s="9" t="s">
+      <c r="C142" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="41"/>
+      <c r="B143" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C142" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="31"/>
-      <c r="B143" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="C143" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="31" t="str">
+      <c r="A144" s="41" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
       <c r="B144" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="41"/>
+      <c r="B145" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C144" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="31"/>
-      <c r="B145" s="9" t="s">
+      <c r="C145" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="41"/>
+      <c r="B146" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="41"/>
+      <c r="B147" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C145" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="31"/>
-      <c r="B146" s="9" t="s">
+      <c r="C147" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="41"/>
+      <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C146" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="31"/>
-      <c r="B147" s="9" t="s">
+      <c r="C148" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="41"/>
+      <c r="B149" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C147" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="31"/>
-      <c r="B148" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="31"/>
-      <c r="B149" s="9" t="s">
-        <v>206</v>
-      </c>
       <c r="C149" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="31" t="str">
+      <c r="A150" s="41" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
       <c r="B150" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="41"/>
+      <c r="B151" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="41"/>
+      <c r="B152" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="C150" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="31"/>
-      <c r="B151" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="31"/>
-      <c r="B152" s="16" t="s">
-        <v>193</v>
-      </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="31" t="str">
+      <c r="A153" s="41" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
       <c r="B153" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="41"/>
+      <c r="B154" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C153" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="31"/>
-      <c r="B154" s="9" t="s">
-        <v>197</v>
-      </c>
       <c r="C154" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="31"/>
+      <c r="A155" s="41"/>
       <c r="B155" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="41"/>
+      <c r="B156" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C155" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="31"/>
-      <c r="B156" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="C156" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="31"/>
+      <c r="A157" s="41"/>
       <c r="B157" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2958,10 +3281,10 @@
         <v>Finalising a track section should not be so slow if it doesn't need to adjust the terrain.</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D158">
         <f>COUNTA(C136:C158)</f>
@@ -2969,493 +3292,535 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="B159" s="33"/>
-      <c r="C159" s="33"/>
+      <c r="A159" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B159" s="43"/>
+      <c r="C159" s="43"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="30" t="str">
+      <c r="A160" s="40" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
       <c r="B160" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C160" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="41"/>
+      <c r="B161" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C161" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="41"/>
+      <c r="B162" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="41"/>
+      <c r="B163" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C163" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="41"/>
+      <c r="B164" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C160" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="31"/>
-      <c r="B161" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C161" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="31"/>
-      <c r="B162" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="C162" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="31"/>
-      <c r="B163" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C163" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="31"/>
-      <c r="B164" s="9" t="s">
-        <v>220</v>
-      </c>
       <c r="C164" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="31" t="str">
+      <c r="A165" s="41" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="31"/>
+      <c r="A166" s="41"/>
       <c r="B166" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="31"/>
+      <c r="A167" s="41"/>
       <c r="B167" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C167" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="41"/>
+      <c r="B168" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C167" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="31"/>
-      <c r="B168" s="9" t="s">
-        <v>224</v>
-      </c>
       <c r="C168" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="31" t="str">
+      <c r="A169" s="41" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="31"/>
+      <c r="A170" s="41"/>
       <c r="B170" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="31"/>
+      <c r="A171" s="41"/>
       <c r="B171" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="31"/>
+      <c r="A172" s="41"/>
       <c r="B172" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="31"/>
+      <c r="A173" s="41"/>
       <c r="B173" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="31" t="str">
+      <c r="A174" s="41" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="31"/>
+      <c r="A175" s="41"/>
       <c r="B175" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="31"/>
+      <c r="A176" s="41"/>
       <c r="B176" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="31"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A177" s="41"/>
       <c r="B177" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="41" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
       <c r="B178" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="41"/>
+      <c r="B179" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="C178" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="31"/>
-      <c r="B179" s="9" t="s">
-        <v>246</v>
-      </c>
       <c r="C179" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="31"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="41"/>
       <c r="B180" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="41"/>
+      <c r="B181" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C180" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="31"/>
-      <c r="B181" s="9" t="s">
+      <c r="C181" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="41"/>
+      <c r="B182" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C181" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="31"/>
-      <c r="B182" s="9" t="s">
-        <v>237</v>
-      </c>
       <c r="C182" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="41" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
       <c r="B183" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="41"/>
+      <c r="B184" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="C183" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="31"/>
-      <c r="B184" s="9" t="s">
+      <c r="C184" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="41"/>
+      <c r="B185" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C184" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="31"/>
-      <c r="B185" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="C185" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="31" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="41" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
       <c r="B186" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="41"/>
+      <c r="B187" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="41"/>
+      <c r="B188" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C186" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="31"/>
-      <c r="B187" s="9" t="s">
+      <c r="C188" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="41"/>
+      <c r="B189" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C187" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="31"/>
-      <c r="B188" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="C188" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="34"/>
-      <c r="B189" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>24</v>
+      <c r="C189" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D189">
         <f>COUNTA(C160:C189)</f>
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="B190" s="32"/>
-      <c r="C190" s="32"/>
-    </row>
-    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="B190" s="54"/>
+      <c r="C190" s="55"/>
+      <c r="D190">
+        <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"R","")))</f>
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"C","")))</f>
+        <v>11</v>
+      </c>
+      <c r="G190">
+        <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"P","")))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="str">
         <f>'S 8'!A1</f>
         <v>I want to be able to create large curved sections without the colliders bugging out.</v>
       </c>
-      <c r="B191" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="str">
+      <c r="B191" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C191" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="29" t="str">
         <f>'S 8'!A2</f>
         <v>I want a way to remove a locomotive from the world.</v>
       </c>
-      <c r="B192" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="C192" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="32" t="str">
+      <c r="B192" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C192" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="51" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
-      <c r="B193" s="9" t="s">
+      <c r="B193" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C193" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="51"/>
+      <c r="B194" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C193" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="32"/>
-      <c r="B194" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C194" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="32"/>
-      <c r="B195" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C195" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="32"/>
-      <c r="B196" s="9" t="s">
+      <c r="C194" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="51"/>
+      <c r="B195" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C195" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="51"/>
+      <c r="B196" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="C196" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="51"/>
+      <c r="B197" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="C196" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="32"/>
-      <c r="B197" s="9" t="s">
+      <c r="C197" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="51"/>
+      <c r="B198" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="C197" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="32"/>
-      <c r="B198" s="9" t="s">
+      <c r="C198" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="51"/>
+      <c r="B199" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="C198" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="32"/>
-      <c r="B199" s="9" t="s">
+      <c r="C199" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="D199" s="34"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="51"/>
+      <c r="B200" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="C199" s="8"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="32"/>
-      <c r="B200" s="9" t="s">
+      <c r="C200" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="51"/>
+      <c r="B201" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="C200" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="32"/>
-      <c r="B201" s="9" t="s">
+      <c r="C201" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="51"/>
+      <c r="B202" s="28" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="32"/>
-      <c r="B202" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="32" t="str">
+      <c r="C202" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="51" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
-      <c r="B203" s="9" t="s">
+      <c r="B203" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="C203" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="51"/>
+      <c r="B204" s="28" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="32"/>
-      <c r="B204" s="9" t="s">
+      <c r="C204" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="51"/>
+      <c r="B205" s="28" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="32"/>
-      <c r="B205" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="32" t="str">
+      <c r="C205" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="51" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
-      <c r="B206" s="9" t="s">
+      <c r="B206" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="C206" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="51"/>
+      <c r="B207" s="28" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="32"/>
-      <c r="B207" s="9" t="s">
+      <c r="C207" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="51"/>
+      <c r="B208" s="28" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="32"/>
-      <c r="B208" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="32" t="str">
+      <c r="C208" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="51" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
-      <c r="B209" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C209" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="32"/>
-      <c r="B210" s="9" t="s">
+      <c r="B209" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="C210" t="s">
-        <v>24</v>
-      </c>
-      <c r="D210">
-        <f>COUNTA(C191:C210)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="28"/>
+      <c r="C209" s="31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="52"/>
+      <c r="B210" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C210" s="33" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B211" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="63">
     <mergeCell ref="A206:A208"/>
     <mergeCell ref="A209:A210"/>
     <mergeCell ref="A190:C190"/>
@@ -3483,6 +3848,12 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A56:A57"/>
     <mergeCell ref="A58:A64"/>
     <mergeCell ref="A50:C50"/>
@@ -3492,16 +3863,12 @@
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A69:A72"/>
     <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A150:A152"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A83:A85"/>
     <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A211:B211"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A92:A95"/>
@@ -3517,8 +3884,35 @@
     <mergeCell ref="A121:A124"/>
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A150:A152"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B210 B212:B1048576">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>C1="P"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>C1="R"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>C1="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>C1="C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3526,10 +3920,68 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.85546875" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3539,17 +3991,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -3600,7 +4047,7 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3623,47 +4070,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3686,47 +4133,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3749,52 +4196,52 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3817,37 +4264,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3870,32 +4317,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3918,37 +4365,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3961,7 +4408,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3971,32 +4418,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User stories and task list updated for iteration 9
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="319">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -888,6 +888,99 @@
   </si>
   <si>
     <t>I want a bauble to retain its curvature after saving and reloading a map.</t>
+  </si>
+  <si>
+    <t>Bauble must supply a list of track section refs with 'other end' positions</t>
+  </si>
+  <si>
+    <t>Cursor should be dragged outside bauble hitbox for track to be selected; else select most recent</t>
+  </si>
+  <si>
+    <t>Shape controller must track its own error state</t>
+  </si>
+  <si>
+    <t>Placement tool must check for error state in shape before placing bauble</t>
+  </si>
+  <si>
+    <t>Shape controller must control highlighting based on error state</t>
+  </si>
+  <si>
+    <t>Approximate single transition out with distance == start-&gt;bauble</t>
+  </si>
+  <si>
+    <t>Shape controller should approximate shape after error without adjusting bauble, including:  Approximate fixed endpoint as free</t>
+  </si>
+  <si>
+    <t>Remove requirement for track section to be straight before splitting</t>
+  </si>
+  <si>
+    <t>A track section should be able to be initialised as a clone</t>
+  </si>
+  <si>
+    <t>A track section should be able to be cut off by a bauble; this will reduce the length of the section to bauble's position and attach bauble to end</t>
+  </si>
+  <si>
+    <t>Placement tool should clone section, create new bauble, then cut original and clone either side of bauble</t>
+  </si>
+  <si>
+    <t>I want bauble curvature to be the correct direction regardless which side the track connects to</t>
+  </si>
+  <si>
+    <t>Bauble curve accessed via function which checks track section direction</t>
+  </si>
+  <si>
+    <t>Change access to new function, check bugs and reverse signs where needed</t>
+  </si>
+  <si>
+    <t>Placement tool should move current bauble to closest straight line position to cursor under correct conditions</t>
+  </si>
+  <si>
+    <t>VertexBender should have a provision for fixed-radius curves</t>
+  </si>
+  <si>
+    <t>Branch for Story</t>
+  </si>
+  <si>
+    <t>Shape parameters should indicate if fixed curve, and what length/radius</t>
+  </si>
+  <si>
+    <t>Shape controller use alternate VertexBender function for fix-radius curves</t>
+  </si>
+  <si>
+    <t>Placement tool should move current bauble to closest circle position to cursor under correct conditions, and tell shape controller of fixed radius</t>
+  </si>
+  <si>
+    <t>Do math for Fixed/Radius -&gt; Rotate/Radius</t>
+  </si>
+  <si>
+    <t>Rename FresnelMath Numeric Analysis functions properly</t>
+  </si>
+  <si>
+    <t>Put math into Numeric Analysys function and test it</t>
+  </si>
+  <si>
+    <t>Add rotate/radius -&gt; fixed/radius to shape controller</t>
+  </si>
+  <si>
+    <t>Add fixed/radius -&gt; rotate/radius to shape controller</t>
+  </si>
+  <si>
+    <t>Add 'switch' button to track submenu</t>
+  </si>
+  <si>
+    <t>Create a switch object, and allow it to be placed on baubles with &gt;2 sections</t>
+  </si>
+  <si>
+    <t>Switch object should use TrackLights model to indicate presence</t>
+  </si>
+  <si>
+    <t>Bauble should refer to switch when making decisions for train movement</t>
+  </si>
+  <si>
+    <t>Switch should have two switching vars, one for each direction.  Must know how many tracks branch each way, and provide n switch positions</t>
+  </si>
+  <si>
+    <t>Deadline</t>
   </si>
 </sst>
 </file>
@@ -917,7 +1010,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -948,8 +1041,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1181,20 +1286,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1274,42 +1370,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,11 +1385,111 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D6FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD961"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D6FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD961"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1693,12 +1853,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G211"/>
+  <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A187" activePane="bottomLeft"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A211" sqref="A211:B211"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="615" topLeftCell="A210" activePane="bottomLeft"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,9 +1870,10 @@
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1734,16 +1895,19 @@
       <c r="G1" s="38" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="H1" s="55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="str">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1754,8 +1918,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1763,8 +1927,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1772,8 +1936,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="str">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1784,8 +1948,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1793,8 +1957,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1802,8 +1966,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1811,8 +1975,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1820,8 +1984,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1829,8 +1993,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="str">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1841,8 +2005,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1850,8 +2014,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1859,8 +2023,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="str">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -1871,8 +2035,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1881,7 +2045,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -1890,7 +2054,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1899,7 +2063,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="str">
+      <c r="A19" s="44" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -1911,7 +2075,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +2084,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="str">
+      <c r="A21" s="44" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -1932,7 +2096,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1945,11 +2109,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="45"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="49"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -1964,7 +2128,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="str">
+      <c r="A25" s="44" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -1976,7 +2140,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
@@ -1985,7 +2149,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="str">
+      <c r="A27" s="44" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -1997,7 +2161,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -2006,7 +2170,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
@@ -2015,7 +2179,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="10" t="s">
         <v>65</v>
       </c>
@@ -2024,7 +2188,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
@@ -2033,7 +2197,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
@@ -2042,7 +2206,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -2051,7 +2215,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="str">
+      <c r="A34" s="44" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -2063,7 +2227,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="10" t="s">
         <v>49</v>
       </c>
@@ -2072,7 +2236,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
@@ -2081,7 +2245,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
@@ -2090,7 +2254,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="41" t="str">
+      <c r="A38" s="44" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -2102,7 +2266,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
@@ -2123,7 +2287,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41" t="str">
+      <c r="A41" s="44" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -2135,7 +2299,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
@@ -2144,7 +2308,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="10" t="s">
         <v>57</v>
       </c>
@@ -2153,7 +2317,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="10" t="s">
         <v>58</v>
       </c>
@@ -2162,7 +2326,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="str">
+      <c r="A45" s="44" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -2174,7 +2338,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="10" t="s">
         <v>61</v>
       </c>
@@ -2183,7 +2347,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="41" t="str">
+      <c r="A47" s="44" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -2195,7 +2359,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="41"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="10" t="s">
         <v>63</v>
       </c>
@@ -2204,7 +2368,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="13" t="s">
         <v>64</v>
       </c>
@@ -2217,14 +2381,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="48"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="53"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="41" t="str">
+      <c r="A51" s="44" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -2236,7 +2400,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="41"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
@@ -2245,7 +2409,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
@@ -2254,7 +2418,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="41" t="str">
+      <c r="A54" s="44" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -2266,7 +2430,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
@@ -2275,7 +2439,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="41" t="str">
+      <c r="A56" s="44" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -2287,7 +2451,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="41"/>
+      <c r="A57" s="44"/>
       <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
@@ -2296,7 +2460,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="41" t="str">
+      <c r="A58" s="44" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -2308,7 +2472,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="41"/>
+      <c r="A59" s="44"/>
       <c r="B59" s="9" t="s">
         <v>98</v>
       </c>
@@ -2317,7 +2481,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="41"/>
+      <c r="A60" s="44"/>
       <c r="B60" s="10" t="s">
         <v>83</v>
       </c>
@@ -2326,7 +2490,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
+      <c r="A61" s="44"/>
       <c r="B61" s="10" t="s">
         <v>84</v>
       </c>
@@ -2335,7 +2499,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="15" t="s">
         <v>85</v>
       </c>
@@ -2344,7 +2508,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="41"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="9" t="s">
         <v>104</v>
       </c>
@@ -2353,7 +2517,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="41"/>
+      <c r="A64" s="44"/>
       <c r="B64" s="10" t="s">
         <v>90</v>
       </c>
@@ -2362,7 +2526,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="str">
+      <c r="A65" s="44" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -2372,7 +2536,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
+      <c r="A66" s="44"/>
       <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
@@ -2381,7 +2545,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41" t="str">
+      <c r="A67" s="44" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -2393,7 +2557,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="41"/>
+      <c r="A68" s="44"/>
       <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
@@ -2402,7 +2566,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="41" t="str">
+      <c r="A69" s="44" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2414,21 +2578,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
+      <c r="A70" s="44"/>
       <c r="B70" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="41"/>
+      <c r="A71" s="44"/>
       <c r="B71" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="41"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
@@ -2437,7 +2601,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="41" t="str">
+      <c r="A73" s="44" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2449,7 +2613,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="41"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="19" t="s">
         <v>96</v>
       </c>
@@ -2458,7 +2622,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="41" t="str">
+      <c r="A75" s="44" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2470,7 +2634,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="41"/>
+      <c r="A76" s="44"/>
       <c r="B76" s="19" t="s">
         <v>102</v>
       </c>
@@ -2479,7 +2643,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
+      <c r="A77" s="50"/>
       <c r="B77" s="20" t="s">
         <v>103</v>
       </c>
@@ -2492,14 +2656,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="40" t="s">
+      <c r="A78" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="43"/>
-      <c r="C78" s="45"/>
+      <c r="B78" s="45"/>
+      <c r="C78" s="49"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="41" t="str">
+      <c r="A79" s="44" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2511,7 +2675,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
+      <c r="A80" s="44"/>
       <c r="B80" s="9" t="s">
         <v>118</v>
       </c>
@@ -2520,7 +2684,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="41" t="str">
+      <c r="A81" s="44" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2532,7 +2696,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="41"/>
+      <c r="A82" s="44"/>
       <c r="B82" s="9" t="s">
         <v>119</v>
       </c>
@@ -2541,7 +2705,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="41" t="str">
+      <c r="A83" s="44" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2553,7 +2717,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="41"/>
+      <c r="A84" s="44"/>
       <c r="B84" s="9" t="s">
         <v>121</v>
       </c>
@@ -2562,14 +2726,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="41"/>
+      <c r="A85" s="44"/>
       <c r="B85" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="41" t="str">
+      <c r="A86" s="44" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2581,7 +2745,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="41"/>
+      <c r="A87" s="44"/>
       <c r="B87" s="9" t="s">
         <v>124</v>
       </c>
@@ -2590,7 +2754,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="41"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="9" t="s">
         <v>125</v>
       </c>
@@ -2599,7 +2763,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="41"/>
+      <c r="A89" s="44"/>
       <c r="B89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2608,7 +2772,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="41"/>
+      <c r="A90" s="44"/>
       <c r="B90" s="9" t="s">
         <v>127</v>
       </c>
@@ -2617,7 +2781,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="41"/>
+      <c r="A91" s="44"/>
       <c r="B91" s="9" t="s">
         <v>128</v>
       </c>
@@ -2626,7 +2790,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="41" t="str">
+      <c r="A92" s="44" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2638,7 +2802,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="41"/>
+      <c r="A93" s="44"/>
       <c r="B93" s="9" t="s">
         <v>130</v>
       </c>
@@ -2647,7 +2811,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="41"/>
+      <c r="A94" s="44"/>
       <c r="B94" s="9" t="s">
         <v>131</v>
       </c>
@@ -2656,7 +2820,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="41"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="9" t="s">
         <v>132</v>
       </c>
@@ -2665,7 +2829,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="41" t="str">
+      <c r="A96" s="44" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2677,7 +2841,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="41"/>
+      <c r="A97" s="44"/>
       <c r="B97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2686,7 +2850,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="41"/>
+      <c r="A98" s="44"/>
       <c r="B98" s="9" t="s">
         <v>134</v>
       </c>
@@ -2695,7 +2859,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="41" t="str">
+      <c r="A99" s="44" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2707,7 +2871,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="41"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="9" t="s">
         <v>137</v>
       </c>
@@ -2716,7 +2880,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="41"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="9" t="s">
         <v>136</v>
       </c>
@@ -2725,7 +2889,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="41"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="9" t="s">
         <v>138</v>
       </c>
@@ -2734,7 +2898,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="41"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="9" t="s">
         <v>146</v>
       </c>
@@ -2743,7 +2907,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="41" t="str">
+      <c r="A104" s="44" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2755,7 +2919,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="41"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="9" t="s">
         <v>140</v>
       </c>
@@ -2764,7 +2928,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="41"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="9" t="s">
         <v>141</v>
       </c>
@@ -2773,7 +2937,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="41" t="str">
+      <c r="A107" s="44" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2785,7 +2949,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="41"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="9" t="s">
         <v>143</v>
       </c>
@@ -2810,14 +2974,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="42" t="s">
+      <c r="A110" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="42"/>
-      <c r="C110" s="42"/>
+      <c r="B110" s="54"/>
+      <c r="C110" s="54"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="40" t="str">
+      <c r="A111" s="46" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2829,7 +2993,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="41"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="9" t="s">
         <v>170</v>
       </c>
@@ -2838,7 +3002,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="41"/>
+      <c r="A113" s="44"/>
       <c r="B113" s="9" t="s">
         <v>154</v>
       </c>
@@ -2847,7 +3011,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="41"/>
+      <c r="A114" s="44"/>
       <c r="B114" s="9" t="s">
         <v>157</v>
       </c>
@@ -2856,7 +3020,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="41"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="9" t="s">
         <v>158</v>
       </c>
@@ -2865,7 +3029,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="41" t="str">
+      <c r="A116" s="44" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -2877,7 +3041,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="41"/>
+      <c r="A117" s="44"/>
       <c r="B117" s="9" t="s">
         <v>156</v>
       </c>
@@ -2886,7 +3050,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="41" t="str">
+      <c r="A118" s="44" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -2898,7 +3062,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="41"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="9" t="s">
         <v>160</v>
       </c>
@@ -2907,7 +3071,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="41"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="9" t="s">
         <v>171</v>
       </c>
@@ -2916,7 +3080,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="41" t="str">
+      <c r="A121" s="44" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -2928,7 +3092,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="41"/>
+      <c r="A122" s="44"/>
       <c r="B122" s="24" t="s">
         <v>161</v>
       </c>
@@ -2937,7 +3101,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="41"/>
+      <c r="A123" s="44"/>
       <c r="B123" s="9" t="s">
         <v>175</v>
       </c>
@@ -2946,7 +3110,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="41"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="9" t="s">
         <v>176</v>
       </c>
@@ -2955,7 +3119,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="41" t="str">
+      <c r="A125" s="44" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -2967,7 +3131,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="41"/>
+      <c r="A126" s="44"/>
       <c r="B126" s="9" t="s">
         <v>164</v>
       </c>
@@ -2976,7 +3140,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="41"/>
+      <c r="A127" s="44"/>
       <c r="B127" s="9" t="s">
         <v>165</v>
       </c>
@@ -2985,7 +3149,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="41" t="str">
+      <c r="A128" s="44" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -2997,7 +3161,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="41"/>
+      <c r="A129" s="44"/>
       <c r="B129" s="9" t="s">
         <v>167</v>
       </c>
@@ -3006,7 +3170,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="41"/>
+      <c r="A130" s="44"/>
       <c r="B130" s="9" t="s">
         <v>168</v>
       </c>
@@ -3015,7 +3179,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="41"/>
+      <c r="A131" s="44"/>
       <c r="B131" s="9" t="s">
         <v>177</v>
       </c>
@@ -3024,7 +3188,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="41" t="str">
+      <c r="A132" s="44" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -3036,7 +3200,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="41"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="9" t="s">
         <v>169</v>
       </c>
@@ -3045,7 +3209,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="44"/>
+      <c r="A134" s="50"/>
       <c r="B134" s="22" t="s">
         <v>179</v>
       </c>
@@ -3058,14 +3222,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="43" t="s">
+      <c r="A135" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="43"/>
-      <c r="C135" s="43"/>
+      <c r="B135" s="45"/>
+      <c r="C135" s="45"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="40" t="str">
+      <c r="A136" s="46" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -3077,7 +3241,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="41"/>
+      <c r="A137" s="44"/>
       <c r="B137" s="9" t="s">
         <v>185</v>
       </c>
@@ -3086,7 +3250,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="41"/>
+      <c r="A138" s="44"/>
       <c r="B138" s="9" t="s">
         <v>199</v>
       </c>
@@ -3095,7 +3259,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="41"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="9" t="s">
         <v>186</v>
       </c>
@@ -3104,7 +3268,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="41"/>
+      <c r="A140" s="44"/>
       <c r="B140" s="9" t="s">
         <v>187</v>
       </c>
@@ -3113,7 +3277,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="41" t="str">
+      <c r="A141" s="44" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -3125,7 +3289,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="41"/>
+      <c r="A142" s="44"/>
       <c r="B142" s="9" t="s">
         <v>189</v>
       </c>
@@ -3134,7 +3298,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="41"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="9" t="s">
         <v>190</v>
       </c>
@@ -3143,7 +3307,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="41" t="str">
+      <c r="A144" s="44" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -3155,7 +3319,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="41"/>
+      <c r="A145" s="44"/>
       <c r="B145" s="9" t="s">
         <v>203</v>
       </c>
@@ -3164,7 +3328,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="41"/>
+      <c r="A146" s="44"/>
       <c r="B146" s="9" t="s">
         <v>206</v>
       </c>
@@ -3173,7 +3337,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="41"/>
+      <c r="A147" s="44"/>
       <c r="B147" s="9" t="s">
         <v>204</v>
       </c>
@@ -3182,7 +3346,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="41"/>
+      <c r="A148" s="44"/>
       <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
@@ -3191,7 +3355,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="41"/>
+      <c r="A149" s="44"/>
       <c r="B149" s="9" t="s">
         <v>205</v>
       </c>
@@ -3200,7 +3364,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="41" t="str">
+      <c r="A150" s="44" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -3212,7 +3376,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="41"/>
+      <c r="A151" s="44"/>
       <c r="B151" s="24" t="s">
         <v>208</v>
       </c>
@@ -3221,14 +3385,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="41"/>
+      <c r="A152" s="44"/>
       <c r="B152" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="41" t="str">
+      <c r="A153" s="44" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -3240,7 +3404,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="41"/>
+      <c r="A154" s="44"/>
       <c r="B154" s="9" t="s">
         <v>196</v>
       </c>
@@ -3249,7 +3413,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="41"/>
+      <c r="A155" s="44"/>
       <c r="B155" s="9" t="s">
         <v>193</v>
       </c>
@@ -3258,7 +3422,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="41"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="9" t="s">
         <v>194</v>
       </c>
@@ -3267,7 +3431,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="41"/>
+      <c r="A157" s="44"/>
       <c r="B157" s="9" t="s">
         <v>211</v>
       </c>
@@ -3292,14 +3456,14 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="43" t="s">
+      <c r="A159" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="B159" s="43"/>
-      <c r="C159" s="43"/>
+      <c r="B159" s="45"/>
+      <c r="C159" s="45"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="40" t="str">
+      <c r="A160" s="46" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3311,7 +3475,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="41"/>
+      <c r="A161" s="44"/>
       <c r="B161" s="9" t="s">
         <v>226</v>
       </c>
@@ -3320,7 +3484,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="41"/>
+      <c r="A162" s="44"/>
       <c r="B162" s="9" t="s">
         <v>242</v>
       </c>
@@ -3329,7 +3493,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="41"/>
+      <c r="A163" s="44"/>
       <c r="B163" s="9" t="s">
         <v>221</v>
       </c>
@@ -3338,7 +3502,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="41"/>
+      <c r="A164" s="44"/>
       <c r="B164" s="9" t="s">
         <v>219</v>
       </c>
@@ -3347,7 +3511,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="41" t="str">
+      <c r="A165" s="44" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -3359,7 +3523,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="41"/>
+      <c r="A166" s="44"/>
       <c r="B166" s="9" t="s">
         <v>228</v>
       </c>
@@ -3368,7 +3532,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="41"/>
+      <c r="A167" s="44"/>
       <c r="B167" s="9" t="s">
         <v>222</v>
       </c>
@@ -3377,7 +3541,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="41"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="9" t="s">
         <v>223</v>
       </c>
@@ -3386,7 +3550,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="41" t="str">
+      <c r="A169" s="44" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -3398,7 +3562,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="41"/>
+      <c r="A170" s="44"/>
       <c r="B170" s="9" t="s">
         <v>224</v>
       </c>
@@ -3407,14 +3571,14 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="41"/>
+      <c r="A171" s="44"/>
       <c r="B171" s="16" t="s">
         <v>241</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="41"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="9" t="s">
         <v>243</v>
       </c>
@@ -3423,7 +3587,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="41"/>
+      <c r="A173" s="44"/>
       <c r="B173" s="9" t="s">
         <v>230</v>
       </c>
@@ -3432,7 +3596,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="41" t="str">
+      <c r="A174" s="44" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3444,7 +3608,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="41"/>
+      <c r="A175" s="44"/>
       <c r="B175" s="9" t="s">
         <v>232</v>
       </c>
@@ -3453,7 +3617,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="41"/>
+      <c r="A176" s="44"/>
       <c r="B176" s="9" t="s">
         <v>229</v>
       </c>
@@ -3462,7 +3626,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="41"/>
+      <c r="A177" s="44"/>
       <c r="B177" s="9" t="s">
         <v>231</v>
       </c>
@@ -3471,7 +3635,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="41" t="str">
+      <c r="A178" s="44" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3483,7 +3647,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="41"/>
+      <c r="A179" s="44"/>
       <c r="B179" s="9" t="s">
         <v>245</v>
       </c>
@@ -3492,7 +3656,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="41"/>
+      <c r="A180" s="44"/>
       <c r="B180" s="9" t="s">
         <v>234</v>
       </c>
@@ -3501,7 +3665,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="41"/>
+      <c r="A181" s="44"/>
       <c r="B181" s="9" t="s">
         <v>235</v>
       </c>
@@ -3510,7 +3674,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="41"/>
+      <c r="A182" s="44"/>
       <c r="B182" s="9" t="s">
         <v>236</v>
       </c>
@@ -3519,7 +3683,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="41" t="str">
+      <c r="A183" s="44" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
@@ -3531,7 +3695,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="41"/>
+      <c r="A184" s="44"/>
       <c r="B184" s="9" t="s">
         <v>248</v>
       </c>
@@ -3540,7 +3704,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="41"/>
+      <c r="A185" s="44"/>
       <c r="B185" s="9" t="s">
         <v>249</v>
       </c>
@@ -3549,7 +3713,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="41" t="str">
+      <c r="A186" s="44" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
@@ -3561,7 +3725,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="41"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="9" t="s">
         <v>237</v>
       </c>
@@ -3570,7 +3734,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="41"/>
+      <c r="A188" s="44"/>
       <c r="B188" s="9" t="s">
         <v>240</v>
       </c>
@@ -3579,7 +3743,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="41"/>
+      <c r="A189" s="44"/>
       <c r="B189" s="9" t="s">
         <v>238</v>
       </c>
@@ -3592,11 +3756,11 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="53" t="s">
+      <c r="A190" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="B190" s="54"/>
-      <c r="C190" s="55"/>
+      <c r="B190" s="42"/>
+      <c r="C190" s="43"/>
       <c r="D190">
         <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
         <v>0</v>
@@ -3639,7 +3803,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="51" t="str">
+      <c r="A193" s="39" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3651,7 +3815,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="51"/>
+      <c r="A194" s="39"/>
       <c r="B194" s="28" t="s">
         <v>257</v>
       </c>
@@ -3660,7 +3824,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="51"/>
+      <c r="A195" s="39"/>
       <c r="B195" s="28" t="s">
         <v>259</v>
       </c>
@@ -3669,7 +3833,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="51"/>
+      <c r="A196" s="39"/>
       <c r="B196" s="28" t="s">
         <v>268</v>
       </c>
@@ -3678,7 +3842,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="51"/>
+      <c r="A197" s="39"/>
       <c r="B197" s="28" t="s">
         <v>269</v>
       </c>
@@ -3687,7 +3851,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="51"/>
+      <c r="A198" s="39"/>
       <c r="B198" s="28" t="s">
         <v>270</v>
       </c>
@@ -3696,7 +3860,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="51"/>
+      <c r="A199" s="39"/>
       <c r="B199" s="28" t="s">
         <v>271</v>
       </c>
@@ -3706,7 +3870,7 @@
       <c r="D199" s="34"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="51"/>
+      <c r="A200" s="39"/>
       <c r="B200" s="28" t="s">
         <v>272</v>
       </c>
@@ -3715,7 +3879,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="51"/>
+      <c r="A201" s="39"/>
       <c r="B201" s="28" t="s">
         <v>273</v>
       </c>
@@ -3724,7 +3888,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="51"/>
+      <c r="A202" s="39"/>
       <c r="B202" s="28" t="s">
         <v>274</v>
       </c>
@@ -3733,7 +3897,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="51" t="str">
+      <c r="A203" s="39" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3745,7 +3909,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="51"/>
+      <c r="A204" s="39"/>
       <c r="B204" s="28" t="s">
         <v>261</v>
       </c>
@@ -3754,7 +3918,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="51"/>
+      <c r="A205" s="39"/>
       <c r="B205" s="28" t="s">
         <v>262</v>
       </c>
@@ -3763,7 +3927,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="51" t="str">
+      <c r="A206" s="39" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3775,7 +3939,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="51"/>
+      <c r="A207" s="39"/>
       <c r="B207" s="28" t="s">
         <v>264</v>
       </c>
@@ -3784,7 +3948,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="51"/>
+      <c r="A208" s="39"/>
       <c r="B208" s="28" t="s">
         <v>265</v>
       </c>
@@ -3792,8 +3956,8 @@
         <v>281</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="51" t="str">
+    <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="39" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3804,8 +3968,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="52"/>
+    <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="40"/>
       <c r="B210" s="32" t="s">
         <v>266</v>
       </c>
@@ -3813,57 +3977,269 @@
         <v>280</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="39" t="s">
+    <row r="211" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="B211" s="39"/>
-    </row>
+      <c r="B211" s="42"/>
+      <c r="C211" s="56"/>
+      <c r="D211">
+        <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"S","")))</f>
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"R","")))</f>
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"C","")))</f>
+        <v>0</v>
+      </c>
+      <c r="G211">
+        <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"P","")))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="57" t="str">
+        <f>'S 9'!A1</f>
+        <v>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</v>
+      </c>
+      <c r="B212" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C212" s="31"/>
+    </row>
+    <row r="213" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="57"/>
+      <c r="B213" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C213" s="31"/>
+    </row>
+    <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="58" t="str">
+        <f>'S 9'!A2</f>
+        <v>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</v>
+      </c>
+      <c r="B214" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C214" s="31"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="58"/>
+      <c r="B215" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="C215" s="31"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="58"/>
+      <c r="B216" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C216" s="31"/>
+    </row>
+    <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" s="58"/>
+      <c r="B217" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C217" s="31"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218" s="58"/>
+      <c r="B218" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="C218" s="31"/>
+    </row>
+    <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="58" t="str">
+        <f>'S 9'!A3</f>
+        <v>I want to be able to create a new bauble partway along curved track.</v>
+      </c>
+      <c r="B219" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="C219" s="31"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="58"/>
+      <c r="B220" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C220" s="31"/>
+    </row>
+    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A221" s="58"/>
+      <c r="B221" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="C221" s="31"/>
+    </row>
+    <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A222" s="58"/>
+      <c r="B222" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="C222" s="31"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223" s="39" t="str">
+        <f>'S 9'!A4</f>
+        <v>I want bauble curvature to be the correct direction regardless which side the track connects to</v>
+      </c>
+      <c r="B223" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C223" s="31"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224" s="39"/>
+      <c r="B224" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C224" s="31"/>
+    </row>
+    <row r="225" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="58" t="str">
+        <f>'S 9'!A5</f>
+        <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
+      </c>
+      <c r="B225" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="C225" s="31"/>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="58"/>
+      <c r="B226" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="C226" s="31"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="58"/>
+      <c r="B227" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="C227" s="31"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="58"/>
+      <c r="B228" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="C228" s="31"/>
+    </row>
+    <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A229" s="58"/>
+      <c r="B229" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C229" s="31"/>
+    </row>
+    <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="39" t="str">
+        <f>'S 9'!A6</f>
+        <v>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</v>
+      </c>
+      <c r="B230" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="C230" s="31"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="39"/>
+      <c r="B231" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C231" s="31"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="39"/>
+      <c r="B232" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="C232" s="31"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="39"/>
+      <c r="B233" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C233" s="31"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="39"/>
+      <c r="B234" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C234" s="31"/>
+    </row>
+    <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="39" t="str">
+        <f>'S 9'!A7</f>
+        <v>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</v>
+      </c>
+      <c r="B235" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="C235" s="31"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="39"/>
+      <c r="B236" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C236" s="31"/>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="39"/>
+      <c r="B237" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="C237" s="31"/>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="39"/>
+      <c r="B238" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="C238" s="31"/>
+    </row>
+    <row r="239" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="40"/>
+      <c r="B239" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="C239" s="33"/>
+      <c r="D239" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="E239" s="60">
+        <v>0.625</v>
+      </c>
+      <c r="F239" s="61">
+        <v>42227</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A150:A152"/>
+  <mergeCells count="70">
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="A214:A218"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A83:A85"/>
@@ -3880,37 +4256,90 @@
     <mergeCell ref="A116:A117"/>
     <mergeCell ref="A118:A120"/>
     <mergeCell ref="A159:C159"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B210 B212:B1048576">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="B1:B210 B230:B1048576 B212:B228">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>C1="P"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>C1="R"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>C1="S"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>C1="C"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"C"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B229">
+    <cfRule type="expression" dxfId="3" priority="14">
+      <formula>C228="P"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="15">
+      <formula>C228="R"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>C228="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>C228="C"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3920,10 +4349,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3948,27 +4377,22 @@
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>210</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>283</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3981,7 +4405,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3996,6 +4420,16 @@
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>285</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bauble controller supplies lists of tracks and end positions.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="319">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -987,7 +987,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1005,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1370,40 +1378,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,53 +1422,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF61D6FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB2DE82"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD961"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6161"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1856,14 +1836,14 @@
   <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A210" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A211" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="C212" sqref="C212"/>
+      <selection pane="bottomLeft" activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.28515625" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -1895,19 +1875,19 @@
       <c r="G1" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="39" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="str">
+      <c r="A3" s="47" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1919,7 +1899,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1928,7 +1908,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1937,7 +1917,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="str">
+      <c r="A6" s="47" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1949,7 +1929,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1958,7 +1938,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1967,7 +1947,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1976,7 +1956,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1985,7 +1965,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1994,7 +1974,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="str">
+      <c r="A12" s="47" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -2006,7 +1986,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -2015,7 +1995,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +2004,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="str">
+      <c r="A15" s="47" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -2036,7 +2016,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -2045,7 +2025,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2034,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -2063,7 +2043,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="str">
+      <c r="A19" s="47" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -2075,7 +2055,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2084,7 +2064,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="str">
+      <c r="A21" s="47" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -2096,7 +2076,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2109,11 +2089,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="49"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -2128,7 +2108,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="str">
+      <c r="A25" s="47" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -2140,7 +2120,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
@@ -2149,7 +2129,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="str">
+      <c r="A27" s="47" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -2161,7 +2141,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -2170,7 +2150,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
@@ -2179,7 +2159,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="10" t="s">
         <v>65</v>
       </c>
@@ -2188,7 +2168,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
@@ -2197,7 +2177,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
@@ -2206,7 +2186,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -2215,7 +2195,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="str">
+      <c r="A34" s="47" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -2227,7 +2207,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="10" t="s">
         <v>49</v>
       </c>
@@ -2236,7 +2216,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
@@ -2245,7 +2225,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
@@ -2254,7 +2234,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="str">
+      <c r="A38" s="47" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -2266,7 +2246,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
@@ -2287,7 +2267,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="str">
+      <c r="A41" s="47" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -2299,7 +2279,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
@@ -2308,7 +2288,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="10" t="s">
         <v>57</v>
       </c>
@@ -2317,7 +2297,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="10" t="s">
         <v>58</v>
       </c>
@@ -2326,7 +2306,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="str">
+      <c r="A45" s="47" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -2338,7 +2318,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="10" t="s">
         <v>61</v>
       </c>
@@ -2347,7 +2327,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="str">
+      <c r="A47" s="47" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -2359,7 +2339,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="10" t="s">
         <v>63</v>
       </c>
@@ -2368,7 +2348,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="13" t="s">
         <v>64</v>
       </c>
@@ -2381,14 +2361,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="52"/>
-      <c r="C50" s="53"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="56"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="str">
+      <c r="A51" s="47" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -2400,7 +2380,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
@@ -2409,7 +2389,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
@@ -2418,7 +2398,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="str">
+      <c r="A54" s="47" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -2430,7 +2410,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
@@ -2439,7 +2419,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="str">
+      <c r="A56" s="47" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -2451,7 +2431,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
@@ -2460,7 +2440,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="str">
+      <c r="A58" s="47" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -2472,7 +2452,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="9" t="s">
         <v>98</v>
       </c>
@@ -2481,7 +2461,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="10" t="s">
         <v>83</v>
       </c>
@@ -2490,7 +2470,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="10" t="s">
         <v>84</v>
       </c>
@@ -2499,7 +2479,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="15" t="s">
         <v>85</v>
       </c>
@@ -2508,7 +2488,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="47"/>
       <c r="B63" s="9" t="s">
         <v>104</v>
       </c>
@@ -2517,7 +2497,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="10" t="s">
         <v>90</v>
       </c>
@@ -2526,7 +2506,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="str">
+      <c r="A65" s="47" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -2536,7 +2516,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
@@ -2545,7 +2525,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="44" t="str">
+      <c r="A67" s="47" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -2557,7 +2537,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="47"/>
       <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
@@ -2566,7 +2546,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="44" t="str">
+      <c r="A69" s="47" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2578,21 +2558,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
@@ -2601,7 +2581,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="44" t="str">
+      <c r="A73" s="47" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2613,7 +2593,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="47"/>
       <c r="B74" s="19" t="s">
         <v>96</v>
       </c>
@@ -2622,7 +2602,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="44" t="str">
+      <c r="A75" s="47" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2634,7 +2614,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
+      <c r="A76" s="47"/>
       <c r="B76" s="19" t="s">
         <v>102</v>
       </c>
@@ -2643,7 +2623,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="50"/>
+      <c r="A77" s="48"/>
       <c r="B77" s="20" t="s">
         <v>103</v>
       </c>
@@ -2656,14 +2636,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="46" t="s">
+      <c r="A78" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="45"/>
-      <c r="C78" s="49"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="53"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="44" t="str">
+      <c r="A79" s="47" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2675,7 +2655,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="9" t="s">
         <v>118</v>
       </c>
@@ -2684,7 +2664,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="44" t="str">
+      <c r="A81" s="47" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2696,7 +2676,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
+      <c r="A82" s="47"/>
       <c r="B82" s="9" t="s">
         <v>119</v>
       </c>
@@ -2705,7 +2685,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="str">
+      <c r="A83" s="47" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2717,7 +2697,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
+      <c r="A84" s="47"/>
       <c r="B84" s="9" t="s">
         <v>121</v>
       </c>
@@ -2726,14 +2706,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="44" t="str">
+      <c r="A86" s="47" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2745,7 +2725,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
+      <c r="A87" s="47"/>
       <c r="B87" s="9" t="s">
         <v>124</v>
       </c>
@@ -2754,7 +2734,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
+      <c r="A88" s="47"/>
       <c r="B88" s="9" t="s">
         <v>125</v>
       </c>
@@ -2763,7 +2743,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2772,7 +2752,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
+      <c r="A90" s="47"/>
       <c r="B90" s="9" t="s">
         <v>127</v>
       </c>
@@ -2781,7 +2761,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
+      <c r="A91" s="47"/>
       <c r="B91" s="9" t="s">
         <v>128</v>
       </c>
@@ -2790,7 +2770,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="44" t="str">
+      <c r="A92" s="47" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2802,7 +2782,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="9" t="s">
         <v>130</v>
       </c>
@@ -2811,7 +2791,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
+      <c r="A94" s="47"/>
       <c r="B94" s="9" t="s">
         <v>131</v>
       </c>
@@ -2820,7 +2800,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
+      <c r="A95" s="47"/>
       <c r="B95" s="9" t="s">
         <v>132</v>
       </c>
@@ -2829,7 +2809,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="44" t="str">
+      <c r="A96" s="47" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2841,7 +2821,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
+      <c r="A97" s="47"/>
       <c r="B97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2850,7 +2830,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
+      <c r="A98" s="47"/>
       <c r="B98" s="9" t="s">
         <v>134</v>
       </c>
@@ -2859,7 +2839,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="str">
+      <c r="A99" s="47" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2871,7 +2851,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
+      <c r="A100" s="47"/>
       <c r="B100" s="9" t="s">
         <v>137</v>
       </c>
@@ -2880,7 +2860,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
+      <c r="A101" s="47"/>
       <c r="B101" s="9" t="s">
         <v>136</v>
       </c>
@@ -2889,7 +2869,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
+      <c r="A102" s="47"/>
       <c r="B102" s="9" t="s">
         <v>138</v>
       </c>
@@ -2898,7 +2878,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
+      <c r="A103" s="47"/>
       <c r="B103" s="9" t="s">
         <v>146</v>
       </c>
@@ -2907,7 +2887,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="44" t="str">
+      <c r="A104" s="47" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2919,7 +2899,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
+      <c r="A105" s="47"/>
       <c r="B105" s="9" t="s">
         <v>140</v>
       </c>
@@ -2928,7 +2908,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="44"/>
+      <c r="A106" s="47"/>
       <c r="B106" s="9" t="s">
         <v>141</v>
       </c>
@@ -2937,7 +2917,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="44" t="str">
+      <c r="A107" s="47" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2949,7 +2929,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
+      <c r="A108" s="47"/>
       <c r="B108" s="9" t="s">
         <v>143</v>
       </c>
@@ -2974,14 +2954,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="54" t="s">
+      <c r="A110" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="54"/>
-      <c r="C110" s="54"/>
+      <c r="B110" s="51"/>
+      <c r="C110" s="51"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="str">
+      <c r="A111" s="50" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2993,7 +2973,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="47"/>
       <c r="B112" s="9" t="s">
         <v>170</v>
       </c>
@@ -3002,7 +2982,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="44"/>
+      <c r="A113" s="47"/>
       <c r="B113" s="9" t="s">
         <v>154</v>
       </c>
@@ -3011,7 +2991,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="47"/>
       <c r="B114" s="9" t="s">
         <v>157</v>
       </c>
@@ -3020,7 +3000,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="44"/>
+      <c r="A115" s="47"/>
       <c r="B115" s="9" t="s">
         <v>158</v>
       </c>
@@ -3029,7 +3009,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="44" t="str">
+      <c r="A116" s="47" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -3041,7 +3021,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="44"/>
+      <c r="A117" s="47"/>
       <c r="B117" s="9" t="s">
         <v>156</v>
       </c>
@@ -3050,7 +3030,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="44" t="str">
+      <c r="A118" s="47" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -3062,7 +3042,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="44"/>
+      <c r="A119" s="47"/>
       <c r="B119" s="9" t="s">
         <v>160</v>
       </c>
@@ -3071,7 +3051,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="44"/>
+      <c r="A120" s="47"/>
       <c r="B120" s="9" t="s">
         <v>171</v>
       </c>
@@ -3080,7 +3060,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="44" t="str">
+      <c r="A121" s="47" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -3092,7 +3072,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="44"/>
+      <c r="A122" s="47"/>
       <c r="B122" s="24" t="s">
         <v>161</v>
       </c>
@@ -3101,7 +3081,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="44"/>
+      <c r="A123" s="47"/>
       <c r="B123" s="9" t="s">
         <v>175</v>
       </c>
@@ -3110,7 +3090,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="44"/>
+      <c r="A124" s="47"/>
       <c r="B124" s="9" t="s">
         <v>176</v>
       </c>
@@ -3119,7 +3099,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="44" t="str">
+      <c r="A125" s="47" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -3131,7 +3111,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="44"/>
+      <c r="A126" s="47"/>
       <c r="B126" s="9" t="s">
         <v>164</v>
       </c>
@@ -3140,7 +3120,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="44"/>
+      <c r="A127" s="47"/>
       <c r="B127" s="9" t="s">
         <v>165</v>
       </c>
@@ -3149,7 +3129,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="44" t="str">
+      <c r="A128" s="47" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -3161,7 +3141,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="44"/>
+      <c r="A129" s="47"/>
       <c r="B129" s="9" t="s">
         <v>167</v>
       </c>
@@ -3170,7 +3150,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="44"/>
+      <c r="A130" s="47"/>
       <c r="B130" s="9" t="s">
         <v>168</v>
       </c>
@@ -3179,7 +3159,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="44"/>
+      <c r="A131" s="47"/>
       <c r="B131" s="9" t="s">
         <v>177</v>
       </c>
@@ -3188,7 +3168,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="44" t="str">
+      <c r="A132" s="47" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -3200,7 +3180,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="44"/>
+      <c r="A133" s="47"/>
       <c r="B133" s="9" t="s">
         <v>169</v>
       </c>
@@ -3209,7 +3189,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="50"/>
+      <c r="A134" s="48"/>
       <c r="B134" s="22" t="s">
         <v>179</v>
       </c>
@@ -3222,14 +3202,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="45" t="s">
+      <c r="A135" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="45"/>
-      <c r="C135" s="45"/>
+      <c r="B135" s="52"/>
+      <c r="C135" s="52"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="46" t="str">
+      <c r="A136" s="50" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -3241,7 +3221,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="44"/>
+      <c r="A137" s="47"/>
       <c r="B137" s="9" t="s">
         <v>185</v>
       </c>
@@ -3250,7 +3230,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="44"/>
+      <c r="A138" s="47"/>
       <c r="B138" s="9" t="s">
         <v>199</v>
       </c>
@@ -3259,7 +3239,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="44"/>
+      <c r="A139" s="47"/>
       <c r="B139" s="9" t="s">
         <v>186</v>
       </c>
@@ -3268,7 +3248,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="44"/>
+      <c r="A140" s="47"/>
       <c r="B140" s="9" t="s">
         <v>187</v>
       </c>
@@ -3277,7 +3257,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="44" t="str">
+      <c r="A141" s="47" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -3289,7 +3269,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="44"/>
+      <c r="A142" s="47"/>
       <c r="B142" s="9" t="s">
         <v>189</v>
       </c>
@@ -3298,7 +3278,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="44"/>
+      <c r="A143" s="47"/>
       <c r="B143" s="9" t="s">
         <v>190</v>
       </c>
@@ -3307,7 +3287,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="44" t="str">
+      <c r="A144" s="47" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -3319,7 +3299,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="44"/>
+      <c r="A145" s="47"/>
       <c r="B145" s="9" t="s">
         <v>203</v>
       </c>
@@ -3328,7 +3308,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="44"/>
+      <c r="A146" s="47"/>
       <c r="B146" s="9" t="s">
         <v>206</v>
       </c>
@@ -3337,7 +3317,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="44"/>
+      <c r="A147" s="47"/>
       <c r="B147" s="9" t="s">
         <v>204</v>
       </c>
@@ -3346,7 +3326,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="44"/>
+      <c r="A148" s="47"/>
       <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
@@ -3355,7 +3335,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="44"/>
+      <c r="A149" s="47"/>
       <c r="B149" s="9" t="s">
         <v>205</v>
       </c>
@@ -3364,7 +3344,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="44" t="str">
+      <c r="A150" s="47" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -3376,7 +3356,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="44"/>
+      <c r="A151" s="47"/>
       <c r="B151" s="24" t="s">
         <v>208</v>
       </c>
@@ -3385,14 +3365,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="44"/>
+      <c r="A152" s="47"/>
       <c r="B152" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="44" t="str">
+      <c r="A153" s="47" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -3404,7 +3384,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="44"/>
+      <c r="A154" s="47"/>
       <c r="B154" s="9" t="s">
         <v>196</v>
       </c>
@@ -3413,7 +3393,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="44"/>
+      <c r="A155" s="47"/>
       <c r="B155" s="9" t="s">
         <v>193</v>
       </c>
@@ -3422,7 +3402,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="44"/>
+      <c r="A156" s="47"/>
       <c r="B156" s="9" t="s">
         <v>194</v>
       </c>
@@ -3431,7 +3411,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="44"/>
+      <c r="A157" s="47"/>
       <c r="B157" s="9" t="s">
         <v>211</v>
       </c>
@@ -3456,14 +3436,14 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="45" t="s">
+      <c r="A159" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="B159" s="45"/>
-      <c r="C159" s="45"/>
+      <c r="B159" s="52"/>
+      <c r="C159" s="52"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="46" t="str">
+      <c r="A160" s="50" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3475,7 +3455,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="44"/>
+      <c r="A161" s="47"/>
       <c r="B161" s="9" t="s">
         <v>226</v>
       </c>
@@ -3484,7 +3464,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="44"/>
+      <c r="A162" s="47"/>
       <c r="B162" s="9" t="s">
         <v>242</v>
       </c>
@@ -3493,7 +3473,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="44"/>
+      <c r="A163" s="47"/>
       <c r="B163" s="9" t="s">
         <v>221</v>
       </c>
@@ -3502,7 +3482,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="44"/>
+      <c r="A164" s="47"/>
       <c r="B164" s="9" t="s">
         <v>219</v>
       </c>
@@ -3511,7 +3491,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="44" t="str">
+      <c r="A165" s="47" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -3523,7 +3503,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="44"/>
+      <c r="A166" s="47"/>
       <c r="B166" s="9" t="s">
         <v>228</v>
       </c>
@@ -3532,7 +3512,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="44"/>
+      <c r="A167" s="47"/>
       <c r="B167" s="9" t="s">
         <v>222</v>
       </c>
@@ -3541,7 +3521,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="44"/>
+      <c r="A168" s="47"/>
       <c r="B168" s="9" t="s">
         <v>223</v>
       </c>
@@ -3550,7 +3530,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="44" t="str">
+      <c r="A169" s="47" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -3562,7 +3542,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="44"/>
+      <c r="A170" s="47"/>
       <c r="B170" s="9" t="s">
         <v>224</v>
       </c>
@@ -3571,14 +3551,14 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="44"/>
+      <c r="A171" s="47"/>
       <c r="B171" s="16" t="s">
         <v>241</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="44"/>
+      <c r="A172" s="47"/>
       <c r="B172" s="9" t="s">
         <v>243</v>
       </c>
@@ -3587,7 +3567,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="44"/>
+      <c r="A173" s="47"/>
       <c r="B173" s="9" t="s">
         <v>230</v>
       </c>
@@ -3596,7 +3576,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="44" t="str">
+      <c r="A174" s="47" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3608,7 +3588,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="44"/>
+      <c r="A175" s="47"/>
       <c r="B175" s="9" t="s">
         <v>232</v>
       </c>
@@ -3617,7 +3597,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="44"/>
+      <c r="A176" s="47"/>
       <c r="B176" s="9" t="s">
         <v>229</v>
       </c>
@@ -3626,7 +3606,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="44"/>
+      <c r="A177" s="47"/>
       <c r="B177" s="9" t="s">
         <v>231</v>
       </c>
@@ -3635,7 +3615,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="44" t="str">
+      <c r="A178" s="47" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3647,7 +3627,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="44"/>
+      <c r="A179" s="47"/>
       <c r="B179" s="9" t="s">
         <v>245</v>
       </c>
@@ -3656,7 +3636,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="44"/>
+      <c r="A180" s="47"/>
       <c r="B180" s="9" t="s">
         <v>234</v>
       </c>
@@ -3665,7 +3645,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="44"/>
+      <c r="A181" s="47"/>
       <c r="B181" s="9" t="s">
         <v>235</v>
       </c>
@@ -3674,7 +3654,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="44"/>
+      <c r="A182" s="47"/>
       <c r="B182" s="9" t="s">
         <v>236</v>
       </c>
@@ -3683,7 +3663,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="44" t="str">
+      <c r="A183" s="47" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
@@ -3695,7 +3675,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="44"/>
+      <c r="A184" s="47"/>
       <c r="B184" s="9" t="s">
         <v>248</v>
       </c>
@@ -3704,7 +3684,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="44"/>
+      <c r="A185" s="47"/>
       <c r="B185" s="9" t="s">
         <v>249</v>
       </c>
@@ -3713,7 +3693,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="44" t="str">
+      <c r="A186" s="47" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
@@ -3725,7 +3705,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="44"/>
+      <c r="A187" s="47"/>
       <c r="B187" s="9" t="s">
         <v>237</v>
       </c>
@@ -3734,7 +3714,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="44"/>
+      <c r="A188" s="47"/>
       <c r="B188" s="9" t="s">
         <v>240</v>
       </c>
@@ -3743,7 +3723,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="44"/>
+      <c r="A189" s="47"/>
       <c r="B189" s="9" t="s">
         <v>238</v>
       </c>
@@ -3756,11 +3736,11 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="41" t="s">
+      <c r="A190" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="B190" s="42"/>
-      <c r="C190" s="43"/>
+      <c r="B190" s="60"/>
+      <c r="C190" s="61"/>
       <c r="D190">
         <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
         <v>0</v>
@@ -3803,7 +3783,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="39" t="str">
+      <c r="A193" s="44" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3815,7 +3795,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="39"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="28" t="s">
         <v>257</v>
       </c>
@@ -3824,7 +3804,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="39"/>
+      <c r="A195" s="44"/>
       <c r="B195" s="28" t="s">
         <v>259</v>
       </c>
@@ -3833,7 +3813,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="39"/>
+      <c r="A196" s="44"/>
       <c r="B196" s="28" t="s">
         <v>268</v>
       </c>
@@ -3842,7 +3822,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="39"/>
+      <c r="A197" s="44"/>
       <c r="B197" s="28" t="s">
         <v>269</v>
       </c>
@@ -3851,7 +3831,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="39"/>
+      <c r="A198" s="44"/>
       <c r="B198" s="28" t="s">
         <v>270</v>
       </c>
@@ -3860,7 +3840,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="39"/>
+      <c r="A199" s="44"/>
       <c r="B199" s="28" t="s">
         <v>271</v>
       </c>
@@ -3870,7 +3850,7 @@
       <c r="D199" s="34"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="39"/>
+      <c r="A200" s="44"/>
       <c r="B200" s="28" t="s">
         <v>272</v>
       </c>
@@ -3879,7 +3859,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="39"/>
+      <c r="A201" s="44"/>
       <c r="B201" s="28" t="s">
         <v>273</v>
       </c>
@@ -3888,7 +3868,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="39"/>
+      <c r="A202" s="44"/>
       <c r="B202" s="28" t="s">
         <v>274</v>
       </c>
@@ -3897,7 +3877,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="39" t="str">
+      <c r="A203" s="44" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3909,7 +3889,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="39"/>
+      <c r="A204" s="44"/>
       <c r="B204" s="28" t="s">
         <v>261</v>
       </c>
@@ -3918,7 +3898,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="39"/>
+      <c r="A205" s="44"/>
       <c r="B205" s="28" t="s">
         <v>262</v>
       </c>
@@ -3927,7 +3907,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="39" t="str">
+      <c r="A206" s="44" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3939,7 +3919,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="39"/>
+      <c r="A207" s="44"/>
       <c r="B207" s="28" t="s">
         <v>264</v>
       </c>
@@ -3948,7 +3928,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="39"/>
+      <c r="A208" s="44"/>
       <c r="B208" s="28" t="s">
         <v>265</v>
       </c>
@@ -3957,7 +3937,7 @@
       </c>
     </row>
     <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="39" t="str">
+      <c r="A209" s="44" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3969,7 +3949,7 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="40"/>
+      <c r="A210" s="45"/>
       <c r="B210" s="32" t="s">
         <v>266</v>
       </c>
@@ -3978,11 +3958,11 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="41" t="s">
+      <c r="A211" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="B211" s="42"/>
-      <c r="C211" s="56"/>
+      <c r="B211" s="60"/>
+      <c r="C211" s="40"/>
       <c r="D211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"S","")))</f>
         <v>0</v>
@@ -3993,7 +3973,7 @@
       </c>
       <c r="F211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"C","")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"P","")))</f>
@@ -4001,24 +3981,26 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="57" t="str">
+      <c r="A212" s="49" t="str">
         <f>'S 9'!A1</f>
         <v>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</v>
       </c>
       <c r="B212" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="C212" s="31"/>
+      <c r="C212" s="31" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="213" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="57"/>
+      <c r="A213" s="49"/>
       <c r="B213" s="28" t="s">
         <v>289</v>
       </c>
       <c r="C213" s="31"/>
     </row>
     <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="58" t="str">
+      <c r="A214" s="46" t="str">
         <f>'S 9'!A2</f>
         <v>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</v>
       </c>
@@ -4028,35 +4010,35 @@
       <c r="C214" s="31"/>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215" s="58"/>
+      <c r="A215" s="46"/>
       <c r="B215" s="28" t="s">
         <v>292</v>
       </c>
       <c r="C215" s="31"/>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="58"/>
+      <c r="A216" s="46"/>
       <c r="B216" s="28" t="s">
         <v>291</v>
       </c>
       <c r="C216" s="31"/>
     </row>
     <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A217" s="58"/>
+      <c r="A217" s="46"/>
       <c r="B217" s="28" t="s">
         <v>294</v>
       </c>
       <c r="C217" s="31"/>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218" s="58"/>
+      <c r="A218" s="46"/>
       <c r="B218" s="28" t="s">
         <v>293</v>
       </c>
       <c r="C218" s="31"/>
     </row>
     <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="58" t="str">
+      <c r="A219" s="46" t="str">
         <f>'S 9'!A3</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -4066,28 +4048,28 @@
       <c r="C219" s="31"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="58"/>
+      <c r="A220" s="46"/>
       <c r="B220" s="28" t="s">
         <v>296</v>
       </c>
       <c r="C220" s="31"/>
     </row>
     <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="58"/>
+      <c r="A221" s="46"/>
       <c r="B221" s="28" t="s">
         <v>297</v>
       </c>
       <c r="C221" s="31"/>
     </row>
     <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A222" s="58"/>
+      <c r="A222" s="46"/>
       <c r="B222" s="28" t="s">
         <v>298</v>
       </c>
       <c r="C222" s="31"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="39" t="str">
+      <c r="A223" s="44" t="str">
         <f>'S 9'!A4</f>
         <v>I want bauble curvature to be the correct direction regardless which side the track connects to</v>
       </c>
@@ -4097,14 +4079,14 @@
       <c r="C223" s="31"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="39"/>
+      <c r="A224" s="44"/>
       <c r="B224" s="28" t="s">
         <v>301</v>
       </c>
       <c r="C224" s="31"/>
     </row>
     <row r="225" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="58" t="str">
+      <c r="A225" s="46" t="str">
         <f>'S 9'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -4114,35 +4096,35 @@
       <c r="C225" s="31"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="58"/>
+      <c r="A226" s="46"/>
       <c r="B226" s="28" t="s">
         <v>303</v>
       </c>
       <c r="C226" s="31"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="58"/>
+      <c r="A227" s="46"/>
       <c r="B227" s="28" t="s">
         <v>305</v>
       </c>
       <c r="C227" s="31"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="58"/>
+      <c r="A228" s="46"/>
       <c r="B228" s="28" t="s">
         <v>306</v>
       </c>
       <c r="C228" s="31"/>
     </row>
     <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="58"/>
+      <c r="A229" s="46"/>
       <c r="B229" s="28" t="s">
         <v>307</v>
       </c>
       <c r="C229" s="31"/>
     </row>
     <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="39" t="str">
+      <c r="A230" s="44" t="str">
         <f>'S 9'!A6</f>
         <v>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</v>
       </c>
@@ -4152,35 +4134,35 @@
       <c r="C230" s="31"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="39"/>
+      <c r="A231" s="44"/>
       <c r="B231" s="28" t="s">
         <v>309</v>
       </c>
       <c r="C231" s="31"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="39"/>
+      <c r="A232" s="44"/>
       <c r="B232" s="28" t="s">
         <v>310</v>
       </c>
       <c r="C232" s="31"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="39"/>
+      <c r="A233" s="44"/>
       <c r="B233" s="28" t="s">
         <v>312</v>
       </c>
       <c r="C233" s="31"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="39"/>
+      <c r="A234" s="44"/>
       <c r="B234" s="28" t="s">
         <v>311</v>
       </c>
       <c r="C234" s="31"/>
     </row>
     <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="39" t="str">
+      <c r="A235" s="44" t="str">
         <f>'S 9'!A7</f>
         <v>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</v>
       </c>
@@ -4190,55 +4172,78 @@
       <c r="C235" s="31"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="39"/>
+      <c r="A236" s="44"/>
       <c r="B236" s="28" t="s">
         <v>314</v>
       </c>
       <c r="C236" s="31"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="39"/>
+      <c r="A237" s="44"/>
       <c r="B237" s="28" t="s">
         <v>315</v>
       </c>
       <c r="C237" s="31"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="39"/>
+      <c r="A238" s="44"/>
       <c r="B238" s="28" t="s">
         <v>316</v>
       </c>
       <c r="C238" s="31"/>
     </row>
     <row r="239" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="40"/>
+      <c r="A239" s="45"/>
       <c r="B239" s="32" t="s">
         <v>317</v>
       </c>
       <c r="C239" s="33"/>
-      <c r="D239" s="59" t="s">
+      <c r="D239" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="E239" s="60">
+      <c r="E239" s="42">
         <v>0.625</v>
       </c>
-      <c r="F239" s="61">
+      <c r="F239" s="43">
         <v>42227</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A219:A222"/>
-    <mergeCell ref="A223:A224"/>
-    <mergeCell ref="A225:A229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
     <mergeCell ref="A214:A218"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
@@ -4255,33 +4260,12 @@
     <mergeCell ref="A111:A115"/>
     <mergeCell ref="A116:A117"/>
     <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A212:A213"/>
     <mergeCell ref="A159:C159"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
     <mergeCell ref="A153:A157"/>
     <mergeCell ref="A135:C135"/>
     <mergeCell ref="A136:A140"/>
@@ -4292,13 +4276,11 @@
     <mergeCell ref="A169:A173"/>
     <mergeCell ref="A174:A177"/>
     <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A230:A234"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B210 B230:B1048576 B212:B228">
     <cfRule type="expression" dxfId="11" priority="1">

</xml_diff>

<commit_message>
Track sections can be selected for editing by dragging across the bauble
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="319">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -674,9 +674,6 @@
     <t>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</t>
   </si>
   <si>
-    <t>When I select a bauble to move it, it should move the whole bauble, with all attached track sections moving with it.  If a track section can't meet the bauble, the bauble transitions backwards to where all track sections can meet it.</t>
-  </si>
-  <si>
     <t>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</t>
   </si>
   <si>
@@ -981,6 +978,9 @@
   </si>
   <si>
     <t>Deadline</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1401,13 +1401,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1426,12 +1432,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1836,9 +1836,9 @@
   <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A211" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A208" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="C213" sqref="C213"/>
+      <selection pane="bottomLeft" activeCell="A214" sqref="A214:A218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,30 +1861,30 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="G1" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>279</v>
-      </c>
       <c r="H1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="str">
@@ -2089,11 +2089,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -2361,11 +2361,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="56"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="58"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="str">
@@ -2636,11 +2636,11 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="50" t="s">
+      <c r="A78" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="52"/>
-      <c r="C78" s="53"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="55"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="str">
@@ -2954,14 +2954,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="51"/>
-      <c r="C110" s="51"/>
+      <c r="B110" s="54"/>
+      <c r="C110" s="54"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="50" t="str">
+      <c r="A111" s="51" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -3202,14 +3202,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="52" t="s">
+      <c r="A135" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="52"/>
-      <c r="C135" s="52"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="50"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="50" t="str">
+      <c r="A136" s="51" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -3436,19 +3436,19 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="52" t="s">
+      <c r="A159" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="B159" s="52"/>
-      <c r="C159" s="52"/>
+      <c r="B159" s="50"/>
+      <c r="C159" s="50"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="50" t="str">
+      <c r="A160" s="51" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
       <c r="B160" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C160" s="26" t="s">
         <v>23</v>
@@ -3457,7 +3457,7 @@
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="47"/>
       <c r="B161" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>23</v>
@@ -3466,7 +3466,7 @@
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="47"/>
       <c r="B162" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>23</v>
@@ -3475,7 +3475,7 @@
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="47"/>
       <c r="B163" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>23</v>
@@ -3484,7 +3484,7 @@
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="47"/>
       <c r="B164" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C164" s="12" t="s">
         <v>23</v>
@@ -3496,7 +3496,7 @@
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>23</v>
@@ -3505,7 +3505,7 @@
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="47"/>
       <c r="B166" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>23</v>
@@ -3514,7 +3514,7 @@
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="47"/>
       <c r="B167" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C167" s="12" t="s">
         <v>23</v>
@@ -3523,7 +3523,7 @@
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="47"/>
       <c r="B168" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C168" s="12" t="s">
         <v>23</v>
@@ -3535,7 +3535,7 @@
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C169" s="12" t="s">
         <v>23</v>
@@ -3544,7 +3544,7 @@
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="47"/>
       <c r="B170" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C170" s="12" t="s">
         <v>23</v>
@@ -3553,14 +3553,14 @@
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="47"/>
       <c r="B171" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="47"/>
       <c r="B172" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>23</v>
@@ -3569,7 +3569,7 @@
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="47"/>
       <c r="B173" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>23</v>
@@ -3581,7 +3581,7 @@
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>23</v>
@@ -3590,7 +3590,7 @@
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="47"/>
       <c r="B175" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>23</v>
@@ -3599,7 +3599,7 @@
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="47"/>
       <c r="B176" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>23</v>
@@ -3608,7 +3608,7 @@
     <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="47"/>
       <c r="B177" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>23</v>
@@ -3620,7 +3620,7 @@
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>23</v>
@@ -3629,7 +3629,7 @@
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="47"/>
       <c r="B179" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>23</v>
@@ -3638,7 +3638,7 @@
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="47"/>
       <c r="B180" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>23</v>
@@ -3647,7 +3647,7 @@
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="47"/>
       <c r="B181" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>23</v>
@@ -3656,7 +3656,7 @@
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="47"/>
       <c r="B182" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>23</v>
@@ -3668,7 +3668,7 @@
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>23</v>
@@ -3677,7 +3677,7 @@
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="47"/>
       <c r="B184" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>23</v>
@@ -3686,7 +3686,7 @@
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="47"/>
       <c r="B185" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>23</v>
@@ -3698,7 +3698,7 @@
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>23</v>
@@ -3707,7 +3707,7 @@
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="47"/>
       <c r="B187" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>23</v>
@@ -3716,7 +3716,7 @@
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="47"/>
       <c r="B188" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>23</v>
@@ -3725,7 +3725,7 @@
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="47"/>
       <c r="B189" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>23</v>
@@ -3736,10 +3736,10 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="B190" s="60"/>
+      <c r="A190" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="B190" s="53"/>
       <c r="C190" s="61"/>
       <c r="D190">
         <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
@@ -3764,10 +3764,10 @@
         <v>I want to be able to create large curved sections without the colliders bugging out.</v>
       </c>
       <c r="B191" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C191" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -3776,10 +3776,10 @@
         <v>I want a way to remove a locomotive from the world.</v>
       </c>
       <c r="B192" s="28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C192" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3788,92 +3788,92 @@
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
       <c r="B193" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C193" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="44"/>
       <c r="B194" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C194" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="44"/>
       <c r="B195" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C195" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="44"/>
       <c r="B196" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C196" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="44"/>
       <c r="B197" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C197" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="44"/>
       <c r="B198" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C198" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="44"/>
       <c r="B199" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C199" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D199" s="34"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="44"/>
       <c r="B200" s="28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C200" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="44"/>
       <c r="B201" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C201" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="44"/>
       <c r="B202" s="28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C202" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,28 +3882,28 @@
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
       <c r="B203" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C203" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="44"/>
       <c r="B204" s="28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C204" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="44"/>
       <c r="B205" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C205" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3912,28 +3912,28 @@
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
       <c r="B206" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C206" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="44"/>
       <c r="B207" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C207" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="44"/>
       <c r="B208" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C208" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3942,30 +3942,30 @@
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
       <c r="B209" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="45"/>
       <c r="B210" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C210" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="59" t="s">
-        <v>282</v>
-      </c>
-      <c r="B211" s="60"/>
+      <c r="A211" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="B211" s="53"/>
       <c r="C211" s="40"/>
       <c r="D211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"S","")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"R","")))</f>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="F211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"C","")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"P","")))</f>
@@ -3986,18 +3986,20 @@
         <v>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</v>
       </c>
       <c r="B212" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="49"/>
       <c r="B213" s="28" t="s">
-        <v>289</v>
-      </c>
-      <c r="C213" s="31"/>
+        <v>288</v>
+      </c>
+      <c r="C213" s="31" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="46" t="str">
@@ -4005,35 +4007,37 @@
         <v>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</v>
       </c>
       <c r="B214" s="28" t="s">
-        <v>290</v>
-      </c>
-      <c r="C214" s="31"/>
+        <v>289</v>
+      </c>
+      <c r="C214" s="31" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="46"/>
       <c r="B215" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C215" s="31"/>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="46"/>
       <c r="B216" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C216" s="31"/>
     </row>
     <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="46"/>
       <c r="B217" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C217" s="31"/>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="46"/>
       <c r="B218" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C218" s="31"/>
     </row>
@@ -4043,28 +4047,28 @@
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
       <c r="B219" s="28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C219" s="31"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="46"/>
       <c r="B220" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C220" s="31"/>
     </row>
     <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="46"/>
       <c r="B221" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C221" s="31"/>
     </row>
     <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="46"/>
       <c r="B222" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C222" s="31"/>
     </row>
@@ -4074,14 +4078,14 @@
         <v>I want bauble curvature to be the correct direction regardless which side the track connects to</v>
       </c>
       <c r="B223" s="28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C223" s="31"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="44"/>
       <c r="B224" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C224" s="31"/>
     </row>
@@ -4091,35 +4095,35 @@
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
       <c r="B225" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C225" s="31"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="46"/>
       <c r="B226" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C226" s="31"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="46"/>
       <c r="B227" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C227" s="31"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="46"/>
       <c r="B228" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C228" s="31"/>
     </row>
     <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="46"/>
       <c r="B229" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C229" s="31"/>
     </row>
@@ -4129,35 +4133,35 @@
         <v>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</v>
       </c>
       <c r="B230" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C230" s="31"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="44"/>
       <c r="B231" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C231" s="31"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="44"/>
       <c r="B232" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C232" s="31"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="44"/>
       <c r="B233" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C233" s="31"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="44"/>
       <c r="B234" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C234" s="31"/>
     </row>
@@ -4167,39 +4171,39 @@
         <v>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</v>
       </c>
       <c r="B235" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C235" s="31"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="44"/>
       <c r="B236" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C236" s="31"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="44"/>
       <c r="B237" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C237" s="31"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="44"/>
       <c r="B238" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C238" s="31"/>
     </row>
     <row r="239" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="45"/>
       <c r="B239" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C239" s="33"/>
       <c r="D239" s="41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E239" s="42">
         <v>0.625</v>
@@ -4344,12 +4348,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4359,7 +4363,7 @@
     </row>
     <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4369,12 +4373,12 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4387,7 +4391,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4396,23 +4400,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>216</v>
+      <c r="A1" s="14" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4806,12 +4805,12 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4834,12 +4833,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4859,7 +4858,7 @@
     </row>
     <row r="6" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A track section will no longer be placed if its shape is invalid
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="319">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -1383,28 +1383,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1413,10 +1398,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1428,14 +1428,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1836,9 +1836,9 @@
   <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A208" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A211" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A214" sqref="A214:A218"/>
+      <selection pane="bottomLeft" activeCell="C217" sqref="C217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,14 +1880,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="str">
+      <c r="A3" s="44" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1899,7 +1899,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1908,7 +1908,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="str">
+      <c r="A6" s="44" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1929,7 +1929,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1938,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +1965,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="str">
+      <c r="A12" s="44" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1986,7 +1986,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -2004,7 +2004,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="str">
+      <c r="A15" s="44" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="str">
+      <c r="A19" s="44" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -2055,7 +2055,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2064,7 +2064,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="str">
+      <c r="A21" s="44" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -2076,7 +2076,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2089,11 +2089,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="55"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -2108,7 +2108,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="str">
+      <c r="A25" s="44" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="str">
+      <c r="A27" s="44" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
@@ -2159,7 +2159,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="10" t="s">
         <v>65</v>
       </c>
@@ -2168,7 +2168,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
@@ -2186,7 +2186,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="str">
+      <c r="A34" s="44" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="10" t="s">
         <v>49</v>
       </c>
@@ -2216,7 +2216,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="47" t="str">
+      <c r="A38" s="44" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -2246,7 +2246,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
@@ -2267,7 +2267,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47" t="str">
+      <c r="A41" s="44" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="10" t="s">
         <v>57</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="10" t="s">
         <v>58</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="str">
+      <c r="A45" s="44" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="10" t="s">
         <v>61</v>
       </c>
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="47" t="str">
+      <c r="A47" s="44" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="10" t="s">
         <v>63</v>
       </c>
@@ -2348,7 +2348,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="48"/>
+      <c r="A49" s="55"/>
       <c r="B49" s="13" t="s">
         <v>64</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="C50" s="58"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="47" t="str">
+      <c r="A51" s="44" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -2380,7 +2380,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="47" t="str">
+      <c r="A54" s="44" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -2410,7 +2410,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
@@ -2419,7 +2419,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="47" t="str">
+      <c r="A56" s="44" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -2431,7 +2431,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
+      <c r="A57" s="44"/>
       <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
@@ -2440,7 +2440,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="47" t="str">
+      <c r="A58" s="44" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
+      <c r="A59" s="44"/>
       <c r="B59" s="9" t="s">
         <v>98</v>
       </c>
@@ -2461,7 +2461,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="44"/>
       <c r="B60" s="10" t="s">
         <v>83</v>
       </c>
@@ -2470,7 +2470,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
+      <c r="A61" s="44"/>
       <c r="B61" s="10" t="s">
         <v>84</v>
       </c>
@@ -2479,7 +2479,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="15" t="s">
         <v>85</v>
       </c>
@@ -2488,7 +2488,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="9" t="s">
         <v>104</v>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
+      <c r="A64" s="44"/>
       <c r="B64" s="10" t="s">
         <v>90</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47" t="str">
+      <c r="A65" s="44" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
+      <c r="A66" s="44"/>
       <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="str">
+      <c r="A67" s="44" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
+      <c r="A68" s="44"/>
       <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
@@ -2546,7 +2546,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="47" t="str">
+      <c r="A69" s="44" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2558,21 +2558,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
+      <c r="A70" s="44"/>
       <c r="B70" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
+      <c r="A71" s="44"/>
       <c r="B71" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="47" t="str">
+      <c r="A73" s="44" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="19" t="s">
         <v>96</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="47" t="str">
+      <c r="A75" s="44" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2614,7 +2614,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
+      <c r="A76" s="44"/>
       <c r="B76" s="19" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2623,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="48"/>
+      <c r="A77" s="55"/>
       <c r="B77" s="20" t="s">
         <v>103</v>
       </c>
@@ -2636,14 +2636,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="51" t="s">
+      <c r="A78" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="50"/>
-      <c r="C78" s="55"/>
+      <c r="B78" s="53"/>
+      <c r="C78" s="54"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="47" t="str">
+      <c r="A79" s="44" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2655,7 +2655,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
+      <c r="A80" s="44"/>
       <c r="B80" s="9" t="s">
         <v>118</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="47" t="str">
+      <c r="A81" s="44" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2676,7 +2676,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
+      <c r="A82" s="44"/>
       <c r="B82" s="9" t="s">
         <v>119</v>
       </c>
@@ -2685,7 +2685,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="str">
+      <c r="A83" s="44" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
+      <c r="A84" s="44"/>
       <c r="B84" s="9" t="s">
         <v>121</v>
       </c>
@@ -2706,14 +2706,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
+      <c r="A85" s="44"/>
       <c r="B85" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="47" t="str">
+      <c r="A86" s="44" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2725,7 +2725,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
+      <c r="A87" s="44"/>
       <c r="B87" s="9" t="s">
         <v>124</v>
       </c>
@@ -2734,7 +2734,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="9" t="s">
         <v>125</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="47"/>
+      <c r="A89" s="44"/>
       <c r="B89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2752,7 +2752,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
+      <c r="A90" s="44"/>
       <c r="B90" s="9" t="s">
         <v>127</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
+      <c r="A91" s="44"/>
       <c r="B91" s="9" t="s">
         <v>128</v>
       </c>
@@ -2770,7 +2770,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="47" t="str">
+      <c r="A92" s="44" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2782,7 +2782,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
+      <c r="A93" s="44"/>
       <c r="B93" s="9" t="s">
         <v>130</v>
       </c>
@@ -2791,7 +2791,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
+      <c r="A94" s="44"/>
       <c r="B94" s="9" t="s">
         <v>131</v>
       </c>
@@ -2800,7 +2800,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="47"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="9" t="s">
         <v>132</v>
       </c>
@@ -2809,7 +2809,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="47" t="str">
+      <c r="A96" s="44" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2821,7 +2821,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="47"/>
+      <c r="A97" s="44"/>
       <c r="B97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="47"/>
+      <c r="A98" s="44"/>
       <c r="B98" s="9" t="s">
         <v>134</v>
       </c>
@@ -2839,7 +2839,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="47" t="str">
+      <c r="A99" s="44" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2851,7 +2851,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="9" t="s">
         <v>137</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="47"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="9" t="s">
         <v>136</v>
       </c>
@@ -2869,7 +2869,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="9" t="s">
         <v>138</v>
       </c>
@@ -2878,7 +2878,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="47"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="9" t="s">
         <v>146</v>
       </c>
@@ -2887,7 +2887,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="47" t="str">
+      <c r="A104" s="44" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2899,7 +2899,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="47"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="9" t="s">
         <v>140</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="47"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="9" t="s">
         <v>141</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="47" t="str">
+      <c r="A107" s="44" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="47"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="9" t="s">
         <v>143</v>
       </c>
@@ -2954,14 +2954,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="54" t="s">
+      <c r="A110" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="54"/>
-      <c r="C110" s="54"/>
+      <c r="B110" s="60"/>
+      <c r="C110" s="60"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="51" t="str">
+      <c r="A111" s="52" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2973,7 +2973,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="47"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="9" t="s">
         <v>170</v>
       </c>
@@ -2982,7 +2982,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="47"/>
+      <c r="A113" s="44"/>
       <c r="B113" s="9" t="s">
         <v>154</v>
       </c>
@@ -2991,7 +2991,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="47"/>
+      <c r="A114" s="44"/>
       <c r="B114" s="9" t="s">
         <v>157</v>
       </c>
@@ -3000,7 +3000,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="47"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="9" t="s">
         <v>158</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="47" t="str">
+      <c r="A116" s="44" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="47"/>
+      <c r="A117" s="44"/>
       <c r="B117" s="9" t="s">
         <v>156</v>
       </c>
@@ -3030,7 +3030,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="47" t="str">
+      <c r="A118" s="44" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -3042,7 +3042,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="47"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="9" t="s">
         <v>160</v>
       </c>
@@ -3051,7 +3051,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="9" t="s">
         <v>171</v>
       </c>
@@ -3060,7 +3060,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="47" t="str">
+      <c r="A121" s="44" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -3072,7 +3072,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="47"/>
+      <c r="A122" s="44"/>
       <c r="B122" s="24" t="s">
         <v>161</v>
       </c>
@@ -3081,7 +3081,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="47"/>
+      <c r="A123" s="44"/>
       <c r="B123" s="9" t="s">
         <v>175</v>
       </c>
@@ -3090,7 +3090,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="47"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="9" t="s">
         <v>176</v>
       </c>
@@ -3099,7 +3099,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="47" t="str">
+      <c r="A125" s="44" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -3111,7 +3111,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="47"/>
+      <c r="A126" s="44"/>
       <c r="B126" s="9" t="s">
         <v>164</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="47"/>
+      <c r="A127" s="44"/>
       <c r="B127" s="9" t="s">
         <v>165</v>
       </c>
@@ -3129,7 +3129,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="47" t="str">
+      <c r="A128" s="44" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="47"/>
+      <c r="A129" s="44"/>
       <c r="B129" s="9" t="s">
         <v>167</v>
       </c>
@@ -3150,7 +3150,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="47"/>
+      <c r="A130" s="44"/>
       <c r="B130" s="9" t="s">
         <v>168</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="47"/>
+      <c r="A131" s="44"/>
       <c r="B131" s="9" t="s">
         <v>177</v>
       </c>
@@ -3168,7 +3168,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="47" t="str">
+      <c r="A132" s="44" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -3180,7 +3180,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="47"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="9" t="s">
         <v>169</v>
       </c>
@@ -3189,7 +3189,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="48"/>
+      <c r="A134" s="55"/>
       <c r="B134" s="22" t="s">
         <v>179</v>
       </c>
@@ -3202,14 +3202,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="50" t="s">
+      <c r="A135" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="50"/>
-      <c r="C135" s="50"/>
+      <c r="B135" s="53"/>
+      <c r="C135" s="53"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="51" t="str">
+      <c r="A136" s="52" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="47"/>
+      <c r="A137" s="44"/>
       <c r="B137" s="9" t="s">
         <v>185</v>
       </c>
@@ -3230,7 +3230,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="47"/>
+      <c r="A138" s="44"/>
       <c r="B138" s="9" t="s">
         <v>199</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="47"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="9" t="s">
         <v>186</v>
       </c>
@@ -3248,7 +3248,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="47"/>
+      <c r="A140" s="44"/>
       <c r="B140" s="9" t="s">
         <v>187</v>
       </c>
@@ -3257,7 +3257,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="47" t="str">
+      <c r="A141" s="44" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -3269,7 +3269,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="47"/>
+      <c r="A142" s="44"/>
       <c r="B142" s="9" t="s">
         <v>189</v>
       </c>
@@ -3278,7 +3278,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="47"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="9" t="s">
         <v>190</v>
       </c>
@@ -3287,7 +3287,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="47" t="str">
+      <c r="A144" s="44" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -3299,7 +3299,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="47"/>
+      <c r="A145" s="44"/>
       <c r="B145" s="9" t="s">
         <v>203</v>
       </c>
@@ -3308,7 +3308,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="47"/>
+      <c r="A146" s="44"/>
       <c r="B146" s="9" t="s">
         <v>206</v>
       </c>
@@ -3317,7 +3317,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="47"/>
+      <c r="A147" s="44"/>
       <c r="B147" s="9" t="s">
         <v>204</v>
       </c>
@@ -3326,7 +3326,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="47"/>
+      <c r="A148" s="44"/>
       <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
@@ -3335,7 +3335,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="47"/>
+      <c r="A149" s="44"/>
       <c r="B149" s="9" t="s">
         <v>205</v>
       </c>
@@ -3344,7 +3344,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="47" t="str">
+      <c r="A150" s="44" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="47"/>
+      <c r="A151" s="44"/>
       <c r="B151" s="24" t="s">
         <v>208</v>
       </c>
@@ -3365,14 +3365,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="47"/>
+      <c r="A152" s="44"/>
       <c r="B152" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="47" t="str">
+      <c r="A153" s="44" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="47"/>
+      <c r="A154" s="44"/>
       <c r="B154" s="9" t="s">
         <v>196</v>
       </c>
@@ -3393,7 +3393,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="47"/>
+      <c r="A155" s="44"/>
       <c r="B155" s="9" t="s">
         <v>193</v>
       </c>
@@ -3402,7 +3402,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="47"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="9" t="s">
         <v>194</v>
       </c>
@@ -3411,7 +3411,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="47"/>
+      <c r="A157" s="44"/>
       <c r="B157" s="9" t="s">
         <v>211</v>
       </c>
@@ -3436,14 +3436,14 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="50" t="s">
+      <c r="A159" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="B159" s="50"/>
-      <c r="C159" s="50"/>
+      <c r="B159" s="53"/>
+      <c r="C159" s="53"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="51" t="str">
+      <c r="A160" s="52" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3455,7 +3455,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="47"/>
+      <c r="A161" s="44"/>
       <c r="B161" s="9" t="s">
         <v>225</v>
       </c>
@@ -3464,7 +3464,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="47"/>
+      <c r="A162" s="44"/>
       <c r="B162" s="9" t="s">
         <v>241</v>
       </c>
@@ -3473,7 +3473,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="47"/>
+      <c r="A163" s="44"/>
       <c r="B163" s="9" t="s">
         <v>220</v>
       </c>
@@ -3482,7 +3482,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="47"/>
+      <c r="A164" s="44"/>
       <c r="B164" s="9" t="s">
         <v>218</v>
       </c>
@@ -3491,7 +3491,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="47" t="str">
+      <c r="A165" s="44" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -3503,7 +3503,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="47"/>
+      <c r="A166" s="44"/>
       <c r="B166" s="9" t="s">
         <v>227</v>
       </c>
@@ -3512,7 +3512,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="47"/>
+      <c r="A167" s="44"/>
       <c r="B167" s="9" t="s">
         <v>221</v>
       </c>
@@ -3521,7 +3521,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="47"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="9" t="s">
         <v>222</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="47" t="str">
+      <c r="A169" s="44" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -3542,7 +3542,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="47"/>
+      <c r="A170" s="44"/>
       <c r="B170" s="9" t="s">
         <v>223</v>
       </c>
@@ -3551,14 +3551,14 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="47"/>
+      <c r="A171" s="44"/>
       <c r="B171" s="16" t="s">
         <v>240</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="47"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="9" t="s">
         <v>242</v>
       </c>
@@ -3567,7 +3567,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="47"/>
+      <c r="A173" s="44"/>
       <c r="B173" s="9" t="s">
         <v>229</v>
       </c>
@@ -3576,7 +3576,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="47" t="str">
+      <c r="A174" s="44" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3588,7 +3588,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="47"/>
+      <c r="A175" s="44"/>
       <c r="B175" s="9" t="s">
         <v>231</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="47"/>
+      <c r="A176" s="44"/>
       <c r="B176" s="9" t="s">
         <v>228</v>
       </c>
@@ -3606,7 +3606,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="47"/>
+      <c r="A177" s="44"/>
       <c r="B177" s="9" t="s">
         <v>230</v>
       </c>
@@ -3615,7 +3615,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="47" t="str">
+      <c r="A178" s="44" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3627,7 +3627,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="47"/>
+      <c r="A179" s="44"/>
       <c r="B179" s="9" t="s">
         <v>244</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="47"/>
+      <c r="A180" s="44"/>
       <c r="B180" s="9" t="s">
         <v>233</v>
       </c>
@@ -3645,7 +3645,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="47"/>
+      <c r="A181" s="44"/>
       <c r="B181" s="9" t="s">
         <v>234</v>
       </c>
@@ -3654,7 +3654,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="47"/>
+      <c r="A182" s="44"/>
       <c r="B182" s="9" t="s">
         <v>235</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="47" t="str">
+      <c r="A183" s="44" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
@@ -3675,7 +3675,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="47"/>
+      <c r="A184" s="44"/>
       <c r="B184" s="9" t="s">
         <v>247</v>
       </c>
@@ -3684,7 +3684,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="47"/>
+      <c r="A185" s="44"/>
       <c r="B185" s="9" t="s">
         <v>248</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="47" t="str">
+      <c r="A186" s="44" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
@@ -3705,7 +3705,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="47"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="9" t="s">
         <v>236</v>
       </c>
@@ -3714,7 +3714,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="47"/>
+      <c r="A188" s="44"/>
       <c r="B188" s="9" t="s">
         <v>239</v>
       </c>
@@ -3723,7 +3723,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="47"/>
+      <c r="A189" s="44"/>
       <c r="B189" s="9" t="s">
         <v>237</v>
       </c>
@@ -3736,11 +3736,11 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="52" t="s">
+      <c r="A190" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="B190" s="53"/>
-      <c r="C190" s="61"/>
+      <c r="B190" s="48"/>
+      <c r="C190" s="49"/>
       <c r="D190">
         <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
         <v>0</v>
@@ -3783,7 +3783,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="44" t="str">
+      <c r="A193" s="45" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3795,7 +3795,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="44"/>
+      <c r="A194" s="45"/>
       <c r="B194" s="28" t="s">
         <v>256</v>
       </c>
@@ -3804,7 +3804,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="44"/>
+      <c r="A195" s="45"/>
       <c r="B195" s="28" t="s">
         <v>258</v>
       </c>
@@ -3813,7 +3813,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="44"/>
+      <c r="A196" s="45"/>
       <c r="B196" s="28" t="s">
         <v>267</v>
       </c>
@@ -3822,7 +3822,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="44"/>
+      <c r="A197" s="45"/>
       <c r="B197" s="28" t="s">
         <v>268</v>
       </c>
@@ -3831,7 +3831,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="44"/>
+      <c r="A198" s="45"/>
       <c r="B198" s="28" t="s">
         <v>269</v>
       </c>
@@ -3840,7 +3840,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="44"/>
+      <c r="A199" s="45"/>
       <c r="B199" s="28" t="s">
         <v>270</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="D199" s="34"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="44"/>
+      <c r="A200" s="45"/>
       <c r="B200" s="28" t="s">
         <v>271</v>
       </c>
@@ -3859,7 +3859,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="44"/>
+      <c r="A201" s="45"/>
       <c r="B201" s="28" t="s">
         <v>272</v>
       </c>
@@ -3868,7 +3868,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="44"/>
+      <c r="A202" s="45"/>
       <c r="B202" s="28" t="s">
         <v>273</v>
       </c>
@@ -3877,7 +3877,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="44" t="str">
+      <c r="A203" s="45" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="44"/>
+      <c r="A204" s="45"/>
       <c r="B204" s="28" t="s">
         <v>260</v>
       </c>
@@ -3898,7 +3898,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="44"/>
+      <c r="A205" s="45"/>
       <c r="B205" s="28" t="s">
         <v>261</v>
       </c>
@@ -3907,7 +3907,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="44" t="str">
+      <c r="A206" s="45" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3919,7 +3919,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="44"/>
+      <c r="A207" s="45"/>
       <c r="B207" s="28" t="s">
         <v>263</v>
       </c>
@@ -3928,7 +3928,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="44"/>
+      <c r="A208" s="45"/>
       <c r="B208" s="28" t="s">
         <v>264</v>
       </c>
@@ -3937,7 +3937,7 @@
       </c>
     </row>
     <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="44" t="str">
+      <c r="A209" s="45" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3949,7 +3949,7 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="45"/>
+      <c r="A210" s="46"/>
       <c r="B210" s="32" t="s">
         <v>265</v>
       </c>
@@ -3958,10 +3958,10 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="52" t="s">
+      <c r="A211" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="B211" s="53"/>
+      <c r="B211" s="48"/>
       <c r="C211" s="40"/>
       <c r="D211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"S","")))</f>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="F211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"C","")))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"P","")))</f>
@@ -3981,7 +3981,7 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="49" t="str">
+      <c r="A212" s="61" t="str">
         <f>'S 9'!A1</f>
         <v>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</v>
       </c>
@@ -3993,7 +3993,7 @@
       </c>
     </row>
     <row r="213" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="49"/>
+      <c r="A213" s="61"/>
       <c r="B213" s="28" t="s">
         <v>288</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="46" t="str">
+      <c r="A214" s="59" t="str">
         <f>'S 9'!A2</f>
         <v>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</v>
       </c>
@@ -4010,39 +4010,45 @@
         <v>289</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>318</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215" s="46"/>
+      <c r="A215" s="59"/>
       <c r="B215" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="C215" s="31"/>
+      <c r="C215" s="31" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="46"/>
+      <c r="A216" s="59"/>
       <c r="B216" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="C216" s="31"/>
+      <c r="C216" s="31" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A217" s="46"/>
+      <c r="A217" s="59"/>
       <c r="B217" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="C217" s="31"/>
+      <c r="C217" s="31" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218" s="46"/>
+      <c r="A218" s="59"/>
       <c r="B218" s="28" t="s">
         <v>292</v>
       </c>
       <c r="C218" s="31"/>
     </row>
     <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="46" t="str">
+      <c r="A219" s="59" t="str">
         <f>'S 9'!A3</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -4052,28 +4058,28 @@
       <c r="C219" s="31"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="46"/>
+      <c r="A220" s="59"/>
       <c r="B220" s="28" t="s">
         <v>295</v>
       </c>
       <c r="C220" s="31"/>
     </row>
     <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="46"/>
+      <c r="A221" s="59"/>
       <c r="B221" s="28" t="s">
         <v>296</v>
       </c>
       <c r="C221" s="31"/>
     </row>
     <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A222" s="46"/>
+      <c r="A222" s="59"/>
       <c r="B222" s="28" t="s">
         <v>297</v>
       </c>
       <c r="C222" s="31"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="44" t="str">
+      <c r="A223" s="45" t="str">
         <f>'S 9'!A4</f>
         <v>I want bauble curvature to be the correct direction regardless which side the track connects to</v>
       </c>
@@ -4083,14 +4089,14 @@
       <c r="C223" s="31"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="44"/>
+      <c r="A224" s="45"/>
       <c r="B224" s="28" t="s">
         <v>300</v>
       </c>
       <c r="C224" s="31"/>
     </row>
     <row r="225" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="46" t="str">
+      <c r="A225" s="59" t="str">
         <f>'S 9'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -4100,35 +4106,35 @@
       <c r="C225" s="31"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="46"/>
+      <c r="A226" s="59"/>
       <c r="B226" s="28" t="s">
         <v>302</v>
       </c>
       <c r="C226" s="31"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="46"/>
+      <c r="A227" s="59"/>
       <c r="B227" s="28" t="s">
         <v>304</v>
       </c>
       <c r="C227" s="31"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="46"/>
+      <c r="A228" s="59"/>
       <c r="B228" s="28" t="s">
         <v>305</v>
       </c>
       <c r="C228" s="31"/>
     </row>
     <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="46"/>
+      <c r="A229" s="59"/>
       <c r="B229" s="28" t="s">
         <v>306</v>
       </c>
       <c r="C229" s="31"/>
     </row>
     <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="44" t="str">
+      <c r="A230" s="45" t="str">
         <f>'S 9'!A6</f>
         <v>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</v>
       </c>
@@ -4138,35 +4144,35 @@
       <c r="C230" s="31"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="44"/>
+      <c r="A231" s="45"/>
       <c r="B231" s="28" t="s">
         <v>308</v>
       </c>
       <c r="C231" s="31"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="44"/>
+      <c r="A232" s="45"/>
       <c r="B232" s="28" t="s">
         <v>309</v>
       </c>
       <c r="C232" s="31"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="44"/>
+      <c r="A233" s="45"/>
       <c r="B233" s="28" t="s">
         <v>311</v>
       </c>
       <c r="C233" s="31"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="44"/>
+      <c r="A234" s="45"/>
       <c r="B234" s="28" t="s">
         <v>310</v>
       </c>
       <c r="C234" s="31"/>
     </row>
     <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="44" t="str">
+      <c r="A235" s="45" t="str">
         <f>'S 9'!A7</f>
         <v>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</v>
       </c>
@@ -4176,28 +4182,28 @@
       <c r="C235" s="31"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="44"/>
+      <c r="A236" s="45"/>
       <c r="B236" s="28" t="s">
         <v>313</v>
       </c>
       <c r="C236" s="31"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="44"/>
+      <c r="A237" s="45"/>
       <c r="B237" s="28" t="s">
         <v>314</v>
       </c>
       <c r="C237" s="31"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="44"/>
+      <c r="A238" s="45"/>
       <c r="B238" s="28" t="s">
         <v>315</v>
       </c>
       <c r="C238" s="31"/>
     </row>
     <row r="239" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="45"/>
+      <c r="A239" s="46"/>
       <c r="B239" s="32" t="s">
         <v>316</v>
       </c>
@@ -4215,39 +4221,27 @@
     <row r="240" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="A159:C159"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A165:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A182"/>
     <mergeCell ref="A214:A218"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
@@ -4264,27 +4258,39 @@
     <mergeCell ref="A111:A115"/>
     <mergeCell ref="A116:A117"/>
     <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A212:A213"/>
-    <mergeCell ref="A159:C159"/>
-    <mergeCell ref="A153:A157"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A149"/>
-    <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A165:A168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A219:A222"/>
-    <mergeCell ref="A223:A224"/>
-    <mergeCell ref="A225:A229"/>
-    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B210 B230:B1048576 B212:B228">
     <cfRule type="expression" dxfId="11" priority="1">

</xml_diff>

<commit_message>
Some simple transitions will show approximations while invalid.
</commit_message>
<xml_diff>
--- a/Docs/User Stories and Task List.xlsx
+++ b/Docs/User Stories and Task List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="320">
   <si>
     <t>I want to be able to pan the camera around the play field.</t>
   </si>
@@ -981,6 +981,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -1383,13 +1386,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1398,25 +1416,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1428,14 +1431,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1838,7 +1841,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A211" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="C217" sqref="C217"/>
+      <selection pane="bottomLeft" activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,14 +1883,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="str">
+      <c r="A3" s="47" t="str">
         <f>'S 1'!A1</f>
         <v>I want to be able to pan the camera around the play field.</v>
       </c>
@@ -1899,7 +1902,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1908,7 +1911,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1920,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="str">
+      <c r="A6" s="47" t="str">
         <f>'S 1'!A2</f>
         <v>I want a tool to raise and lower swaths of terrain by clicking or painting it</v>
       </c>
@@ -1929,7 +1932,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1941,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1947,7 +1950,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1956,7 +1959,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +1968,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1974,7 +1977,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="str">
+      <c r="A12" s="47" t="str">
         <f>'S 1'!A3</f>
         <v>I want a tool to flatten an area of terrain</v>
       </c>
@@ -1986,7 +1989,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1995,7 +1998,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -2004,7 +2007,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="str">
+      <c r="A15" s="47" t="str">
         <f>'S 1'!A4</f>
         <v>I want a tool to smooth over an area of terrain</v>
       </c>
@@ -2016,7 +2019,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -2025,7 +2028,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -2034,7 +2037,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="str">
+      <c r="A19" s="47" t="str">
         <f>'S 1'!A5</f>
         <v>I want terrain texture to depend on its steepness: grassy/velvet green for flat, rocky/plastic grey for cliffs.</v>
       </c>
@@ -2055,7 +2058,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2064,7 +2067,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="str">
+      <c r="A21" s="47" t="str">
         <f>'S 1'!A6</f>
         <v>I want the edge of the playfield to look like it has a table under it.</v>
       </c>
@@ -2076,7 +2079,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2089,11 +2092,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
@@ -2108,7 +2111,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="str">
+      <c r="A25" s="47" t="str">
         <f>'S 2'!A2</f>
         <v>I want to be able to create a new, flat terrain of a default height.</v>
       </c>
@@ -2120,7 +2123,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
@@ -2129,7 +2132,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="str">
+      <c r="A27" s="47" t="str">
         <f>'S 2'!A3</f>
         <v>I want to be able to save the terrain that I have been working on.</v>
       </c>
@@ -2141,7 +2144,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -2150,7 +2153,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
@@ -2159,7 +2162,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="10" t="s">
         <v>65</v>
       </c>
@@ -2168,7 +2171,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
@@ -2177,7 +2180,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
@@ -2186,7 +2189,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -2195,7 +2198,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="str">
+      <c r="A34" s="47" t="str">
         <f>'S 2'!A4</f>
         <v>I want to be able to load a saved terrain from disk.</v>
       </c>
@@ -2207,7 +2210,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="10" t="s">
         <v>49</v>
       </c>
@@ -2216,7 +2219,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
@@ -2225,7 +2228,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
@@ -2234,7 +2237,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="str">
+      <c r="A38" s="47" t="str">
         <f>'S 2'!A5</f>
         <v>The camera should not be allowed to move beyond limits defined by the terrain size.</v>
       </c>
@@ -2246,7 +2249,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
@@ -2267,7 +2270,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="str">
+      <c r="A41" s="47" t="str">
         <f>'S 2'!A7</f>
         <v>The game should begin on a main menu with buttons to go to the different play modes.</v>
       </c>
@@ -2279,7 +2282,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
@@ -2288,7 +2291,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="10" t="s">
         <v>57</v>
       </c>
@@ -2297,7 +2300,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="10" t="s">
         <v>58</v>
       </c>
@@ -2306,7 +2309,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="str">
+      <c r="A45" s="47" t="str">
         <f>'S 2'!A8</f>
         <v>I should be able to exit from the terrain editor/sandbox mode to the menu.</v>
       </c>
@@ -2318,7 +2321,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="10" t="s">
         <v>61</v>
       </c>
@@ -2327,7 +2330,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="str">
+      <c r="A47" s="47" t="str">
         <f>'S 2'!A9</f>
         <v>When I quit, I want to be prompted to save if I have changed anything since my last save.</v>
       </c>
@@ -2339,7 +2342,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="10" t="s">
         <v>63</v>
       </c>
@@ -2348,7 +2351,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="13" t="s">
         <v>64</v>
       </c>
@@ -2368,7 +2371,7 @@
       <c r="C50" s="58"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="str">
+      <c r="A51" s="47" t="str">
         <f>'S 3'!A1</f>
         <v>Utilities bar should not have a 'normal' button to deselect.  Instead, clicking on a button that is already selected should deselect it.  Selected buttons should be highlighted</v>
       </c>
@@ -2380,7 +2383,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
@@ -2389,7 +2392,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
@@ -2398,7 +2401,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="str">
+      <c r="A54" s="47" t="str">
         <f>'S 3'!A2</f>
         <v xml:space="preserve">The Camera should zoom more smoothly; use Lerp to transition to a target position.  </v>
       </c>
@@ -2410,7 +2413,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
@@ -2419,7 +2422,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="str">
+      <c r="A56" s="47" t="str">
         <f>'S 3'!A3</f>
         <v>Function for finding world point at zero from screen position should be unit testable.</v>
       </c>
@@ -2431,7 +2434,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
@@ -2440,7 +2443,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="str">
+      <c r="A58" s="47" t="str">
         <f>'S 3'!A4</f>
         <v>I want to be able to place a straight, flat section of track onto the terrain.</v>
       </c>
@@ -2452,7 +2455,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="9" t="s">
         <v>98</v>
       </c>
@@ -2461,7 +2464,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="10" t="s">
         <v>83</v>
       </c>
@@ -2470,7 +2473,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="10" t="s">
         <v>84</v>
       </c>
@@ -2479,7 +2482,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="15" t="s">
         <v>85</v>
       </c>
@@ -2488,7 +2491,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="47"/>
       <c r="B63" s="9" t="s">
         <v>104</v>
       </c>
@@ -2497,7 +2500,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="10" t="s">
         <v>90</v>
       </c>
@@ -2506,7 +2509,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="str">
+      <c r="A65" s="47" t="str">
         <f>'S 3'!A5</f>
         <v>I want to be able to place a straight section of track with an incline.  I want a way to control the inclination.  The terrain should follow the track height</v>
       </c>
@@ -2516,7 +2519,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
@@ -2525,7 +2528,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="44" t="str">
+      <c r="A67" s="47" t="str">
         <f>'S 3'!A6</f>
         <v>I want to be able to select an end of a track section that I have already placed, and adjust it.</v>
       </c>
@@ -2537,7 +2540,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="47"/>
       <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
@@ -2546,7 +2549,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="44" t="str">
+      <c r="A69" s="47" t="str">
         <f>'S 3'!A7</f>
         <v>When I save the map, any track sections I have placed should also be saved.</v>
       </c>
@@ -2558,21 +2561,21 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
@@ -2581,7 +2584,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="44" t="str">
+      <c r="A73" s="47" t="str">
         <f>'S 3'!A8</f>
         <v>When I load a map with track sections, they should be restored.</v>
       </c>
@@ -2593,7 +2596,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="47"/>
       <c r="B74" s="19" t="s">
         <v>96</v>
       </c>
@@ -2602,7 +2605,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="44" t="str">
+      <c r="A75" s="47" t="str">
         <f>'S 3'!A9</f>
         <v>Modularise Menu Behaviours a la http://unity3d.com/learn/tutorials/modules/intermediate/scripting/coding-practices</v>
       </c>
@@ -2614,7 +2617,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
+      <c r="A76" s="47"/>
       <c r="B76" s="19" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2626,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="55"/>
+      <c r="A77" s="48"/>
       <c r="B77" s="20" t="s">
         <v>103</v>
       </c>
@@ -2636,14 +2639,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="52" t="s">
+      <c r="A78" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="53"/>
-      <c r="C78" s="54"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="55"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="44" t="str">
+      <c r="A79" s="47" t="str">
         <f>'S 4'!A1</f>
         <v>Move the project and associated documentation onto a repository</v>
       </c>
@@ -2655,7 +2658,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="9" t="s">
         <v>118</v>
       </c>
@@ -2664,7 +2667,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="44" t="str">
+      <c r="A81" s="47" t="str">
         <f>'S 4'!A2</f>
         <v>Fix camera minimum height irregularity</v>
       </c>
@@ -2676,7 +2679,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
+      <c r="A82" s="47"/>
       <c r="B82" s="9" t="s">
         <v>119</v>
       </c>
@@ -2685,7 +2688,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="str">
+      <c r="A83" s="47" t="str">
         <f>'S 4'!A3</f>
         <v>I shouldn't be able to interact with scene objects if my mouse is over a UI element</v>
       </c>
@@ -2697,7 +2700,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
+      <c r="A84" s="47"/>
       <c r="B84" s="9" t="s">
         <v>121</v>
       </c>
@@ -2706,14 +2709,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="44" t="str">
+      <c r="A86" s="47" t="str">
         <f>'S 4'!A4</f>
         <v>When in track mode, cyan spheres should appear at the ends of each track section.  These are what I want to click on to select a track end.</v>
       </c>
@@ -2725,7 +2728,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
+      <c r="A87" s="47"/>
       <c r="B87" s="9" t="s">
         <v>124</v>
       </c>
@@ -2734,7 +2737,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
+      <c r="A88" s="47"/>
       <c r="B88" s="9" t="s">
         <v>125</v>
       </c>
@@ -2743,7 +2746,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2752,7 +2755,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
+      <c r="A90" s="47"/>
       <c r="B90" s="9" t="s">
         <v>127</v>
       </c>
@@ -2761,7 +2764,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
+      <c r="A91" s="47"/>
       <c r="B91" s="9" t="s">
         <v>128</v>
       </c>
@@ -2770,7 +2773,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="44" t="str">
+      <c r="A92" s="47" t="str">
         <f>'S 4'!A5</f>
         <v>I want a curved section of track to appear curved.</v>
       </c>
@@ -2782,7 +2785,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="9" t="s">
         <v>130</v>
       </c>
@@ -2791,7 +2794,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
+      <c r="A94" s="47"/>
       <c r="B94" s="9" t="s">
         <v>131</v>
       </c>
@@ -2800,7 +2803,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
+      <c r="A95" s="47"/>
       <c r="B95" s="9" t="s">
         <v>132</v>
       </c>
@@ -2809,7 +2812,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="44" t="str">
+      <c r="A96" s="47" t="str">
         <f>'S 4'!A6</f>
         <v>I want a curved section of track to have an appropriate collider/set of colliders.</v>
       </c>
@@ -2821,7 +2824,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
+      <c r="A97" s="47"/>
       <c r="B97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2830,7 +2833,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
+      <c r="A98" s="47"/>
       <c r="B98" s="9" t="s">
         <v>134</v>
       </c>
@@ -2839,7 +2842,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="str">
+      <c r="A99" s="47" t="str">
         <f>'S 4'!A7</f>
         <v>I want to left-click a track end to begin placing a curved section of track.  The track should begin at the track end I clicked on and in the direction of the existing track section.  The other end should follow my mouse pointer, curving as much as it needs to.</v>
       </c>
@@ -2851,7 +2854,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
+      <c r="A100" s="47"/>
       <c r="B100" s="9" t="s">
         <v>137</v>
       </c>
@@ -2860,7 +2863,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
+      <c r="A101" s="47"/>
       <c r="B101" s="9" t="s">
         <v>136</v>
       </c>
@@ -2869,7 +2872,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
+      <c r="A102" s="47"/>
       <c r="B102" s="9" t="s">
         <v>138</v>
       </c>
@@ -2878,7 +2881,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
+      <c r="A103" s="47"/>
       <c r="B103" s="9" t="s">
         <v>146</v>
       </c>
@@ -2887,7 +2890,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="44" t="str">
+      <c r="A104" s="47" t="str">
         <f>'S 4'!A8</f>
         <v>While editing a straight section of track, if I hover over a track end bauble, the section I am editing should become curved to fit into the existing track section</v>
       </c>
@@ -2899,7 +2902,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
+      <c r="A105" s="47"/>
       <c r="B105" s="9" t="s">
         <v>140</v>
       </c>
@@ -2908,7 +2911,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="44"/>
+      <c r="A106" s="47"/>
       <c r="B106" s="9" t="s">
         <v>141</v>
       </c>
@@ -2917,7 +2920,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="44" t="str">
+      <c r="A107" s="47" t="str">
         <f>'S 4'!A9</f>
         <v>I want a curved section of track to have the terrain meet its underside for its entire length once deployed.</v>
       </c>
@@ -2929,7 +2932,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
+      <c r="A108" s="47"/>
       <c r="B108" s="9" t="s">
         <v>143</v>
       </c>
@@ -2954,14 +2957,14 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="60" t="s">
+      <c r="A110" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="60"/>
-      <c r="C110" s="60"/>
+      <c r="B110" s="54"/>
+      <c r="C110" s="54"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="52" t="str">
+      <c r="A111" s="51" t="str">
         <f>'S 5'!A1</f>
         <v>There should only be one track section bauble at each joint.  Right-clicking on it will select the last track section to be connected to it.</v>
       </c>
@@ -2973,7 +2976,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="47"/>
       <c r="B112" s="9" t="s">
         <v>170</v>
       </c>
@@ -2982,7 +2985,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="44"/>
+      <c r="A113" s="47"/>
       <c r="B113" s="9" t="s">
         <v>154</v>
       </c>
@@ -2991,7 +2994,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="47"/>
       <c r="B114" s="9" t="s">
         <v>157</v>
       </c>
@@ -3000,7 +3003,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="44"/>
+      <c r="A115" s="47"/>
       <c r="B115" s="9" t="s">
         <v>158</v>
       </c>
@@ -3009,7 +3012,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="44" t="str">
+      <c r="A116" s="47" t="str">
         <f>'S 5'!A2</f>
         <v>Refactor the reversal of track sections such that it is done entirely in the shape controller, and the track tool doesn't need to know about it.</v>
       </c>
@@ -3021,7 +3024,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="44"/>
+      <c r="A117" s="47"/>
       <c r="B117" s="9" t="s">
         <v>156</v>
       </c>
@@ -3030,7 +3033,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="44" t="str">
+      <c r="A118" s="47" t="str">
         <f>'S 5'!A3</f>
         <v>Loading a map containing linked track sections should allow me to use the links correctly.</v>
       </c>
@@ -3042,7 +3045,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="44"/>
+      <c r="A119" s="47"/>
       <c r="B119" s="9" t="s">
         <v>160</v>
       </c>
@@ -3051,7 +3054,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="44"/>
+      <c r="A120" s="47"/>
       <c r="B120" s="9" t="s">
         <v>171</v>
       </c>
@@ -3060,7 +3063,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="44" t="str">
+      <c r="A121" s="47" t="str">
         <f>'S 5'!A4</f>
         <v>I want to be able to place a curved track from the end of one existing section to the beginning of another.</v>
       </c>
@@ -3072,7 +3075,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="44"/>
+      <c r="A122" s="47"/>
       <c r="B122" s="24" t="s">
         <v>161</v>
       </c>
@@ -3081,7 +3084,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="44"/>
+      <c r="A123" s="47"/>
       <c r="B123" s="9" t="s">
         <v>175</v>
       </c>
@@ -3090,7 +3093,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="44"/>
+      <c r="A124" s="47"/>
       <c r="B124" s="9" t="s">
         <v>176</v>
       </c>
@@ -3099,7 +3102,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="44" t="str">
+      <c r="A125" s="47" t="str">
         <f>'S 5'!A5</f>
         <v>I want to be able to place a buffer stop at an existing track end.</v>
       </c>
@@ -3111,7 +3114,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="44"/>
+      <c r="A126" s="47"/>
       <c r="B126" s="9" t="s">
         <v>164</v>
       </c>
@@ -3120,7 +3123,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="44"/>
+      <c r="A127" s="47"/>
       <c r="B127" s="9" t="s">
         <v>165</v>
       </c>
@@ -3129,7 +3132,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="44" t="str">
+      <c r="A128" s="47" t="str">
         <f>'S 5'!A6</f>
         <v>I should not be able to place a track section in such a way that another track's ballast is disturbed.</v>
       </c>
@@ -3141,7 +3144,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="44"/>
+      <c r="A129" s="47"/>
       <c r="B129" s="9" t="s">
         <v>167</v>
       </c>
@@ -3150,7 +3153,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="44"/>
+      <c r="A130" s="47"/>
       <c r="B130" s="9" t="s">
         <v>168</v>
       </c>
@@ -3159,7 +3162,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="44"/>
+      <c r="A131" s="47"/>
       <c r="B131" s="9" t="s">
         <v>177</v>
       </c>
@@ -3168,7 +3171,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="44" t="str">
+      <c r="A132" s="47" t="str">
         <f>'S 5'!A7</f>
         <v>Saving and loading a map with buffer stops and compound curve sections should keep them</v>
       </c>
@@ -3180,7 +3183,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="44"/>
+      <c r="A133" s="47"/>
       <c r="B133" s="9" t="s">
         <v>169</v>
       </c>
@@ -3189,7 +3192,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="55"/>
+      <c r="A134" s="48"/>
       <c r="B134" s="22" t="s">
         <v>179</v>
       </c>
@@ -3202,14 +3205,14 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="53" t="s">
+      <c r="A135" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="53"/>
-      <c r="C135" s="53"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="50"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="52" t="str">
+      <c r="A136" s="51" t="str">
         <f>'S 6'!A1</f>
         <v>Upgrade to Unity 5</v>
       </c>
@@ -3221,7 +3224,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="44"/>
+      <c r="A137" s="47"/>
       <c r="B137" s="9" t="s">
         <v>185</v>
       </c>
@@ -3230,7 +3233,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="44"/>
+      <c r="A138" s="47"/>
       <c r="B138" s="9" t="s">
         <v>199</v>
       </c>
@@ -3239,7 +3242,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="44"/>
+      <c r="A139" s="47"/>
       <c r="B139" s="9" t="s">
         <v>186</v>
       </c>
@@ -3248,7 +3251,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="44"/>
+      <c r="A140" s="47"/>
       <c r="B140" s="9" t="s">
         <v>187</v>
       </c>
@@ -3257,7 +3260,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="44" t="str">
+      <c r="A141" s="47" t="str">
         <f>'S 6'!A2</f>
         <v>Redesign whole project, including defining locomotives, carriages and props.</v>
       </c>
@@ -3269,7 +3272,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="44"/>
+      <c r="A142" s="47"/>
       <c r="B142" s="9" t="s">
         <v>189</v>
       </c>
@@ -3278,7 +3281,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="44"/>
+      <c r="A143" s="47"/>
       <c r="B143" s="9" t="s">
         <v>190</v>
       </c>
@@ -3287,7 +3290,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="44" t="str">
+      <c r="A144" s="47" t="str">
         <f>'S 6'!A3</f>
         <v>Refactor existing project components into new design.</v>
       </c>
@@ -3299,7 +3302,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="44"/>
+      <c r="A145" s="47"/>
       <c r="B145" s="9" t="s">
         <v>203</v>
       </c>
@@ -3308,7 +3311,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="44"/>
+      <c r="A146" s="47"/>
       <c r="B146" s="9" t="s">
         <v>206</v>
       </c>
@@ -3317,7 +3320,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="44"/>
+      <c r="A147" s="47"/>
       <c r="B147" s="9" t="s">
         <v>204</v>
       </c>
@@ -3326,7 +3329,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="44"/>
+      <c r="A148" s="47"/>
       <c r="B148" s="9" t="s">
         <v>207</v>
       </c>
@@ -3335,7 +3338,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="44"/>
+      <c r="A149" s="47"/>
       <c r="B149" s="9" t="s">
         <v>205</v>
       </c>
@@ -3344,7 +3347,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="44" t="str">
+      <c r="A150" s="47" t="str">
         <f>'S 6'!A4</f>
         <v>"Rail" vectors should be goverened by the same function that adds creases to the bending model</v>
       </c>
@@ -3356,7 +3359,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="44"/>
+      <c r="A151" s="47"/>
       <c r="B151" s="24" t="s">
         <v>208</v>
       </c>
@@ -3365,14 +3368,14 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="44"/>
+      <c r="A152" s="47"/>
       <c r="B152" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="44" t="str">
+      <c r="A153" s="47" t="str">
         <f>'S 6'!A5</f>
         <v>I want to be able to create a new bauble partway along straight track</v>
       </c>
@@ -3384,7 +3387,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="44"/>
+      <c r="A154" s="47"/>
       <c r="B154" s="9" t="s">
         <v>196</v>
       </c>
@@ -3393,7 +3396,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="44"/>
+      <c r="A155" s="47"/>
       <c r="B155" s="9" t="s">
         <v>193</v>
       </c>
@@ -3402,7 +3405,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="44"/>
+      <c r="A156" s="47"/>
       <c r="B156" s="9" t="s">
         <v>194</v>
       </c>
@@ -3411,7 +3414,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="44"/>
+      <c r="A157" s="47"/>
       <c r="B157" s="9" t="s">
         <v>211</v>
       </c>
@@ -3436,14 +3439,14 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="53" t="s">
+      <c r="A159" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="B159" s="53"/>
-      <c r="C159" s="53"/>
+      <c r="B159" s="50"/>
+      <c r="C159" s="50"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="52" t="str">
+      <c r="A160" s="51" t="str">
         <f>'S 7'!A1</f>
         <v>Parameters of the curve (L1, L2 etc) should be owned by the shape controller and passed to the Vertex Bender instead of recalculating in each Bend call.  Rail vectors need to be rewritten to be dependent on curve params</v>
       </c>
@@ -3455,7 +3458,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="44"/>
+      <c r="A161" s="47"/>
       <c r="B161" s="9" t="s">
         <v>225</v>
       </c>
@@ -3464,7 +3467,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="44"/>
+      <c r="A162" s="47"/>
       <c r="B162" s="9" t="s">
         <v>241</v>
       </c>
@@ -3473,7 +3476,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="44"/>
+      <c r="A163" s="47"/>
       <c r="B163" s="9" t="s">
         <v>220</v>
       </c>
@@ -3482,7 +3485,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="44"/>
+      <c r="A164" s="47"/>
       <c r="B164" s="9" t="s">
         <v>218</v>
       </c>
@@ -3491,7 +3494,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="44" t="str">
+      <c r="A165" s="47" t="str">
         <f>'S 7'!A2</f>
         <v>I want all types of curve to be considered compound curves, and for the shape controller to correctly handle them if L1, L2 = 0.</v>
       </c>
@@ -3503,7 +3506,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="44"/>
+      <c r="A166" s="47"/>
       <c r="B166" s="9" t="s">
         <v>227</v>
       </c>
@@ -3512,7 +3515,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="44"/>
+      <c r="A167" s="47"/>
       <c r="B167" s="9" t="s">
         <v>221</v>
       </c>
@@ -3521,7 +3524,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="44"/>
+      <c r="A168" s="47"/>
       <c r="B168" s="9" t="s">
         <v>222</v>
       </c>
@@ -3530,7 +3533,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="44" t="str">
+      <c r="A169" s="47" t="str">
         <f>'S 7'!A3</f>
         <v>Stretching out a section of track should merley be a matter of linking it to two baubles.  The bauble should update the track if it moves.</v>
       </c>
@@ -3542,7 +3545,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="44"/>
+      <c r="A170" s="47"/>
       <c r="B170" s="9" t="s">
         <v>223</v>
       </c>
@@ -3551,14 +3554,14 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="44"/>
+      <c r="A171" s="47"/>
       <c r="B171" s="16" t="s">
         <v>240</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="44"/>
+      <c r="A172" s="47"/>
       <c r="B172" s="9" t="s">
         <v>242</v>
       </c>
@@ -3567,7 +3570,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="44"/>
+      <c r="A173" s="47"/>
       <c r="B173" s="9" t="s">
         <v>229</v>
       </c>
@@ -3576,7 +3579,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="44" t="str">
+      <c r="A174" s="47" t="str">
         <f>'S 7'!A4</f>
         <v>I want to be able to place a locomotive on the track. There should be sufficient control to orient forwards or backwards.</v>
       </c>
@@ -3588,7 +3591,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="44"/>
+      <c r="A175" s="47"/>
       <c r="B175" s="9" t="s">
         <v>231</v>
       </c>
@@ -3597,7 +3600,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="44"/>
+      <c r="A176" s="47"/>
       <c r="B176" s="9" t="s">
         <v>228</v>
       </c>
@@ -3606,7 +3609,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A177" s="44"/>
+      <c r="A177" s="47"/>
       <c r="B177" s="9" t="s">
         <v>230</v>
       </c>
@@ -3615,7 +3618,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="44" t="str">
+      <c r="A178" s="47" t="str">
         <f>'S 7'!A5</f>
         <v>I want to be able to set the power level of a locomotive (in the editor for now) and have it move along the rail accordingly.</v>
       </c>
@@ -3627,7 +3630,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="44"/>
+      <c r="A179" s="47"/>
       <c r="B179" s="9" t="s">
         <v>244</v>
       </c>
@@ -3636,7 +3639,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="44"/>
+      <c r="A180" s="47"/>
       <c r="B180" s="9" t="s">
         <v>233</v>
       </c>
@@ -3645,7 +3648,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="44"/>
+      <c r="A181" s="47"/>
       <c r="B181" s="9" t="s">
         <v>234</v>
       </c>
@@ -3654,7 +3657,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="44"/>
+      <c r="A182" s="47"/>
       <c r="B182" s="9" t="s">
         <v>235</v>
       </c>
@@ -3663,7 +3666,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="44" t="str">
+      <c r="A183" s="47" t="str">
         <f>'S 7'!A6</f>
         <v>I want trains moving along the track to do so smoothly</v>
       </c>
@@ -3675,7 +3678,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="44"/>
+      <c r="A184" s="47"/>
       <c r="B184" s="9" t="s">
         <v>247</v>
       </c>
@@ -3684,7 +3687,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="44"/>
+      <c r="A185" s="47"/>
       <c r="B185" s="9" t="s">
         <v>248</v>
       </c>
@@ -3693,7 +3696,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="44" t="str">
+      <c r="A186" s="47" t="str">
         <f>'S 7'!A7</f>
         <v>I want locomotives to retain their position, velocity, track they're on and other properties when the game is saved and reloaded.</v>
       </c>
@@ -3705,7 +3708,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="44"/>
+      <c r="A187" s="47"/>
       <c r="B187" s="9" t="s">
         <v>236</v>
       </c>
@@ -3714,7 +3717,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="44"/>
+      <c r="A188" s="47"/>
       <c r="B188" s="9" t="s">
         <v>239</v>
       </c>
@@ -3723,7 +3726,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="44"/>
+      <c r="A189" s="47"/>
       <c r="B189" s="9" t="s">
         <v>237</v>
       </c>
@@ -3736,11 +3739,11 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="47" t="s">
+      <c r="A190" s="52" t="s">
         <v>249</v>
       </c>
-      <c r="B190" s="48"/>
-      <c r="C190" s="49"/>
+      <c r="B190" s="53"/>
+      <c r="C190" s="61"/>
       <c r="D190">
         <f>SUMPRODUCT(LEN(C191:C210)-LEN(SUBSTITUTE(C191:C210,"S","")))</f>
         <v>0</v>
@@ -3783,7 +3786,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="45" t="str">
+      <c r="A193" s="44" t="str">
         <f>'S 8'!A3</f>
         <v>I want to be able to control the curvature of the bauble I am placing.  The shape controller should transition only to that curvature.</v>
       </c>
@@ -3795,7 +3798,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="45"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="28" t="s">
         <v>256</v>
       </c>
@@ -3804,7 +3807,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="45"/>
+      <c r="A195" s="44"/>
       <c r="B195" s="28" t="s">
         <v>258</v>
       </c>
@@ -3813,7 +3816,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="45"/>
+      <c r="A196" s="44"/>
       <c r="B196" s="28" t="s">
         <v>267</v>
       </c>
@@ -3822,7 +3825,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="45"/>
+      <c r="A197" s="44"/>
       <c r="B197" s="28" t="s">
         <v>268</v>
       </c>
@@ -3831,7 +3834,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="45"/>
+      <c r="A198" s="44"/>
       <c r="B198" s="28" t="s">
         <v>269</v>
       </c>
@@ -3840,7 +3843,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="45"/>
+      <c r="A199" s="44"/>
       <c r="B199" s="28" t="s">
         <v>270</v>
       </c>
@@ -3850,7 +3853,7 @@
       <c r="D199" s="34"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="45"/>
+      <c r="A200" s="44"/>
       <c r="B200" s="28" t="s">
         <v>271</v>
       </c>
@@ -3859,7 +3862,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="45"/>
+      <c r="A201" s="44"/>
       <c r="B201" s="28" t="s">
         <v>272</v>
       </c>
@@ -3868,7 +3871,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="45"/>
+      <c r="A202" s="44"/>
       <c r="B202" s="28" t="s">
         <v>273</v>
       </c>
@@ -3877,7 +3880,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="45" t="str">
+      <c r="A203" s="44" t="str">
         <f>'S 8'!A4</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -3889,7 +3892,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="45"/>
+      <c r="A204" s="44"/>
       <c r="B204" s="28" t="s">
         <v>260</v>
       </c>
@@ -3898,7 +3901,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="45"/>
+      <c r="A205" s="44"/>
       <c r="B205" s="28" t="s">
         <v>261</v>
       </c>
@@ -3907,7 +3910,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="45" t="str">
+      <c r="A206" s="44" t="str">
         <f>'S 8'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -3919,7 +3922,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="45"/>
+      <c r="A207" s="44"/>
       <c r="B207" s="28" t="s">
         <v>263</v>
       </c>
@@ -3928,7 +3931,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="45"/>
+      <c r="A208" s="44"/>
       <c r="B208" s="28" t="s">
         <v>264</v>
       </c>
@@ -3937,7 +3940,7 @@
       </c>
     </row>
     <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="45" t="str">
+      <c r="A209" s="44" t="str">
         <f>'S 8'!A6</f>
         <v>If a track vehicle runs off the end of the track, it should derail properly.</v>
       </c>
@@ -3949,7 +3952,7 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="46"/>
+      <c r="A210" s="45"/>
       <c r="B210" s="32" t="s">
         <v>265</v>
       </c>
@@ -3958,10 +3961,10 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="47" t="s">
+      <c r="A211" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="B211" s="48"/>
+      <c r="B211" s="53"/>
       <c r="C211" s="40"/>
       <c r="D211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"S","")))</f>
@@ -3969,7 +3972,7 @@
       </c>
       <c r="E211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"R","")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F211">
         <f>SUMPRODUCT(LEN(C212:C239)-LEN(SUBSTITUTE(C212:C239,"C","")))</f>
@@ -3981,7 +3984,7 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="61" t="str">
+      <c r="A212" s="49" t="str">
         <f>'S 9'!A1</f>
         <v>I want to be able to detach a specific track section from a bauble by clicking on the bauble and dragging towards the other end of the section.</v>
       </c>
@@ -3993,7 +3996,7 @@
       </c>
     </row>
     <row r="213" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="61"/>
+      <c r="A213" s="49"/>
       <c r="B213" s="28" t="s">
         <v>288</v>
       </c>
@@ -4002,7 +4005,7 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="59" t="str">
+      <c r="A214" s="46" t="str">
         <f>'S 9'!A2</f>
         <v>Track sections which do not shape properly should highlight as red and prevent placement of the bauble.</v>
       </c>
@@ -4014,7 +4017,7 @@
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215" s="59"/>
+      <c r="A215" s="46"/>
       <c r="B215" s="28" t="s">
         <v>291</v>
       </c>
@@ -4023,7 +4026,7 @@
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="59"/>
+      <c r="A216" s="46"/>
       <c r="B216" s="28" t="s">
         <v>290</v>
       </c>
@@ -4032,23 +4035,25 @@
       </c>
     </row>
     <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A217" s="59"/>
+      <c r="A217" s="46"/>
       <c r="B217" s="28" t="s">
         <v>293</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218" s="59"/>
+      <c r="A218" s="46"/>
       <c r="B218" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="C218" s="31"/>
+      <c r="C218" s="31" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="59" t="str">
+      <c r="A219" s="46" t="str">
         <f>'S 9'!A3</f>
         <v>I want to be able to create a new bauble partway along curved track.</v>
       </c>
@@ -4058,28 +4063,28 @@
       <c r="C219" s="31"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="59"/>
+      <c r="A220" s="46"/>
       <c r="B220" s="28" t="s">
         <v>295</v>
       </c>
       <c r="C220" s="31"/>
     </row>
     <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="59"/>
+      <c r="A221" s="46"/>
       <c r="B221" s="28" t="s">
         <v>296</v>
       </c>
       <c r="C221" s="31"/>
     </row>
     <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A222" s="59"/>
+      <c r="A222" s="46"/>
       <c r="B222" s="28" t="s">
         <v>297</v>
       </c>
       <c r="C222" s="31"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="45" t="str">
+      <c r="A223" s="44" t="str">
         <f>'S 9'!A4</f>
         <v>I want bauble curvature to be the correct direction regardless which side the track connects to</v>
       </c>
@@ -4089,14 +4094,14 @@
       <c r="C223" s="31"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="45"/>
+      <c r="A224" s="44"/>
       <c r="B224" s="28" t="s">
         <v>300</v>
       </c>
       <c r="C224" s="31"/>
     </row>
     <row r="225" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="59" t="str">
+      <c r="A225" s="46" t="str">
         <f>'S 9'!A5</f>
         <v>I want to be able to hold a button (shift) and for the track to retain the same curvature all the way along, be it straight or fixed radius.</v>
       </c>
@@ -4106,35 +4111,35 @@
       <c r="C225" s="31"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="59"/>
+      <c r="A226" s="46"/>
       <c r="B226" s="28" t="s">
         <v>302</v>
       </c>
       <c r="C226" s="31"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="59"/>
+      <c r="A227" s="46"/>
       <c r="B227" s="28" t="s">
         <v>304</v>
       </c>
       <c r="C227" s="31"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="59"/>
+      <c r="A228" s="46"/>
       <c r="B228" s="28" t="s">
         <v>305</v>
       </c>
       <c r="C228" s="31"/>
     </row>
     <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="59"/>
+      <c r="A229" s="46"/>
       <c r="B229" s="28" t="s">
         <v>306</v>
       </c>
       <c r="C229" s="31"/>
     </row>
     <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="45" t="str">
+      <c r="A230" s="44" t="str">
         <f>'S 9'!A6</f>
         <v>I want the track to be able to transition [Fixed/Radius -&gt; Rotate/Radius]</v>
       </c>
@@ -4144,35 +4149,35 @@
       <c r="C230" s="31"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="45"/>
+      <c r="A231" s="44"/>
       <c r="B231" s="28" t="s">
         <v>308</v>
       </c>
       <c r="C231" s="31"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="45"/>
+      <c r="A232" s="44"/>
       <c r="B232" s="28" t="s">
         <v>309</v>
       </c>
       <c r="C232" s="31"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="45"/>
+      <c r="A233" s="44"/>
       <c r="B233" s="28" t="s">
         <v>311</v>
       </c>
       <c r="C233" s="31"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="45"/>
+      <c r="A234" s="44"/>
       <c r="B234" s="28" t="s">
         <v>310</v>
       </c>
       <c r="C234" s="31"/>
     </row>
     <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="45" t="str">
+      <c r="A235" s="44" t="str">
         <f>'S 9'!A7</f>
         <v>I want to be able to control (from the editor for now) which track a vehicle moves onto from a junction.</v>
       </c>
@@ -4182,28 +4187,28 @@
       <c r="C235" s="31"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="45"/>
+      <c r="A236" s="44"/>
       <c r="B236" s="28" t="s">
         <v>313</v>
       </c>
       <c r="C236" s="31"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="45"/>
+      <c r="A237" s="44"/>
       <c r="B237" s="28" t="s">
         <v>314</v>
       </c>
       <c r="C237" s="31"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="45"/>
+      <c r="A238" s="44"/>
       <c r="B238" s="28" t="s">
         <v>315</v>
       </c>
       <c r="C238" s="31"/>
     </row>
     <row r="239" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="46"/>
+      <c r="A239" s="45"/>
       <c r="B239" s="32" t="s">
         <v>316</v>
       </c>
@@ -4221,11 +4226,55 @@
     <row r="240" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A219:A222"/>
-    <mergeCell ref="A223:A224"/>
-    <mergeCell ref="A225:A229"/>
-    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A206:A208"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A193:A202"/>
+    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A214:A218"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A211:B211"/>
+    <mergeCell ref="A160:A164"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A120"/>
     <mergeCell ref="A132:A134"/>
     <mergeCell ref="A121:A124"/>
     <mergeCell ref="A125:A127"/>
@@ -4242,55 +4291,11 @@
     <mergeCell ref="A169:A173"/>
     <mergeCell ref="A174:A177"/>
     <mergeCell ref="A178:A182"/>
-    <mergeCell ref="A214:A218"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A211:B211"/>
-    <mergeCell ref="A160:A164"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A206:A208"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="A193:A202"/>
-    <mergeCell ref="A203:A205"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A230:A234"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B210 B230:B1048576 B212:B228">
     <cfRule type="expression" dxfId="11" priority="1">

</xml_diff>